<commit_message>
Add Nombre Cientifico plaga
</commit_message>
<xml_diff>
--- a/Matriz Cacao, Cafe y Arroz/MATRIZ FINAL DEL CAFÉ.xlsx
+++ b/Matriz Cacao, Cafe y Arroz/MATRIZ FINAL DEL CAFÉ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cafe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\proyecto\Matriz Cacao, Cafe y Arroz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38CD72F8-248A-4F19-B0E4-BD41511F3404}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="7575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="7575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="157">
   <si>
     <r>
       <rPr>
@@ -741,11 +740,14 @@
   <si>
     <t>Pratylenchus (lesionadores) y Meloidogyne (agalladores)</t>
   </si>
+  <si>
+    <t>Hemileia vastatrix Berkeley y Broome</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1232,6 +1234,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,9 +1261,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1280,6 +1282,84 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1289,6 +1369,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1323,102 +1421,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1461,7 +1463,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1522,7 +1524,7 @@
         <xdr:cNvPr id="3" name="Imagen 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1585,7 @@
         <xdr:cNvPr id="4" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1644,7 +1646,7 @@
         <xdr:cNvPr id="9" name="8 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1688,7 +1690,7 @@
         <xdr:cNvPr id="11" name="10 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1738,7 +1740,7 @@
         <xdr:cNvPr id="13" name="Imagen 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2068,11 +2070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H8"/>
+      <selection activeCell="J3" sqref="J3:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,331 +2325,331 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BC174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100:N101"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="6:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="95" t="s">
+      <c r="G2" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="98" t="s">
+      <c r="H2" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="104" t="str">
+      <c r="J2" s="89" t="str">
         <f>[1]Hoja1!$B$6</f>
         <v xml:space="preserve">EL café tiene su origen en África – Etiopia luego paso a Europa y después de algunos siglos llego al continente americano.
 Al Ecuador el café llego en los años 1800 y desde entonces ha tenido importantes aportaciones como fuente de empleo y de divisas al país
 El café se siembra y se cosecha en el litoral ecuatoriano y parte del oriente, la provincia de Manabí fue uno de preponderante del cultivo del Café, a partir del año 1860 ya se cultivaba el producto en este sector
 </v>
       </c>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
-      <c r="X2" s="106"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="91"/>
     </row>
     <row r="3" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F3" s="93"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="109"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="94"/>
     </row>
     <row r="4" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F4" s="93"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108"/>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="108"/>
-      <c r="X4" s="109"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="93"/>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="94"/>
     </row>
     <row r="5" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F5" s="93"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
-      <c r="M5" s="108"/>
-      <c r="N5" s="108"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="109"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="93"/>
+      <c r="X5" s="94"/>
     </row>
     <row r="6" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F6" s="93"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="108"/>
-      <c r="S6" s="108"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="109"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
+      <c r="T6" s="93"/>
+      <c r="U6" s="93"/>
+      <c r="V6" s="93"/>
+      <c r="W6" s="93"/>
+      <c r="X6" s="94"/>
     </row>
     <row r="7" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F7" s="93"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="107"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="108"/>
-      <c r="S7" s="108"/>
-      <c r="T7" s="108"/>
-      <c r="U7" s="108"/>
-      <c r="V7" s="108"/>
-      <c r="W7" s="108"/>
-      <c r="X7" s="109"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="93"/>
+      <c r="W7" s="93"/>
+      <c r="X7" s="94"/>
     </row>
     <row r="8" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F8" s="93"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="108"/>
-      <c r="Q8" s="108"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="108"/>
-      <c r="T8" s="108"/>
-      <c r="U8" s="108"/>
-      <c r="V8" s="108"/>
-      <c r="W8" s="108"/>
-      <c r="X8" s="109"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="93"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="93"/>
+      <c r="W8" s="93"/>
+      <c r="X8" s="94"/>
     </row>
     <row r="9" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F9" s="93"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="107"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="108"/>
-      <c r="N9" s="108"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="108"/>
-      <c r="R9" s="108"/>
-      <c r="S9" s="108"/>
-      <c r="T9" s="108"/>
-      <c r="U9" s="108"/>
-      <c r="V9" s="108"/>
-      <c r="W9" s="108"/>
-      <c r="X9" s="109"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="93"/>
+      <c r="V9" s="93"/>
+      <c r="W9" s="93"/>
+      <c r="X9" s="94"/>
     </row>
     <row r="10" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="93"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="108"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="108"/>
-      <c r="N10" s="108"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="108"/>
-      <c r="R10" s="108"/>
-      <c r="S10" s="108"/>
-      <c r="T10" s="108"/>
-      <c r="U10" s="108"/>
-      <c r="V10" s="108"/>
-      <c r="W10" s="108"/>
-      <c r="X10" s="109"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="93"/>
+      <c r="R10" s="93"/>
+      <c r="S10" s="93"/>
+      <c r="T10" s="93"/>
+      <c r="U10" s="93"/>
+      <c r="V10" s="93"/>
+      <c r="W10" s="93"/>
+      <c r="X10" s="94"/>
     </row>
     <row r="11" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="93"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="108"/>
-      <c r="M11" s="108"/>
-      <c r="N11" s="108"/>
-      <c r="O11" s="108"/>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="108"/>
-      <c r="R11" s="108"/>
-      <c r="S11" s="108"/>
-      <c r="T11" s="108"/>
-      <c r="U11" s="108"/>
-      <c r="V11" s="108"/>
-      <c r="W11" s="108"/>
-      <c r="X11" s="109"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="93"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="93"/>
+      <c r="T11" s="93"/>
+      <c r="U11" s="93"/>
+      <c r="V11" s="93"/>
+      <c r="W11" s="93"/>
+      <c r="X11" s="94"/>
     </row>
     <row r="12" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="93"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="108"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
-      <c r="O12" s="108"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="108"/>
-      <c r="S12" s="108"/>
-      <c r="T12" s="108"/>
-      <c r="U12" s="108"/>
-      <c r="V12" s="108"/>
-      <c r="W12" s="108"/>
-      <c r="X12" s="109"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="93"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="93"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="93"/>
+      <c r="V12" s="93"/>
+      <c r="W12" s="93"/>
+      <c r="X12" s="94"/>
     </row>
     <row r="13" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="94"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="111"/>
-      <c r="S13" s="111"/>
-      <c r="T13" s="111"/>
-      <c r="U13" s="111"/>
-      <c r="V13" s="111"/>
-      <c r="W13" s="111"/>
-      <c r="X13" s="112"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
+      <c r="O13" s="96"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="96"/>
+      <c r="S13" s="96"/>
+      <c r="T13" s="96"/>
+      <c r="U13" s="96"/>
+      <c r="V13" s="96"/>
+      <c r="W13" s="96"/>
+      <c r="X13" s="97"/>
     </row>
     <row r="16" spans="6:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="75" t="s">
+      <c r="F16" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="77"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="109"/>
       <c r="O16" s="6"/>
     </row>
     <row r="17" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F17" s="78"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="80"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="111"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="112"/>
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="81" t="s">
+      <c r="F18" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="83"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="115"/>
       <c r="O18" s="6"/>
     </row>
     <row r="19" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F19" s="84"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="86"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="118"/>
       <c r="O19" s="6"/>
     </row>
     <row r="20" spans="2:55" x14ac:dyDescent="0.25">
@@ -2661,7 +2663,7 @@
         <v>19</v>
       </c>
       <c r="K20" s="52"/>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="98" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="50" t="s">
@@ -2677,7 +2679,7 @@
       <c r="I21" s="55"/>
       <c r="J21" s="65"/>
       <c r="K21" s="67"/>
-      <c r="L21" s="73"/>
+      <c r="L21" s="99"/>
       <c r="M21" s="65"/>
       <c r="N21" s="67"/>
       <c r="O21" s="6"/>
@@ -2699,14 +2701,14 @@
       <c r="I22" s="52"/>
       <c r="J22" s="65"/>
       <c r="K22" s="67"/>
-      <c r="L22" s="73"/>
+      <c r="L22" s="99"/>
       <c r="M22" s="65"/>
       <c r="N22" s="67"/>
       <c r="O22" s="6"/>
-      <c r="P22" s="56" t="s">
+      <c r="P22" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="Q22" s="57"/>
+      <c r="Q22" s="58"/>
       <c r="R22" s="50" t="s">
         <v>68</v>
       </c>
@@ -2777,12 +2779,12 @@
       <c r="I23" s="55"/>
       <c r="J23" s="53"/>
       <c r="K23" s="55"/>
-      <c r="L23" s="74"/>
+      <c r="L23" s="100"/>
       <c r="M23" s="53"/>
       <c r="N23" s="55"/>
       <c r="O23" s="6"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="60"/>
       <c r="R23" s="53"/>
       <c r="S23" s="55"/>
       <c r="T23" s="53"/>
@@ -3353,8 +3355,10 @@
         <v>115</v>
       </c>
       <c r="G33" s="11"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
+      <c r="H33" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="I33" s="56"/>
       <c r="J33" s="9" t="s">
         <v>117</v>
       </c>
@@ -3421,8 +3425,8 @@
       <c r="E34" s="43"/>
       <c r="F34" s="12"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
       <c r="J34" s="12"/>
       <c r="K34" s="14"/>
       <c r="L34" s="48"/>
@@ -3477,8 +3481,8 @@
       <c r="E35" s="43"/>
       <c r="F35" s="12"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="12"/>
       <c r="K35" s="14"/>
       <c r="L35" s="48"/>
@@ -3533,8 +3537,8 @@
       <c r="E36" s="43"/>
       <c r="F36" s="12"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
       <c r="J36" s="12"/>
       <c r="K36" s="14"/>
       <c r="L36" s="48"/>
@@ -3589,8 +3593,8 @@
       <c r="E37" s="43"/>
       <c r="F37" s="12"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
       <c r="J37" s="12"/>
       <c r="K37" s="14"/>
       <c r="L37" s="48"/>
@@ -3645,8 +3649,8 @@
       <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
       <c r="J38" s="12"/>
       <c r="K38" s="14"/>
       <c r="L38" s="48"/>
@@ -3701,8 +3705,8 @@
       <c r="E39" s="43"/>
       <c r="F39" s="12"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
       <c r="J39" s="12"/>
       <c r="K39" s="14"/>
       <c r="L39" s="48"/>
@@ -3757,8 +3761,8 @@
       <c r="E40" s="43"/>
       <c r="F40" s="12"/>
       <c r="G40" s="14"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
       <c r="J40" s="12"/>
       <c r="K40" s="14"/>
       <c r="L40" s="48"/>
@@ -3813,8 +3817,8 @@
       <c r="E41" s="46"/>
       <c r="F41" s="15"/>
       <c r="G41" s="17"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
       <c r="J41" s="15"/>
       <c r="K41" s="17"/>
       <c r="L41" s="49"/>
@@ -4218,9 +4222,9 @@
       <c r="AX47" s="10"/>
       <c r="AY47" s="10"/>
       <c r="AZ47" s="11"/>
-      <c r="BA47" s="64"/>
-      <c r="BB47" s="64"/>
-      <c r="BC47" s="64"/>
+      <c r="BA47" s="56"/>
+      <c r="BB47" s="56"/>
+      <c r="BC47" s="56"/>
     </row>
     <row r="48" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B48" s="41"/>
@@ -4274,9 +4278,9 @@
       <c r="AX48" s="13"/>
       <c r="AY48" s="13"/>
       <c r="AZ48" s="14"/>
-      <c r="BA48" s="64"/>
-      <c r="BB48" s="64"/>
-      <c r="BC48" s="64"/>
+      <c r="BA48" s="56"/>
+      <c r="BB48" s="56"/>
+      <c r="BC48" s="56"/>
     </row>
     <row r="49" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B49" s="41"/>
@@ -4330,9 +4334,9 @@
       <c r="AX49" s="13"/>
       <c r="AY49" s="13"/>
       <c r="AZ49" s="14"/>
-      <c r="BA49" s="64"/>
-      <c r="BB49" s="64"/>
-      <c r="BC49" s="64"/>
+      <c r="BA49" s="56"/>
+      <c r="BB49" s="56"/>
+      <c r="BC49" s="56"/>
     </row>
     <row r="50" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B50" s="41"/>
@@ -4386,9 +4390,9 @@
       <c r="AX50" s="13"/>
       <c r="AY50" s="13"/>
       <c r="AZ50" s="14"/>
-      <c r="BA50" s="64"/>
-      <c r="BB50" s="64"/>
-      <c r="BC50" s="64"/>
+      <c r="BA50" s="56"/>
+      <c r="BB50" s="56"/>
+      <c r="BC50" s="56"/>
     </row>
     <row r="51" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B51" s="41"/>
@@ -4442,9 +4446,9 @@
       <c r="AX51" s="13"/>
       <c r="AY51" s="13"/>
       <c r="AZ51" s="14"/>
-      <c r="BA51" s="64"/>
-      <c r="BB51" s="64"/>
-      <c r="BC51" s="64"/>
+      <c r="BA51" s="56"/>
+      <c r="BB51" s="56"/>
+      <c r="BC51" s="56"/>
     </row>
     <row r="52" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B52" s="41"/>
@@ -4498,9 +4502,9 @@
       <c r="AX52" s="13"/>
       <c r="AY52" s="13"/>
       <c r="AZ52" s="14"/>
-      <c r="BA52" s="64"/>
-      <c r="BB52" s="64"/>
-      <c r="BC52" s="64"/>
+      <c r="BA52" s="56"/>
+      <c r="BB52" s="56"/>
+      <c r="BC52" s="56"/>
     </row>
     <row r="53" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B53" s="44"/>
@@ -4554,9 +4558,9 @@
       <c r="AX53" s="13"/>
       <c r="AY53" s="13"/>
       <c r="AZ53" s="14"/>
-      <c r="BA53" s="64"/>
-      <c r="BB53" s="64"/>
-      <c r="BC53" s="64"/>
+      <c r="BA53" s="56"/>
+      <c r="BB53" s="56"/>
+      <c r="BC53" s="56"/>
     </row>
     <row r="54" spans="2:55" x14ac:dyDescent="0.25">
       <c r="O54" s="4"/>
@@ -4597,9 +4601,9 @@
       <c r="AX54" s="13"/>
       <c r="AY54" s="13"/>
       <c r="AZ54" s="14"/>
-      <c r="BA54" s="64"/>
-      <c r="BB54" s="64"/>
-      <c r="BC54" s="64"/>
+      <c r="BA54" s="56"/>
+      <c r="BB54" s="56"/>
+      <c r="BC54" s="56"/>
     </row>
     <row r="55" spans="2:55" x14ac:dyDescent="0.25">
       <c r="F55" s="4"/>
@@ -4649,22 +4653,22 @@
       <c r="AX55" s="13"/>
       <c r="AY55" s="13"/>
       <c r="AZ55" s="14"/>
-      <c r="BA55" s="64"/>
-      <c r="BB55" s="64"/>
-      <c r="BC55" s="64"/>
+      <c r="BA55" s="56"/>
+      <c r="BB55" s="56"/>
+      <c r="BC55" s="56"/>
     </row>
     <row r="56" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F56" s="113" t="s">
+      <c r="F56" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="G56" s="114"/>
-      <c r="H56" s="114"/>
-      <c r="I56" s="114"/>
-      <c r="J56" s="114"/>
-      <c r="K56" s="114"/>
-      <c r="L56" s="114"/>
-      <c r="M56" s="114"/>
-      <c r="N56" s="115"/>
+      <c r="G56" s="102"/>
+      <c r="H56" s="102"/>
+      <c r="I56" s="102"/>
+      <c r="J56" s="102"/>
+      <c r="K56" s="102"/>
+      <c r="L56" s="102"/>
+      <c r="M56" s="102"/>
+      <c r="N56" s="103"/>
       <c r="O56" s="4"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="14"/>
@@ -4703,20 +4707,20 @@
       <c r="AX56" s="13"/>
       <c r="AY56" s="13"/>
       <c r="AZ56" s="14"/>
-      <c r="BA56" s="64"/>
-      <c r="BB56" s="64"/>
-      <c r="BC56" s="64"/>
+      <c r="BA56" s="56"/>
+      <c r="BB56" s="56"/>
+      <c r="BC56" s="56"/>
     </row>
     <row r="57" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F57" s="116"/>
-      <c r="G57" s="117"/>
-      <c r="H57" s="117"/>
-      <c r="I57" s="117"/>
-      <c r="J57" s="117"/>
-      <c r="K57" s="117"/>
-      <c r="L57" s="117"/>
-      <c r="M57" s="117"/>
-      <c r="N57" s="118"/>
+      <c r="F57" s="104"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="105"/>
+      <c r="I57" s="105"/>
+      <c r="J57" s="105"/>
+      <c r="K57" s="105"/>
+      <c r="L57" s="105"/>
+      <c r="M57" s="105"/>
+      <c r="N57" s="106"/>
       <c r="O57" s="4"/>
       <c r="P57" s="15"/>
       <c r="Q57" s="17"/>
@@ -4755,9 +4759,9 @@
       <c r="AX57" s="16"/>
       <c r="AY57" s="16"/>
       <c r="AZ57" s="17"/>
-      <c r="BA57" s="64"/>
-      <c r="BB57" s="64"/>
-      <c r="BC57" s="64"/>
+      <c r="BA57" s="56"/>
+      <c r="BB57" s="56"/>
+      <c r="BC57" s="56"/>
     </row>
     <row r="58" spans="2:55" x14ac:dyDescent="0.25">
       <c r="F58" s="50" t="s">
@@ -4770,7 +4774,7 @@
         <v>19</v>
       </c>
       <c r="K58" s="52"/>
-      <c r="L58" s="72" t="s">
+      <c r="L58" s="98" t="s">
         <v>20</v>
       </c>
       <c r="M58" s="50" t="s">
@@ -4826,7 +4830,7 @@
       <c r="I59" s="55"/>
       <c r="J59" s="65"/>
       <c r="K59" s="67"/>
-      <c r="L59" s="73"/>
+      <c r="L59" s="99"/>
       <c r="M59" s="65"/>
       <c r="N59" s="67"/>
       <c r="O59" s="4"/>
@@ -4888,14 +4892,14 @@
       <c r="I60" s="52"/>
       <c r="J60" s="65"/>
       <c r="K60" s="67"/>
-      <c r="L60" s="73"/>
+      <c r="L60" s="99"/>
       <c r="M60" s="65"/>
       <c r="N60" s="67"/>
       <c r="O60" s="6"/>
-      <c r="P60" s="60" t="s">
+      <c r="P60" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="Q60" s="61"/>
+      <c r="Q60" s="62"/>
       <c r="R60" s="65" t="s">
         <v>68</v>
       </c>
@@ -4966,12 +4970,12 @@
       <c r="I61" s="55"/>
       <c r="J61" s="53"/>
       <c r="K61" s="55"/>
-      <c r="L61" s="74"/>
+      <c r="L61" s="100"/>
       <c r="M61" s="53"/>
       <c r="N61" s="55"/>
       <c r="O61" s="6"/>
-      <c r="P61" s="62"/>
-      <c r="Q61" s="63"/>
+      <c r="P61" s="63"/>
+      <c r="Q61" s="64"/>
       <c r="R61" s="53"/>
       <c r="S61" s="55"/>
       <c r="T61" s="53"/>
@@ -5016,19 +5020,19 @@
       <c r="C62" s="39"/>
       <c r="D62" s="39"/>
       <c r="E62" s="40"/>
-      <c r="F62" s="64" t="s">
+      <c r="F62" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="G62" s="64"/>
+      <c r="G62" s="56"/>
       <c r="H62" s="9" t="s">
         <v>119</v>
       </c>
       <c r="I62" s="11"/>
-      <c r="J62" s="64" t="s">
+      <c r="J62" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="K62" s="64"/>
-      <c r="L62" s="64"/>
+      <c r="K62" s="56"/>
+      <c r="L62" s="56"/>
       <c r="M62" s="9" t="s">
         <v>121</v>
       </c>
@@ -5075,14 +5079,14 @@
         <v>82</v>
       </c>
       <c r="AN62" s="11"/>
-      <c r="AO62" s="64" t="s">
+      <c r="AO62" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="AP62" s="64"/>
-      <c r="AQ62" s="64"/>
-      <c r="AR62" s="64"/>
-      <c r="AS62" s="64"/>
-      <c r="AT62" s="64"/>
+      <c r="AP62" s="56"/>
+      <c r="AQ62" s="56"/>
+      <c r="AR62" s="56"/>
+      <c r="AS62" s="56"/>
+      <c r="AT62" s="56"/>
       <c r="AU62" s="9" t="s">
         <v>150</v>
       </c>
@@ -5102,13 +5106,13 @@
       <c r="C63" s="42"/>
       <c r="D63" s="42"/>
       <c r="E63" s="43"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
       <c r="H63" s="12"/>
       <c r="I63" s="14"/>
-      <c r="J63" s="64"/>
-      <c r="K63" s="64"/>
-      <c r="L63" s="64"/>
+      <c r="J63" s="56"/>
+      <c r="K63" s="56"/>
+      <c r="L63" s="56"/>
       <c r="M63" s="12"/>
       <c r="N63" s="14"/>
       <c r="O63" s="1"/>
@@ -5137,12 +5141,12 @@
       <c r="AL63" s="14"/>
       <c r="AM63" s="12"/>
       <c r="AN63" s="14"/>
-      <c r="AO63" s="64"/>
-      <c r="AP63" s="64"/>
-      <c r="AQ63" s="64"/>
-      <c r="AR63" s="64"/>
-      <c r="AS63" s="64"/>
-      <c r="AT63" s="64"/>
+      <c r="AO63" s="56"/>
+      <c r="AP63" s="56"/>
+      <c r="AQ63" s="56"/>
+      <c r="AR63" s="56"/>
+      <c r="AS63" s="56"/>
+      <c r="AT63" s="56"/>
       <c r="AU63" s="12"/>
       <c r="AV63" s="13"/>
       <c r="AW63" s="13"/>
@@ -5158,13 +5162,13 @@
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="43"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="64"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
       <c r="H64" s="12"/>
       <c r="I64" s="14"/>
-      <c r="J64" s="64"/>
-      <c r="K64" s="64"/>
-      <c r="L64" s="64"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="56"/>
+      <c r="L64" s="56"/>
       <c r="M64" s="12"/>
       <c r="N64" s="14"/>
       <c r="O64" s="1"/>
@@ -5193,12 +5197,12 @@
       <c r="AL64" s="14"/>
       <c r="AM64" s="12"/>
       <c r="AN64" s="14"/>
-      <c r="AO64" s="64"/>
-      <c r="AP64" s="64"/>
-      <c r="AQ64" s="64"/>
-      <c r="AR64" s="64"/>
-      <c r="AS64" s="64"/>
-      <c r="AT64" s="64"/>
+      <c r="AO64" s="56"/>
+      <c r="AP64" s="56"/>
+      <c r="AQ64" s="56"/>
+      <c r="AR64" s="56"/>
+      <c r="AS64" s="56"/>
+      <c r="AT64" s="56"/>
       <c r="AU64" s="12"/>
       <c r="AV64" s="13"/>
       <c r="AW64" s="13"/>
@@ -5214,13 +5218,13 @@
       <c r="C65" s="42"/>
       <c r="D65" s="42"/>
       <c r="E65" s="43"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
       <c r="H65" s="12"/>
       <c r="I65" s="14"/>
-      <c r="J65" s="64"/>
-      <c r="K65" s="64"/>
-      <c r="L65" s="64"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="56"/>
+      <c r="L65" s="56"/>
       <c r="M65" s="12"/>
       <c r="N65" s="14"/>
       <c r="O65" s="1"/>
@@ -5249,12 +5253,12 @@
       <c r="AL65" s="14"/>
       <c r="AM65" s="12"/>
       <c r="AN65" s="14"/>
-      <c r="AO65" s="64"/>
-      <c r="AP65" s="64"/>
-      <c r="AQ65" s="64"/>
-      <c r="AR65" s="64"/>
-      <c r="AS65" s="64"/>
-      <c r="AT65" s="64"/>
+      <c r="AO65" s="56"/>
+      <c r="AP65" s="56"/>
+      <c r="AQ65" s="56"/>
+      <c r="AR65" s="56"/>
+      <c r="AS65" s="56"/>
+      <c r="AT65" s="56"/>
       <c r="AU65" s="12"/>
       <c r="AV65" s="13"/>
       <c r="AW65" s="13"/>
@@ -5270,13 +5274,13 @@
       <c r="C66" s="42"/>
       <c r="D66" s="42"/>
       <c r="E66" s="43"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="64"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
       <c r="H66" s="12"/>
       <c r="I66" s="14"/>
-      <c r="J66" s="64"/>
-      <c r="K66" s="64"/>
-      <c r="L66" s="64"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="56"/>
+      <c r="L66" s="56"/>
       <c r="M66" s="12"/>
       <c r="N66" s="14"/>
       <c r="O66" s="1"/>
@@ -5305,12 +5309,12 @@
       <c r="AL66" s="14"/>
       <c r="AM66" s="12"/>
       <c r="AN66" s="14"/>
-      <c r="AO66" s="64"/>
-      <c r="AP66" s="64"/>
-      <c r="AQ66" s="64"/>
-      <c r="AR66" s="64"/>
-      <c r="AS66" s="64"/>
-      <c r="AT66" s="64"/>
+      <c r="AO66" s="56"/>
+      <c r="AP66" s="56"/>
+      <c r="AQ66" s="56"/>
+      <c r="AR66" s="56"/>
+      <c r="AS66" s="56"/>
+      <c r="AT66" s="56"/>
       <c r="AU66" s="12"/>
       <c r="AV66" s="13"/>
       <c r="AW66" s="13"/>
@@ -5326,13 +5330,13 @@
       <c r="C67" s="45"/>
       <c r="D67" s="45"/>
       <c r="E67" s="46"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="64"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
       <c r="H67" s="15"/>
       <c r="I67" s="17"/>
-      <c r="J67" s="64"/>
-      <c r="K67" s="64"/>
-      <c r="L67" s="64"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="56"/>
+      <c r="L67" s="56"/>
       <c r="M67" s="15"/>
       <c r="N67" s="17"/>
       <c r="O67" s="1"/>
@@ -5361,12 +5365,12 @@
       <c r="AL67" s="17"/>
       <c r="AM67" s="15"/>
       <c r="AN67" s="17"/>
-      <c r="AO67" s="64"/>
-      <c r="AP67" s="64"/>
-      <c r="AQ67" s="64"/>
-      <c r="AR67" s="64"/>
-      <c r="AS67" s="64"/>
-      <c r="AT67" s="64"/>
+      <c r="AO67" s="56"/>
+      <c r="AP67" s="56"/>
+      <c r="AQ67" s="56"/>
+      <c r="AR67" s="56"/>
+      <c r="AS67" s="56"/>
+      <c r="AT67" s="56"/>
       <c r="AU67" s="15"/>
       <c r="AV67" s="16"/>
       <c r="AW67" s="16"/>
@@ -5397,8 +5401,8 @@
       <c r="L68" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="M68" s="64"/>
-      <c r="N68" s="64"/>
+      <c r="M68" s="56"/>
+      <c r="N68" s="56"/>
       <c r="O68" s="1"/>
       <c r="P68" s="9" t="s">
         <v>22</v>
@@ -5437,26 +5441,26 @@
       <c r="AJ68" s="10"/>
       <c r="AK68" s="10"/>
       <c r="AL68" s="11"/>
-      <c r="AM68" s="64" t="s">
+      <c r="AM68" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="AN68" s="64"/>
-      <c r="AO68" s="64" t="s">
+      <c r="AN68" s="56"/>
+      <c r="AO68" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="AP68" s="64"/>
-      <c r="AQ68" s="64"/>
-      <c r="AR68" s="64"/>
-      <c r="AS68" s="64"/>
-      <c r="AT68" s="64"/>
-      <c r="AU68" s="64" t="s">
+      <c r="AP68" s="56"/>
+      <c r="AQ68" s="56"/>
+      <c r="AR68" s="56"/>
+      <c r="AS68" s="56"/>
+      <c r="AT68" s="56"/>
+      <c r="AU68" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="AV68" s="64"/>
-      <c r="AW68" s="64"/>
-      <c r="AX68" s="64"/>
-      <c r="AY68" s="64"/>
-      <c r="AZ68" s="64"/>
+      <c r="AV68" s="56"/>
+      <c r="AW68" s="56"/>
+      <c r="AX68" s="56"/>
+      <c r="AY68" s="56"/>
+      <c r="AZ68" s="56"/>
       <c r="BA68" s="9" t="s">
         <v>77</v>
       </c>
@@ -5475,8 +5479,8 @@
       <c r="J69" s="12"/>
       <c r="K69" s="14"/>
       <c r="L69" s="48"/>
-      <c r="M69" s="64"/>
-      <c r="N69" s="64"/>
+      <c r="M69" s="56"/>
+      <c r="N69" s="56"/>
       <c r="O69" s="1"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="14"/>
@@ -5501,20 +5505,20 @@
       <c r="AJ69" s="13"/>
       <c r="AK69" s="13"/>
       <c r="AL69" s="14"/>
-      <c r="AM69" s="64"/>
-      <c r="AN69" s="64"/>
-      <c r="AO69" s="64"/>
-      <c r="AP69" s="64"/>
-      <c r="AQ69" s="64"/>
-      <c r="AR69" s="64"/>
-      <c r="AS69" s="64"/>
-      <c r="AT69" s="64"/>
-      <c r="AU69" s="64"/>
-      <c r="AV69" s="64"/>
-      <c r="AW69" s="64"/>
-      <c r="AX69" s="64"/>
-      <c r="AY69" s="64"/>
-      <c r="AZ69" s="64"/>
+      <c r="AM69" s="56"/>
+      <c r="AN69" s="56"/>
+      <c r="AO69" s="56"/>
+      <c r="AP69" s="56"/>
+      <c r="AQ69" s="56"/>
+      <c r="AR69" s="56"/>
+      <c r="AS69" s="56"/>
+      <c r="AT69" s="56"/>
+      <c r="AU69" s="56"/>
+      <c r="AV69" s="56"/>
+      <c r="AW69" s="56"/>
+      <c r="AX69" s="56"/>
+      <c r="AY69" s="56"/>
+      <c r="AZ69" s="56"/>
       <c r="BA69" s="12"/>
       <c r="BB69" s="13"/>
       <c r="BC69" s="14"/>
@@ -5531,8 +5535,8 @@
       <c r="J70" s="12"/>
       <c r="K70" s="14"/>
       <c r="L70" s="48"/>
-      <c r="M70" s="64"/>
-      <c r="N70" s="64"/>
+      <c r="M70" s="56"/>
+      <c r="N70" s="56"/>
       <c r="O70" s="1"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="14"/>
@@ -5557,20 +5561,20 @@
       <c r="AJ70" s="13"/>
       <c r="AK70" s="13"/>
       <c r="AL70" s="14"/>
-      <c r="AM70" s="64"/>
-      <c r="AN70" s="64"/>
-      <c r="AO70" s="64"/>
-      <c r="AP70" s="64"/>
-      <c r="AQ70" s="64"/>
-      <c r="AR70" s="64"/>
-      <c r="AS70" s="64"/>
-      <c r="AT70" s="64"/>
-      <c r="AU70" s="64"/>
-      <c r="AV70" s="64"/>
-      <c r="AW70" s="64"/>
-      <c r="AX70" s="64"/>
-      <c r="AY70" s="64"/>
-      <c r="AZ70" s="64"/>
+      <c r="AM70" s="56"/>
+      <c r="AN70" s="56"/>
+      <c r="AO70" s="56"/>
+      <c r="AP70" s="56"/>
+      <c r="AQ70" s="56"/>
+      <c r="AR70" s="56"/>
+      <c r="AS70" s="56"/>
+      <c r="AT70" s="56"/>
+      <c r="AU70" s="56"/>
+      <c r="AV70" s="56"/>
+      <c r="AW70" s="56"/>
+      <c r="AX70" s="56"/>
+      <c r="AY70" s="56"/>
+      <c r="AZ70" s="56"/>
       <c r="BA70" s="12"/>
       <c r="BB70" s="13"/>
       <c r="BC70" s="14"/>
@@ -5587,8 +5591,8 @@
       <c r="J71" s="12"/>
       <c r="K71" s="14"/>
       <c r="L71" s="48"/>
-      <c r="M71" s="64"/>
-      <c r="N71" s="64"/>
+      <c r="M71" s="56"/>
+      <c r="N71" s="56"/>
       <c r="O71" s="1"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="14"/>
@@ -5613,20 +5617,20 @@
       <c r="AJ71" s="13"/>
       <c r="AK71" s="13"/>
       <c r="AL71" s="14"/>
-      <c r="AM71" s="64"/>
-      <c r="AN71" s="64"/>
-      <c r="AO71" s="64"/>
-      <c r="AP71" s="64"/>
-      <c r="AQ71" s="64"/>
-      <c r="AR71" s="64"/>
-      <c r="AS71" s="64"/>
-      <c r="AT71" s="64"/>
-      <c r="AU71" s="64"/>
-      <c r="AV71" s="64"/>
-      <c r="AW71" s="64"/>
-      <c r="AX71" s="64"/>
-      <c r="AY71" s="64"/>
-      <c r="AZ71" s="64"/>
+      <c r="AM71" s="56"/>
+      <c r="AN71" s="56"/>
+      <c r="AO71" s="56"/>
+      <c r="AP71" s="56"/>
+      <c r="AQ71" s="56"/>
+      <c r="AR71" s="56"/>
+      <c r="AS71" s="56"/>
+      <c r="AT71" s="56"/>
+      <c r="AU71" s="56"/>
+      <c r="AV71" s="56"/>
+      <c r="AW71" s="56"/>
+      <c r="AX71" s="56"/>
+      <c r="AY71" s="56"/>
+      <c r="AZ71" s="56"/>
       <c r="BA71" s="12"/>
       <c r="BB71" s="13"/>
       <c r="BC71" s="14"/>
@@ -5643,8 +5647,8 @@
       <c r="J72" s="12"/>
       <c r="K72" s="14"/>
       <c r="L72" s="48"/>
-      <c r="M72" s="64"/>
-      <c r="N72" s="64"/>
+      <c r="M72" s="56"/>
+      <c r="N72" s="56"/>
       <c r="O72" s="1"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="14"/>
@@ -5669,20 +5673,20 @@
       <c r="AJ72" s="13"/>
       <c r="AK72" s="13"/>
       <c r="AL72" s="14"/>
-      <c r="AM72" s="64"/>
-      <c r="AN72" s="64"/>
-      <c r="AO72" s="64"/>
-      <c r="AP72" s="64"/>
-      <c r="AQ72" s="64"/>
-      <c r="AR72" s="64"/>
-      <c r="AS72" s="64"/>
-      <c r="AT72" s="64"/>
-      <c r="AU72" s="64"/>
-      <c r="AV72" s="64"/>
-      <c r="AW72" s="64"/>
-      <c r="AX72" s="64"/>
-      <c r="AY72" s="64"/>
-      <c r="AZ72" s="64"/>
+      <c r="AM72" s="56"/>
+      <c r="AN72" s="56"/>
+      <c r="AO72" s="56"/>
+      <c r="AP72" s="56"/>
+      <c r="AQ72" s="56"/>
+      <c r="AR72" s="56"/>
+      <c r="AS72" s="56"/>
+      <c r="AT72" s="56"/>
+      <c r="AU72" s="56"/>
+      <c r="AV72" s="56"/>
+      <c r="AW72" s="56"/>
+      <c r="AX72" s="56"/>
+      <c r="AY72" s="56"/>
+      <c r="AZ72" s="56"/>
       <c r="BA72" s="12"/>
       <c r="BB72" s="13"/>
       <c r="BC72" s="14"/>
@@ -5699,8 +5703,8 @@
       <c r="J73" s="12"/>
       <c r="K73" s="14"/>
       <c r="L73" s="48"/>
-      <c r="M73" s="64"/>
-      <c r="N73" s="64"/>
+      <c r="M73" s="56"/>
+      <c r="N73" s="56"/>
       <c r="O73" s="1"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="14"/>
@@ -5725,20 +5729,20 @@
       <c r="AJ73" s="13"/>
       <c r="AK73" s="13"/>
       <c r="AL73" s="14"/>
-      <c r="AM73" s="64"/>
-      <c r="AN73" s="64"/>
-      <c r="AO73" s="64"/>
-      <c r="AP73" s="64"/>
-      <c r="AQ73" s="64"/>
-      <c r="AR73" s="64"/>
-      <c r="AS73" s="64"/>
-      <c r="AT73" s="64"/>
-      <c r="AU73" s="64"/>
-      <c r="AV73" s="64"/>
-      <c r="AW73" s="64"/>
-      <c r="AX73" s="64"/>
-      <c r="AY73" s="64"/>
-      <c r="AZ73" s="64"/>
+      <c r="AM73" s="56"/>
+      <c r="AN73" s="56"/>
+      <c r="AO73" s="56"/>
+      <c r="AP73" s="56"/>
+      <c r="AQ73" s="56"/>
+      <c r="AR73" s="56"/>
+      <c r="AS73" s="56"/>
+      <c r="AT73" s="56"/>
+      <c r="AU73" s="56"/>
+      <c r="AV73" s="56"/>
+      <c r="AW73" s="56"/>
+      <c r="AX73" s="56"/>
+      <c r="AY73" s="56"/>
+      <c r="AZ73" s="56"/>
       <c r="BA73" s="12"/>
       <c r="BB73" s="13"/>
       <c r="BC73" s="14"/>
@@ -5755,8 +5759,8 @@
       <c r="J74" s="12"/>
       <c r="K74" s="14"/>
       <c r="L74" s="48"/>
-      <c r="M74" s="64"/>
-      <c r="N74" s="64"/>
+      <c r="M74" s="56"/>
+      <c r="N74" s="56"/>
       <c r="O74" s="1"/>
       <c r="P74" s="12"/>
       <c r="Q74" s="14"/>
@@ -5781,20 +5785,20 @@
       <c r="AJ74" s="13"/>
       <c r="AK74" s="13"/>
       <c r="AL74" s="14"/>
-      <c r="AM74" s="64"/>
-      <c r="AN74" s="64"/>
-      <c r="AO74" s="64"/>
-      <c r="AP74" s="64"/>
-      <c r="AQ74" s="64"/>
-      <c r="AR74" s="64"/>
-      <c r="AS74" s="64"/>
-      <c r="AT74" s="64"/>
-      <c r="AU74" s="64"/>
-      <c r="AV74" s="64"/>
-      <c r="AW74" s="64"/>
-      <c r="AX74" s="64"/>
-      <c r="AY74" s="64"/>
-      <c r="AZ74" s="64"/>
+      <c r="AM74" s="56"/>
+      <c r="AN74" s="56"/>
+      <c r="AO74" s="56"/>
+      <c r="AP74" s="56"/>
+      <c r="AQ74" s="56"/>
+      <c r="AR74" s="56"/>
+      <c r="AS74" s="56"/>
+      <c r="AT74" s="56"/>
+      <c r="AU74" s="56"/>
+      <c r="AV74" s="56"/>
+      <c r="AW74" s="56"/>
+      <c r="AX74" s="56"/>
+      <c r="AY74" s="56"/>
+      <c r="AZ74" s="56"/>
       <c r="BA74" s="12"/>
       <c r="BB74" s="13"/>
       <c r="BC74" s="14"/>
@@ -5811,8 +5815,8 @@
       <c r="J75" s="12"/>
       <c r="K75" s="14"/>
       <c r="L75" s="48"/>
-      <c r="M75" s="64"/>
-      <c r="N75" s="64"/>
+      <c r="M75" s="56"/>
+      <c r="N75" s="56"/>
       <c r="O75" s="1"/>
       <c r="P75" s="12"/>
       <c r="Q75" s="14"/>
@@ -5837,20 +5841,20 @@
       <c r="AJ75" s="13"/>
       <c r="AK75" s="13"/>
       <c r="AL75" s="14"/>
-      <c r="AM75" s="64"/>
-      <c r="AN75" s="64"/>
-      <c r="AO75" s="64"/>
-      <c r="AP75" s="64"/>
-      <c r="AQ75" s="64"/>
-      <c r="AR75" s="64"/>
-      <c r="AS75" s="64"/>
-      <c r="AT75" s="64"/>
-      <c r="AU75" s="64"/>
-      <c r="AV75" s="64"/>
-      <c r="AW75" s="64"/>
-      <c r="AX75" s="64"/>
-      <c r="AY75" s="64"/>
-      <c r="AZ75" s="64"/>
+      <c r="AM75" s="56"/>
+      <c r="AN75" s="56"/>
+      <c r="AO75" s="56"/>
+      <c r="AP75" s="56"/>
+      <c r="AQ75" s="56"/>
+      <c r="AR75" s="56"/>
+      <c r="AS75" s="56"/>
+      <c r="AT75" s="56"/>
+      <c r="AU75" s="56"/>
+      <c r="AV75" s="56"/>
+      <c r="AW75" s="56"/>
+      <c r="AX75" s="56"/>
+      <c r="AY75" s="56"/>
+      <c r="AZ75" s="56"/>
       <c r="BA75" s="12"/>
       <c r="BB75" s="13"/>
       <c r="BC75" s="14"/>
@@ -5867,8 +5871,8 @@
       <c r="J76" s="12"/>
       <c r="K76" s="14"/>
       <c r="L76" s="48"/>
-      <c r="M76" s="64"/>
-      <c r="N76" s="64"/>
+      <c r="M76" s="56"/>
+      <c r="N76" s="56"/>
       <c r="O76" s="1"/>
       <c r="P76" s="12"/>
       <c r="Q76" s="14"/>
@@ -5893,20 +5897,20 @@
       <c r="AJ76" s="13"/>
       <c r="AK76" s="13"/>
       <c r="AL76" s="14"/>
-      <c r="AM76" s="64"/>
-      <c r="AN76" s="64"/>
-      <c r="AO76" s="64"/>
-      <c r="AP76" s="64"/>
-      <c r="AQ76" s="64"/>
-      <c r="AR76" s="64"/>
-      <c r="AS76" s="64"/>
-      <c r="AT76" s="64"/>
-      <c r="AU76" s="64"/>
-      <c r="AV76" s="64"/>
-      <c r="AW76" s="64"/>
-      <c r="AX76" s="64"/>
-      <c r="AY76" s="64"/>
-      <c r="AZ76" s="64"/>
+      <c r="AM76" s="56"/>
+      <c r="AN76" s="56"/>
+      <c r="AO76" s="56"/>
+      <c r="AP76" s="56"/>
+      <c r="AQ76" s="56"/>
+      <c r="AR76" s="56"/>
+      <c r="AS76" s="56"/>
+      <c r="AT76" s="56"/>
+      <c r="AU76" s="56"/>
+      <c r="AV76" s="56"/>
+      <c r="AW76" s="56"/>
+      <c r="AX76" s="56"/>
+      <c r="AY76" s="56"/>
+      <c r="AZ76" s="56"/>
       <c r="BA76" s="12"/>
       <c r="BB76" s="13"/>
       <c r="BC76" s="14"/>
@@ -5923,8 +5927,8 @@
       <c r="J77" s="15"/>
       <c r="K77" s="17"/>
       <c r="L77" s="49"/>
-      <c r="M77" s="64"/>
-      <c r="N77" s="64"/>
+      <c r="M77" s="56"/>
+      <c r="N77" s="56"/>
       <c r="O77" s="1"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="14"/>
@@ -5992,66 +5996,66 @@
       </c>
       <c r="N78" s="11"/>
       <c r="O78" s="1"/>
-      <c r="P78" s="64" t="s">
+      <c r="P78" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="Q78" s="64"/>
+      <c r="Q78" s="56"/>
       <c r="R78" s="68" t="s">
         <v>63</v>
       </c>
       <c r="S78" s="68"/>
-      <c r="T78" s="64" t="s">
+      <c r="T78" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="U78" s="64"/>
-      <c r="V78" s="64" t="s">
+      <c r="U78" s="56"/>
+      <c r="V78" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="W78" s="64"/>
-      <c r="X78" s="64" t="s">
+      <c r="W78" s="56"/>
+      <c r="X78" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="Y78" s="64"/>
-      <c r="Z78" s="64"/>
-      <c r="AA78" s="64"/>
-      <c r="AB78" s="64" t="s">
+      <c r="Y78" s="56"/>
+      <c r="Z78" s="56"/>
+      <c r="AA78" s="56"/>
+      <c r="AB78" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="AC78" s="64"/>
-      <c r="AD78" s="64"/>
-      <c r="AE78" s="64"/>
-      <c r="AF78" s="64"/>
-      <c r="AG78" s="64" t="s">
+      <c r="AC78" s="56"/>
+      <c r="AD78" s="56"/>
+      <c r="AE78" s="56"/>
+      <c r="AF78" s="56"/>
+      <c r="AG78" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="AH78" s="64"/>
-      <c r="AI78" s="64"/>
-      <c r="AJ78" s="64"/>
-      <c r="AK78" s="64"/>
-      <c r="AL78" s="64"/>
-      <c r="AM78" s="64" t="s">
+      <c r="AH78" s="56"/>
+      <c r="AI78" s="56"/>
+      <c r="AJ78" s="56"/>
+      <c r="AK78" s="56"/>
+      <c r="AL78" s="56"/>
+      <c r="AM78" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="AN78" s="64"/>
-      <c r="AO78" s="64" t="s">
+      <c r="AN78" s="56"/>
+      <c r="AO78" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="AP78" s="64"/>
-      <c r="AQ78" s="64"/>
-      <c r="AR78" s="64"/>
-      <c r="AS78" s="64"/>
-      <c r="AT78" s="64"/>
-      <c r="AU78" s="64"/>
-      <c r="AV78" s="64"/>
-      <c r="AW78" s="64"/>
-      <c r="AX78" s="64"/>
-      <c r="AY78" s="64"/>
-      <c r="AZ78" s="64"/>
-      <c r="BA78" s="64" t="s">
+      <c r="AP78" s="56"/>
+      <c r="AQ78" s="56"/>
+      <c r="AR78" s="56"/>
+      <c r="AS78" s="56"/>
+      <c r="AT78" s="56"/>
+      <c r="AU78" s="56"/>
+      <c r="AV78" s="56"/>
+      <c r="AW78" s="56"/>
+      <c r="AX78" s="56"/>
+      <c r="AY78" s="56"/>
+      <c r="AZ78" s="56"/>
+      <c r="BA78" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="BB78" s="64"/>
-      <c r="BC78" s="64"/>
+      <c r="BB78" s="56"/>
+      <c r="BC78" s="56"/>
     </row>
     <row r="79" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B79" s="41"/>
@@ -6068,46 +6072,46 @@
       <c r="M79" s="12"/>
       <c r="N79" s="14"/>
       <c r="O79" s="1"/>
-      <c r="P79" s="64"/>
-      <c r="Q79" s="64"/>
+      <c r="P79" s="56"/>
+      <c r="Q79" s="56"/>
       <c r="R79" s="68"/>
       <c r="S79" s="68"/>
-      <c r="T79" s="64"/>
-      <c r="U79" s="64"/>
-      <c r="V79" s="64"/>
-      <c r="W79" s="64"/>
-      <c r="X79" s="64"/>
-      <c r="Y79" s="64"/>
-      <c r="Z79" s="64"/>
-      <c r="AA79" s="64"/>
-      <c r="AB79" s="64"/>
-      <c r="AC79" s="64"/>
-      <c r="AD79" s="64"/>
-      <c r="AE79" s="64"/>
-      <c r="AF79" s="64"/>
-      <c r="AG79" s="64"/>
-      <c r="AH79" s="64"/>
-      <c r="AI79" s="64"/>
-      <c r="AJ79" s="64"/>
-      <c r="AK79" s="64"/>
-      <c r="AL79" s="64"/>
-      <c r="AM79" s="64"/>
-      <c r="AN79" s="64"/>
-      <c r="AO79" s="64"/>
-      <c r="AP79" s="64"/>
-      <c r="AQ79" s="64"/>
-      <c r="AR79" s="64"/>
-      <c r="AS79" s="64"/>
-      <c r="AT79" s="64"/>
-      <c r="AU79" s="64"/>
-      <c r="AV79" s="64"/>
-      <c r="AW79" s="64"/>
-      <c r="AX79" s="64"/>
-      <c r="AY79" s="64"/>
-      <c r="AZ79" s="64"/>
-      <c r="BA79" s="64"/>
-      <c r="BB79" s="64"/>
-      <c r="BC79" s="64"/>
+      <c r="T79" s="56"/>
+      <c r="U79" s="56"/>
+      <c r="V79" s="56"/>
+      <c r="W79" s="56"/>
+      <c r="X79" s="56"/>
+      <c r="Y79" s="56"/>
+      <c r="Z79" s="56"/>
+      <c r="AA79" s="56"/>
+      <c r="AB79" s="56"/>
+      <c r="AC79" s="56"/>
+      <c r="AD79" s="56"/>
+      <c r="AE79" s="56"/>
+      <c r="AF79" s="56"/>
+      <c r="AG79" s="56"/>
+      <c r="AH79" s="56"/>
+      <c r="AI79" s="56"/>
+      <c r="AJ79" s="56"/>
+      <c r="AK79" s="56"/>
+      <c r="AL79" s="56"/>
+      <c r="AM79" s="56"/>
+      <c r="AN79" s="56"/>
+      <c r="AO79" s="56"/>
+      <c r="AP79" s="56"/>
+      <c r="AQ79" s="56"/>
+      <c r="AR79" s="56"/>
+      <c r="AS79" s="56"/>
+      <c r="AT79" s="56"/>
+      <c r="AU79" s="56"/>
+      <c r="AV79" s="56"/>
+      <c r="AW79" s="56"/>
+      <c r="AX79" s="56"/>
+      <c r="AY79" s="56"/>
+      <c r="AZ79" s="56"/>
+      <c r="BA79" s="56"/>
+      <c r="BB79" s="56"/>
+      <c r="BC79" s="56"/>
     </row>
     <row r="80" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B80" s="41"/>
@@ -6124,46 +6128,46 @@
       <c r="M80" s="12"/>
       <c r="N80" s="14"/>
       <c r="O80" s="1"/>
-      <c r="P80" s="64"/>
-      <c r="Q80" s="64"/>
+      <c r="P80" s="56"/>
+      <c r="Q80" s="56"/>
       <c r="R80" s="68"/>
       <c r="S80" s="68"/>
-      <c r="T80" s="64"/>
-      <c r="U80" s="64"/>
-      <c r="V80" s="64"/>
-      <c r="W80" s="64"/>
-      <c r="X80" s="64"/>
-      <c r="Y80" s="64"/>
-      <c r="Z80" s="64"/>
-      <c r="AA80" s="64"/>
-      <c r="AB80" s="64"/>
-      <c r="AC80" s="64"/>
-      <c r="AD80" s="64"/>
-      <c r="AE80" s="64"/>
-      <c r="AF80" s="64"/>
-      <c r="AG80" s="64"/>
-      <c r="AH80" s="64"/>
-      <c r="AI80" s="64"/>
-      <c r="AJ80" s="64"/>
-      <c r="AK80" s="64"/>
-      <c r="AL80" s="64"/>
-      <c r="AM80" s="64"/>
-      <c r="AN80" s="64"/>
-      <c r="AO80" s="64"/>
-      <c r="AP80" s="64"/>
-      <c r="AQ80" s="64"/>
-      <c r="AR80" s="64"/>
-      <c r="AS80" s="64"/>
-      <c r="AT80" s="64"/>
-      <c r="AU80" s="64"/>
-      <c r="AV80" s="64"/>
-      <c r="AW80" s="64"/>
-      <c r="AX80" s="64"/>
-      <c r="AY80" s="64"/>
-      <c r="AZ80" s="64"/>
-      <c r="BA80" s="64"/>
-      <c r="BB80" s="64"/>
-      <c r="BC80" s="64"/>
+      <c r="T80" s="56"/>
+      <c r="U80" s="56"/>
+      <c r="V80" s="56"/>
+      <c r="W80" s="56"/>
+      <c r="X80" s="56"/>
+      <c r="Y80" s="56"/>
+      <c r="Z80" s="56"/>
+      <c r="AA80" s="56"/>
+      <c r="AB80" s="56"/>
+      <c r="AC80" s="56"/>
+      <c r="AD80" s="56"/>
+      <c r="AE80" s="56"/>
+      <c r="AF80" s="56"/>
+      <c r="AG80" s="56"/>
+      <c r="AH80" s="56"/>
+      <c r="AI80" s="56"/>
+      <c r="AJ80" s="56"/>
+      <c r="AK80" s="56"/>
+      <c r="AL80" s="56"/>
+      <c r="AM80" s="56"/>
+      <c r="AN80" s="56"/>
+      <c r="AO80" s="56"/>
+      <c r="AP80" s="56"/>
+      <c r="AQ80" s="56"/>
+      <c r="AR80" s="56"/>
+      <c r="AS80" s="56"/>
+      <c r="AT80" s="56"/>
+      <c r="AU80" s="56"/>
+      <c r="AV80" s="56"/>
+      <c r="AW80" s="56"/>
+      <c r="AX80" s="56"/>
+      <c r="AY80" s="56"/>
+      <c r="AZ80" s="56"/>
+      <c r="BA80" s="56"/>
+      <c r="BB80" s="56"/>
+      <c r="BC80" s="56"/>
     </row>
     <row r="81" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B81" s="41"/>
@@ -6180,46 +6184,46 @@
       <c r="M81" s="12"/>
       <c r="N81" s="14"/>
       <c r="O81" s="1"/>
-      <c r="P81" s="64"/>
-      <c r="Q81" s="64"/>
+      <c r="P81" s="56"/>
+      <c r="Q81" s="56"/>
       <c r="R81" s="68"/>
       <c r="S81" s="68"/>
-      <c r="T81" s="64"/>
-      <c r="U81" s="64"/>
-      <c r="V81" s="64"/>
-      <c r="W81" s="64"/>
-      <c r="X81" s="64"/>
-      <c r="Y81" s="64"/>
-      <c r="Z81" s="64"/>
-      <c r="AA81" s="64"/>
-      <c r="AB81" s="64"/>
-      <c r="AC81" s="64"/>
-      <c r="AD81" s="64"/>
-      <c r="AE81" s="64"/>
-      <c r="AF81" s="64"/>
-      <c r="AG81" s="64"/>
-      <c r="AH81" s="64"/>
-      <c r="AI81" s="64"/>
-      <c r="AJ81" s="64"/>
-      <c r="AK81" s="64"/>
-      <c r="AL81" s="64"/>
-      <c r="AM81" s="64"/>
-      <c r="AN81" s="64"/>
-      <c r="AO81" s="64"/>
-      <c r="AP81" s="64"/>
-      <c r="AQ81" s="64"/>
-      <c r="AR81" s="64"/>
-      <c r="AS81" s="64"/>
-      <c r="AT81" s="64"/>
-      <c r="AU81" s="64"/>
-      <c r="AV81" s="64"/>
-      <c r="AW81" s="64"/>
-      <c r="AX81" s="64"/>
-      <c r="AY81" s="64"/>
-      <c r="AZ81" s="64"/>
-      <c r="BA81" s="64"/>
-      <c r="BB81" s="64"/>
-      <c r="BC81" s="64"/>
+      <c r="T81" s="56"/>
+      <c r="U81" s="56"/>
+      <c r="V81" s="56"/>
+      <c r="W81" s="56"/>
+      <c r="X81" s="56"/>
+      <c r="Y81" s="56"/>
+      <c r="Z81" s="56"/>
+      <c r="AA81" s="56"/>
+      <c r="AB81" s="56"/>
+      <c r="AC81" s="56"/>
+      <c r="AD81" s="56"/>
+      <c r="AE81" s="56"/>
+      <c r="AF81" s="56"/>
+      <c r="AG81" s="56"/>
+      <c r="AH81" s="56"/>
+      <c r="AI81" s="56"/>
+      <c r="AJ81" s="56"/>
+      <c r="AK81" s="56"/>
+      <c r="AL81" s="56"/>
+      <c r="AM81" s="56"/>
+      <c r="AN81" s="56"/>
+      <c r="AO81" s="56"/>
+      <c r="AP81" s="56"/>
+      <c r="AQ81" s="56"/>
+      <c r="AR81" s="56"/>
+      <c r="AS81" s="56"/>
+      <c r="AT81" s="56"/>
+      <c r="AU81" s="56"/>
+      <c r="AV81" s="56"/>
+      <c r="AW81" s="56"/>
+      <c r="AX81" s="56"/>
+      <c r="AY81" s="56"/>
+      <c r="AZ81" s="56"/>
+      <c r="BA81" s="56"/>
+      <c r="BB81" s="56"/>
+      <c r="BC81" s="56"/>
     </row>
     <row r="82" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B82" s="41"/>
@@ -6236,46 +6240,46 @@
       <c r="M82" s="12"/>
       <c r="N82" s="14"/>
       <c r="O82" s="1"/>
-      <c r="P82" s="64"/>
-      <c r="Q82" s="64"/>
+      <c r="P82" s="56"/>
+      <c r="Q82" s="56"/>
       <c r="R82" s="68"/>
       <c r="S82" s="68"/>
-      <c r="T82" s="64"/>
-      <c r="U82" s="64"/>
-      <c r="V82" s="64"/>
-      <c r="W82" s="64"/>
-      <c r="X82" s="64"/>
-      <c r="Y82" s="64"/>
-      <c r="Z82" s="64"/>
-      <c r="AA82" s="64"/>
-      <c r="AB82" s="64"/>
-      <c r="AC82" s="64"/>
-      <c r="AD82" s="64"/>
-      <c r="AE82" s="64"/>
-      <c r="AF82" s="64"/>
-      <c r="AG82" s="64"/>
-      <c r="AH82" s="64"/>
-      <c r="AI82" s="64"/>
-      <c r="AJ82" s="64"/>
-      <c r="AK82" s="64"/>
-      <c r="AL82" s="64"/>
-      <c r="AM82" s="64"/>
-      <c r="AN82" s="64"/>
-      <c r="AO82" s="64"/>
-      <c r="AP82" s="64"/>
-      <c r="AQ82" s="64"/>
-      <c r="AR82" s="64"/>
-      <c r="AS82" s="64"/>
-      <c r="AT82" s="64"/>
-      <c r="AU82" s="64"/>
-      <c r="AV82" s="64"/>
-      <c r="AW82" s="64"/>
-      <c r="AX82" s="64"/>
-      <c r="AY82" s="64"/>
-      <c r="AZ82" s="64"/>
-      <c r="BA82" s="64"/>
-      <c r="BB82" s="64"/>
-      <c r="BC82" s="64"/>
+      <c r="T82" s="56"/>
+      <c r="U82" s="56"/>
+      <c r="V82" s="56"/>
+      <c r="W82" s="56"/>
+      <c r="X82" s="56"/>
+      <c r="Y82" s="56"/>
+      <c r="Z82" s="56"/>
+      <c r="AA82" s="56"/>
+      <c r="AB82" s="56"/>
+      <c r="AC82" s="56"/>
+      <c r="AD82" s="56"/>
+      <c r="AE82" s="56"/>
+      <c r="AF82" s="56"/>
+      <c r="AG82" s="56"/>
+      <c r="AH82" s="56"/>
+      <c r="AI82" s="56"/>
+      <c r="AJ82" s="56"/>
+      <c r="AK82" s="56"/>
+      <c r="AL82" s="56"/>
+      <c r="AM82" s="56"/>
+      <c r="AN82" s="56"/>
+      <c r="AO82" s="56"/>
+      <c r="AP82" s="56"/>
+      <c r="AQ82" s="56"/>
+      <c r="AR82" s="56"/>
+      <c r="AS82" s="56"/>
+      <c r="AT82" s="56"/>
+      <c r="AU82" s="56"/>
+      <c r="AV82" s="56"/>
+      <c r="AW82" s="56"/>
+      <c r="AX82" s="56"/>
+      <c r="AY82" s="56"/>
+      <c r="AZ82" s="56"/>
+      <c r="BA82" s="56"/>
+      <c r="BB82" s="56"/>
+      <c r="BC82" s="56"/>
     </row>
     <row r="83" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B83" s="41"/>
@@ -6292,46 +6296,46 @@
       <c r="M83" s="12"/>
       <c r="N83" s="14"/>
       <c r="O83" s="1"/>
-      <c r="P83" s="64"/>
-      <c r="Q83" s="64"/>
+      <c r="P83" s="56"/>
+      <c r="Q83" s="56"/>
       <c r="R83" s="68"/>
       <c r="S83" s="68"/>
-      <c r="T83" s="64"/>
-      <c r="U83" s="64"/>
-      <c r="V83" s="64"/>
-      <c r="W83" s="64"/>
-      <c r="X83" s="64"/>
-      <c r="Y83" s="64"/>
-      <c r="Z83" s="64"/>
-      <c r="AA83" s="64"/>
-      <c r="AB83" s="64"/>
-      <c r="AC83" s="64"/>
-      <c r="AD83" s="64"/>
-      <c r="AE83" s="64"/>
-      <c r="AF83" s="64"/>
-      <c r="AG83" s="64"/>
-      <c r="AH83" s="64"/>
-      <c r="AI83" s="64"/>
-      <c r="AJ83" s="64"/>
-      <c r="AK83" s="64"/>
-      <c r="AL83" s="64"/>
-      <c r="AM83" s="64"/>
-      <c r="AN83" s="64"/>
-      <c r="AO83" s="64"/>
-      <c r="AP83" s="64"/>
-      <c r="AQ83" s="64"/>
-      <c r="AR83" s="64"/>
-      <c r="AS83" s="64"/>
-      <c r="AT83" s="64"/>
-      <c r="AU83" s="64"/>
-      <c r="AV83" s="64"/>
-      <c r="AW83" s="64"/>
-      <c r="AX83" s="64"/>
-      <c r="AY83" s="64"/>
-      <c r="AZ83" s="64"/>
-      <c r="BA83" s="64"/>
-      <c r="BB83" s="64"/>
-      <c r="BC83" s="64"/>
+      <c r="T83" s="56"/>
+      <c r="U83" s="56"/>
+      <c r="V83" s="56"/>
+      <c r="W83" s="56"/>
+      <c r="X83" s="56"/>
+      <c r="Y83" s="56"/>
+      <c r="Z83" s="56"/>
+      <c r="AA83" s="56"/>
+      <c r="AB83" s="56"/>
+      <c r="AC83" s="56"/>
+      <c r="AD83" s="56"/>
+      <c r="AE83" s="56"/>
+      <c r="AF83" s="56"/>
+      <c r="AG83" s="56"/>
+      <c r="AH83" s="56"/>
+      <c r="AI83" s="56"/>
+      <c r="AJ83" s="56"/>
+      <c r="AK83" s="56"/>
+      <c r="AL83" s="56"/>
+      <c r="AM83" s="56"/>
+      <c r="AN83" s="56"/>
+      <c r="AO83" s="56"/>
+      <c r="AP83" s="56"/>
+      <c r="AQ83" s="56"/>
+      <c r="AR83" s="56"/>
+      <c r="AS83" s="56"/>
+      <c r="AT83" s="56"/>
+      <c r="AU83" s="56"/>
+      <c r="AV83" s="56"/>
+      <c r="AW83" s="56"/>
+      <c r="AX83" s="56"/>
+      <c r="AY83" s="56"/>
+      <c r="AZ83" s="56"/>
+      <c r="BA83" s="56"/>
+      <c r="BB83" s="56"/>
+      <c r="BC83" s="56"/>
     </row>
     <row r="84" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B84" s="41"/>
@@ -6348,46 +6352,46 @@
       <c r="M84" s="12"/>
       <c r="N84" s="14"/>
       <c r="O84" s="1"/>
-      <c r="P84" s="64"/>
-      <c r="Q84" s="64"/>
+      <c r="P84" s="56"/>
+      <c r="Q84" s="56"/>
       <c r="R84" s="68"/>
       <c r="S84" s="68"/>
-      <c r="T84" s="64"/>
-      <c r="U84" s="64"/>
-      <c r="V84" s="64"/>
-      <c r="W84" s="64"/>
-      <c r="X84" s="64"/>
-      <c r="Y84" s="64"/>
-      <c r="Z84" s="64"/>
-      <c r="AA84" s="64"/>
-      <c r="AB84" s="64"/>
-      <c r="AC84" s="64"/>
-      <c r="AD84" s="64"/>
-      <c r="AE84" s="64"/>
-      <c r="AF84" s="64"/>
-      <c r="AG84" s="64"/>
-      <c r="AH84" s="64"/>
-      <c r="AI84" s="64"/>
-      <c r="AJ84" s="64"/>
-      <c r="AK84" s="64"/>
-      <c r="AL84" s="64"/>
-      <c r="AM84" s="64"/>
-      <c r="AN84" s="64"/>
-      <c r="AO84" s="64"/>
-      <c r="AP84" s="64"/>
-      <c r="AQ84" s="64"/>
-      <c r="AR84" s="64"/>
-      <c r="AS84" s="64"/>
-      <c r="AT84" s="64"/>
-      <c r="AU84" s="64"/>
-      <c r="AV84" s="64"/>
-      <c r="AW84" s="64"/>
-      <c r="AX84" s="64"/>
-      <c r="AY84" s="64"/>
-      <c r="AZ84" s="64"/>
-      <c r="BA84" s="64"/>
-      <c r="BB84" s="64"/>
-      <c r="BC84" s="64"/>
+      <c r="T84" s="56"/>
+      <c r="U84" s="56"/>
+      <c r="V84" s="56"/>
+      <c r="W84" s="56"/>
+      <c r="X84" s="56"/>
+      <c r="Y84" s="56"/>
+      <c r="Z84" s="56"/>
+      <c r="AA84" s="56"/>
+      <c r="AB84" s="56"/>
+      <c r="AC84" s="56"/>
+      <c r="AD84" s="56"/>
+      <c r="AE84" s="56"/>
+      <c r="AF84" s="56"/>
+      <c r="AG84" s="56"/>
+      <c r="AH84" s="56"/>
+      <c r="AI84" s="56"/>
+      <c r="AJ84" s="56"/>
+      <c r="AK84" s="56"/>
+      <c r="AL84" s="56"/>
+      <c r="AM84" s="56"/>
+      <c r="AN84" s="56"/>
+      <c r="AO84" s="56"/>
+      <c r="AP84" s="56"/>
+      <c r="AQ84" s="56"/>
+      <c r="AR84" s="56"/>
+      <c r="AS84" s="56"/>
+      <c r="AT84" s="56"/>
+      <c r="AU84" s="56"/>
+      <c r="AV84" s="56"/>
+      <c r="AW84" s="56"/>
+      <c r="AX84" s="56"/>
+      <c r="AY84" s="56"/>
+      <c r="AZ84" s="56"/>
+      <c r="BA84" s="56"/>
+      <c r="BB84" s="56"/>
+      <c r="BC84" s="56"/>
     </row>
     <row r="85" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B85" s="41"/>
@@ -6404,46 +6408,46 @@
       <c r="M85" s="12"/>
       <c r="N85" s="14"/>
       <c r="O85" s="1"/>
-      <c r="P85" s="64"/>
-      <c r="Q85" s="64"/>
+      <c r="P85" s="56"/>
+      <c r="Q85" s="56"/>
       <c r="R85" s="68"/>
       <c r="S85" s="68"/>
-      <c r="T85" s="64"/>
-      <c r="U85" s="64"/>
-      <c r="V85" s="64"/>
-      <c r="W85" s="64"/>
-      <c r="X85" s="64"/>
-      <c r="Y85" s="64"/>
-      <c r="Z85" s="64"/>
-      <c r="AA85" s="64"/>
-      <c r="AB85" s="64"/>
-      <c r="AC85" s="64"/>
-      <c r="AD85" s="64"/>
-      <c r="AE85" s="64"/>
-      <c r="AF85" s="64"/>
-      <c r="AG85" s="64"/>
-      <c r="AH85" s="64"/>
-      <c r="AI85" s="64"/>
-      <c r="AJ85" s="64"/>
-      <c r="AK85" s="64"/>
-      <c r="AL85" s="64"/>
-      <c r="AM85" s="64"/>
-      <c r="AN85" s="64"/>
-      <c r="AO85" s="64"/>
-      <c r="AP85" s="64"/>
-      <c r="AQ85" s="64"/>
-      <c r="AR85" s="64"/>
-      <c r="AS85" s="64"/>
-      <c r="AT85" s="64"/>
-      <c r="AU85" s="64"/>
-      <c r="AV85" s="64"/>
-      <c r="AW85" s="64"/>
-      <c r="AX85" s="64"/>
-      <c r="AY85" s="64"/>
-      <c r="AZ85" s="64"/>
-      <c r="BA85" s="64"/>
-      <c r="BB85" s="64"/>
-      <c r="BC85" s="64"/>
+      <c r="T85" s="56"/>
+      <c r="U85" s="56"/>
+      <c r="V85" s="56"/>
+      <c r="W85" s="56"/>
+      <c r="X85" s="56"/>
+      <c r="Y85" s="56"/>
+      <c r="Z85" s="56"/>
+      <c r="AA85" s="56"/>
+      <c r="AB85" s="56"/>
+      <c r="AC85" s="56"/>
+      <c r="AD85" s="56"/>
+      <c r="AE85" s="56"/>
+      <c r="AF85" s="56"/>
+      <c r="AG85" s="56"/>
+      <c r="AH85" s="56"/>
+      <c r="AI85" s="56"/>
+      <c r="AJ85" s="56"/>
+      <c r="AK85" s="56"/>
+      <c r="AL85" s="56"/>
+      <c r="AM85" s="56"/>
+      <c r="AN85" s="56"/>
+      <c r="AO85" s="56"/>
+      <c r="AP85" s="56"/>
+      <c r="AQ85" s="56"/>
+      <c r="AR85" s="56"/>
+      <c r="AS85" s="56"/>
+      <c r="AT85" s="56"/>
+      <c r="AU85" s="56"/>
+      <c r="AV85" s="56"/>
+      <c r="AW85" s="56"/>
+      <c r="AX85" s="56"/>
+      <c r="AY85" s="56"/>
+      <c r="AZ85" s="56"/>
+      <c r="BA85" s="56"/>
+      <c r="BB85" s="56"/>
+      <c r="BC85" s="56"/>
     </row>
     <row r="86" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B86" s="41"/>
@@ -6460,46 +6464,46 @@
       <c r="M86" s="12"/>
       <c r="N86" s="14"/>
       <c r="O86" s="1"/>
-      <c r="P86" s="64"/>
-      <c r="Q86" s="64"/>
+      <c r="P86" s="56"/>
+      <c r="Q86" s="56"/>
       <c r="R86" s="68"/>
       <c r="S86" s="68"/>
-      <c r="T86" s="64"/>
-      <c r="U86" s="64"/>
-      <c r="V86" s="64"/>
-      <c r="W86" s="64"/>
-      <c r="X86" s="64"/>
-      <c r="Y86" s="64"/>
-      <c r="Z86" s="64"/>
-      <c r="AA86" s="64"/>
-      <c r="AB86" s="64"/>
-      <c r="AC86" s="64"/>
-      <c r="AD86" s="64"/>
-      <c r="AE86" s="64"/>
-      <c r="AF86" s="64"/>
-      <c r="AG86" s="64"/>
-      <c r="AH86" s="64"/>
-      <c r="AI86" s="64"/>
-      <c r="AJ86" s="64"/>
-      <c r="AK86" s="64"/>
-      <c r="AL86" s="64"/>
-      <c r="AM86" s="64"/>
-      <c r="AN86" s="64"/>
-      <c r="AO86" s="64"/>
-      <c r="AP86" s="64"/>
-      <c r="AQ86" s="64"/>
-      <c r="AR86" s="64"/>
-      <c r="AS86" s="64"/>
-      <c r="AT86" s="64"/>
-      <c r="AU86" s="64"/>
-      <c r="AV86" s="64"/>
-      <c r="AW86" s="64"/>
-      <c r="AX86" s="64"/>
-      <c r="AY86" s="64"/>
-      <c r="AZ86" s="64"/>
-      <c r="BA86" s="64"/>
-      <c r="BB86" s="64"/>
-      <c r="BC86" s="64"/>
+      <c r="T86" s="56"/>
+      <c r="U86" s="56"/>
+      <c r="V86" s="56"/>
+      <c r="W86" s="56"/>
+      <c r="X86" s="56"/>
+      <c r="Y86" s="56"/>
+      <c r="Z86" s="56"/>
+      <c r="AA86" s="56"/>
+      <c r="AB86" s="56"/>
+      <c r="AC86" s="56"/>
+      <c r="AD86" s="56"/>
+      <c r="AE86" s="56"/>
+      <c r="AF86" s="56"/>
+      <c r="AG86" s="56"/>
+      <c r="AH86" s="56"/>
+      <c r="AI86" s="56"/>
+      <c r="AJ86" s="56"/>
+      <c r="AK86" s="56"/>
+      <c r="AL86" s="56"/>
+      <c r="AM86" s="56"/>
+      <c r="AN86" s="56"/>
+      <c r="AO86" s="56"/>
+      <c r="AP86" s="56"/>
+      <c r="AQ86" s="56"/>
+      <c r="AR86" s="56"/>
+      <c r="AS86" s="56"/>
+      <c r="AT86" s="56"/>
+      <c r="AU86" s="56"/>
+      <c r="AV86" s="56"/>
+      <c r="AW86" s="56"/>
+      <c r="AX86" s="56"/>
+      <c r="AY86" s="56"/>
+      <c r="AZ86" s="56"/>
+      <c r="BA86" s="56"/>
+      <c r="BB86" s="56"/>
+      <c r="BC86" s="56"/>
     </row>
     <row r="87" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B87" s="44"/>
@@ -6516,46 +6520,46 @@
       <c r="M87" s="15"/>
       <c r="N87" s="17"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="64"/>
-      <c r="Q87" s="64"/>
+      <c r="P87" s="56"/>
+      <c r="Q87" s="56"/>
       <c r="R87" s="68"/>
       <c r="S87" s="68"/>
-      <c r="T87" s="64"/>
-      <c r="U87" s="64"/>
-      <c r="V87" s="64"/>
-      <c r="W87" s="64"/>
-      <c r="X87" s="64"/>
-      <c r="Y87" s="64"/>
-      <c r="Z87" s="64"/>
-      <c r="AA87" s="64"/>
-      <c r="AB87" s="64"/>
-      <c r="AC87" s="64"/>
-      <c r="AD87" s="64"/>
-      <c r="AE87" s="64"/>
-      <c r="AF87" s="64"/>
-      <c r="AG87" s="64"/>
-      <c r="AH87" s="64"/>
-      <c r="AI87" s="64"/>
-      <c r="AJ87" s="64"/>
-      <c r="AK87" s="64"/>
-      <c r="AL87" s="64"/>
-      <c r="AM87" s="64"/>
-      <c r="AN87" s="64"/>
-      <c r="AO87" s="64"/>
-      <c r="AP87" s="64"/>
-      <c r="AQ87" s="64"/>
-      <c r="AR87" s="64"/>
-      <c r="AS87" s="64"/>
-      <c r="AT87" s="64"/>
-      <c r="AU87" s="64"/>
-      <c r="AV87" s="64"/>
-      <c r="AW87" s="64"/>
-      <c r="AX87" s="64"/>
-      <c r="AY87" s="64"/>
-      <c r="AZ87" s="64"/>
-      <c r="BA87" s="64"/>
-      <c r="BB87" s="64"/>
-      <c r="BC87" s="64"/>
+      <c r="T87" s="56"/>
+      <c r="U87" s="56"/>
+      <c r="V87" s="56"/>
+      <c r="W87" s="56"/>
+      <c r="X87" s="56"/>
+      <c r="Y87" s="56"/>
+      <c r="Z87" s="56"/>
+      <c r="AA87" s="56"/>
+      <c r="AB87" s="56"/>
+      <c r="AC87" s="56"/>
+      <c r="AD87" s="56"/>
+      <c r="AE87" s="56"/>
+      <c r="AF87" s="56"/>
+      <c r="AG87" s="56"/>
+      <c r="AH87" s="56"/>
+      <c r="AI87" s="56"/>
+      <c r="AJ87" s="56"/>
+      <c r="AK87" s="56"/>
+      <c r="AL87" s="56"/>
+      <c r="AM87" s="56"/>
+      <c r="AN87" s="56"/>
+      <c r="AO87" s="56"/>
+      <c r="AP87" s="56"/>
+      <c r="AQ87" s="56"/>
+      <c r="AR87" s="56"/>
+      <c r="AS87" s="56"/>
+      <c r="AT87" s="56"/>
+      <c r="AU87" s="56"/>
+      <c r="AV87" s="56"/>
+      <c r="AW87" s="56"/>
+      <c r="AX87" s="56"/>
+      <c r="AY87" s="56"/>
+      <c r="AZ87" s="56"/>
+      <c r="BA87" s="56"/>
+      <c r="BB87" s="56"/>
+      <c r="BC87" s="56"/>
     </row>
     <row r="88" spans="2:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O88" s="1"/>
@@ -7104,68 +7108,68 @@
       <c r="M100" s="71"/>
       <c r="N100" s="71"/>
       <c r="O100" s="4"/>
-      <c r="P100" s="88" t="s">
+      <c r="P100" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="Q100" s="88"/>
-      <c r="R100" s="87" t="s">
+      <c r="Q100" s="72"/>
+      <c r="R100" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="S100" s="87"/>
-      <c r="T100" s="87" t="s">
+      <c r="S100" s="73"/>
+      <c r="T100" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="U100" s="87"/>
-      <c r="V100" s="87" t="s">
+      <c r="U100" s="73"/>
+      <c r="V100" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="W100" s="87"/>
-      <c r="X100" s="87" t="s">
+      <c r="W100" s="73"/>
+      <c r="X100" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="Y100" s="87"/>
-      <c r="Z100" s="87"/>
-      <c r="AA100" s="87"/>
-      <c r="AB100" s="87" t="s">
+      <c r="Y100" s="73"/>
+      <c r="Z100" s="73"/>
+      <c r="AA100" s="73"/>
+      <c r="AB100" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="AC100" s="87"/>
-      <c r="AD100" s="87"/>
-      <c r="AE100" s="87"/>
-      <c r="AF100" s="87"/>
-      <c r="AG100" s="87" t="s">
+      <c r="AC100" s="73"/>
+      <c r="AD100" s="73"/>
+      <c r="AE100" s="73"/>
+      <c r="AF100" s="73"/>
+      <c r="AG100" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AH100" s="87"/>
-      <c r="AI100" s="87"/>
-      <c r="AJ100" s="87"/>
-      <c r="AK100" s="87"/>
-      <c r="AL100" s="87"/>
-      <c r="AM100" s="87" t="s">
+      <c r="AH100" s="73"/>
+      <c r="AI100" s="73"/>
+      <c r="AJ100" s="73"/>
+      <c r="AK100" s="73"/>
+      <c r="AL100" s="73"/>
+      <c r="AM100" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="AN100" s="87"/>
-      <c r="AO100" s="87" t="s">
+      <c r="AN100" s="73"/>
+      <c r="AO100" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="AP100" s="87"/>
-      <c r="AQ100" s="87"/>
-      <c r="AR100" s="87"/>
-      <c r="AS100" s="87"/>
-      <c r="AT100" s="87"/>
-      <c r="AU100" s="87" t="s">
+      <c r="AP100" s="73"/>
+      <c r="AQ100" s="73"/>
+      <c r="AR100" s="73"/>
+      <c r="AS100" s="73"/>
+      <c r="AT100" s="73"/>
+      <c r="AU100" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="AV100" s="87"/>
-      <c r="AW100" s="87"/>
-      <c r="AX100" s="87"/>
-      <c r="AY100" s="87"/>
-      <c r="AZ100" s="87"/>
-      <c r="BA100" s="87" t="s">
+      <c r="AV100" s="73"/>
+      <c r="AW100" s="73"/>
+      <c r="AX100" s="73"/>
+      <c r="AY100" s="73"/>
+      <c r="AZ100" s="73"/>
+      <c r="BA100" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="BB100" s="87"/>
-      <c r="BC100" s="87"/>
+      <c r="BB100" s="73"/>
+      <c r="BC100" s="73"/>
     </row>
     <row r="101" spans="6:55" x14ac:dyDescent="0.25">
       <c r="F101" s="71"/>
@@ -7178,46 +7182,46 @@
       <c r="M101" s="71"/>
       <c r="N101" s="71"/>
       <c r="O101" s="4"/>
-      <c r="P101" s="88"/>
-      <c r="Q101" s="88"/>
-      <c r="R101" s="87"/>
-      <c r="S101" s="87"/>
-      <c r="T101" s="87"/>
-      <c r="U101" s="87"/>
-      <c r="V101" s="87"/>
-      <c r="W101" s="87"/>
-      <c r="X101" s="87"/>
-      <c r="Y101" s="87"/>
-      <c r="Z101" s="87"/>
-      <c r="AA101" s="87"/>
-      <c r="AB101" s="87"/>
-      <c r="AC101" s="87"/>
-      <c r="AD101" s="87"/>
-      <c r="AE101" s="87"/>
-      <c r="AF101" s="87"/>
-      <c r="AG101" s="87"/>
-      <c r="AH101" s="87"/>
-      <c r="AI101" s="87"/>
-      <c r="AJ101" s="87"/>
-      <c r="AK101" s="87"/>
-      <c r="AL101" s="87"/>
-      <c r="AM101" s="87"/>
-      <c r="AN101" s="87"/>
-      <c r="AO101" s="87"/>
-      <c r="AP101" s="87"/>
-      <c r="AQ101" s="87"/>
-      <c r="AR101" s="87"/>
-      <c r="AS101" s="87"/>
-      <c r="AT101" s="87"/>
-      <c r="AU101" s="87"/>
-      <c r="AV101" s="87"/>
-      <c r="AW101" s="87"/>
-      <c r="AX101" s="87"/>
-      <c r="AY101" s="87"/>
-      <c r="AZ101" s="87"/>
-      <c r="BA101" s="87"/>
-      <c r="BB101" s="87"/>
-      <c r="BC101" s="87"/>
+      <c r="P101" s="72"/>
+      <c r="Q101" s="72"/>
+      <c r="R101" s="73"/>
+      <c r="S101" s="73"/>
+      <c r="T101" s="73"/>
+      <c r="U101" s="73"/>
+      <c r="V101" s="73"/>
+      <c r="W101" s="73"/>
+      <c r="X101" s="73"/>
+      <c r="Y101" s="73"/>
+      <c r="Z101" s="73"/>
+      <c r="AA101" s="73"/>
+      <c r="AB101" s="73"/>
+      <c r="AC101" s="73"/>
+      <c r="AD101" s="73"/>
+      <c r="AE101" s="73"/>
+      <c r="AF101" s="73"/>
+      <c r="AG101" s="73"/>
+      <c r="AH101" s="73"/>
+      <c r="AI101" s="73"/>
+      <c r="AJ101" s="73"/>
+      <c r="AK101" s="73"/>
+      <c r="AL101" s="73"/>
+      <c r="AM101" s="73"/>
+      <c r="AN101" s="73"/>
+      <c r="AO101" s="73"/>
+      <c r="AP101" s="73"/>
+      <c r="AQ101" s="73"/>
+      <c r="AR101" s="73"/>
+      <c r="AS101" s="73"/>
+      <c r="AT101" s="73"/>
+      <c r="AU101" s="73"/>
+      <c r="AV101" s="73"/>
+      <c r="AW101" s="73"/>
+      <c r="AX101" s="73"/>
+      <c r="AY101" s="73"/>
+      <c r="AZ101" s="73"/>
+      <c r="BA101" s="73"/>
+      <c r="BB101" s="73"/>
+      <c r="BC101" s="73"/>
     </row>
     <row r="102" spans="6:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F102" s="50" t="s">
@@ -7230,7 +7234,7 @@
         <v>19</v>
       </c>
       <c r="K102" s="52"/>
-      <c r="L102" s="72" t="s">
+      <c r="L102" s="98" t="s">
         <v>20</v>
       </c>
       <c r="M102" s="50" t="s">
@@ -7306,7 +7310,7 @@
       <c r="I103" s="55"/>
       <c r="J103" s="65"/>
       <c r="K103" s="67"/>
-      <c r="L103" s="73"/>
+      <c r="L103" s="99"/>
       <c r="M103" s="65"/>
       <c r="N103" s="67"/>
       <c r="O103" s="4"/>
@@ -7362,7 +7366,7 @@
       <c r="I104" s="52"/>
       <c r="J104" s="65"/>
       <c r="K104" s="67"/>
-      <c r="L104" s="73"/>
+      <c r="L104" s="99"/>
       <c r="M104" s="65"/>
       <c r="N104" s="67"/>
       <c r="O104" s="4"/>
@@ -7414,7 +7418,7 @@
       <c r="I105" s="55"/>
       <c r="J105" s="53"/>
       <c r="K105" s="55"/>
-      <c r="L105" s="74"/>
+      <c r="L105" s="100"/>
       <c r="M105" s="53"/>
       <c r="N105" s="55"/>
       <c r="O105" s="4"/>
@@ -7475,10 +7479,10 @@
       <c r="L106" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="M106" s="64" t="s">
+      <c r="M106" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="N106" s="64"/>
+      <c r="N106" s="56"/>
       <c r="O106" s="6"/>
       <c r="P106" s="12"/>
       <c r="Q106" s="14"/>
@@ -7529,8 +7533,8 @@
       <c r="J107" s="12"/>
       <c r="K107" s="14"/>
       <c r="L107" s="48"/>
-      <c r="M107" s="64"/>
-      <c r="N107" s="64"/>
+      <c r="M107" s="56"/>
+      <c r="N107" s="56"/>
       <c r="O107" s="6"/>
       <c r="P107" s="12"/>
       <c r="Q107" s="14"/>
@@ -7581,8 +7585,8 @@
       <c r="J108" s="12"/>
       <c r="K108" s="14"/>
       <c r="L108" s="48"/>
-      <c r="M108" s="64"/>
-      <c r="N108" s="64"/>
+      <c r="M108" s="56"/>
+      <c r="N108" s="56"/>
       <c r="O108" s="1"/>
       <c r="P108" s="12"/>
       <c r="Q108" s="14"/>
@@ -7633,8 +7637,8 @@
       <c r="J109" s="12"/>
       <c r="K109" s="14"/>
       <c r="L109" s="48"/>
-      <c r="M109" s="64"/>
-      <c r="N109" s="64"/>
+      <c r="M109" s="56"/>
+      <c r="N109" s="56"/>
       <c r="O109" s="1"/>
       <c r="P109" s="12"/>
       <c r="Q109" s="14"/>
@@ -7685,8 +7689,8 @@
       <c r="J110" s="12"/>
       <c r="K110" s="14"/>
       <c r="L110" s="48"/>
-      <c r="M110" s="64"/>
-      <c r="N110" s="64"/>
+      <c r="M110" s="56"/>
+      <c r="N110" s="56"/>
       <c r="O110" s="1"/>
       <c r="P110" s="12"/>
       <c r="Q110" s="14"/>
@@ -7737,8 +7741,8 @@
       <c r="J111" s="12"/>
       <c r="K111" s="14"/>
       <c r="L111" s="48"/>
-      <c r="M111" s="64"/>
-      <c r="N111" s="64"/>
+      <c r="M111" s="56"/>
+      <c r="N111" s="56"/>
       <c r="O111" s="1"/>
       <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
@@ -7797,8 +7801,8 @@
       <c r="L112" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="M112" s="64"/>
-      <c r="N112" s="64"/>
+      <c r="M112" s="56"/>
+      <c r="N112" s="56"/>
       <c r="O112" s="1"/>
       <c r="P112" s="13"/>
       <c r="Q112" s="13"/>
@@ -7849,8 +7853,8 @@
       <c r="J113" s="12"/>
       <c r="K113" s="14"/>
       <c r="L113" s="48"/>
-      <c r="M113" s="64"/>
-      <c r="N113" s="64"/>
+      <c r="M113" s="56"/>
+      <c r="N113" s="56"/>
       <c r="O113" s="1"/>
       <c r="P113" s="13"/>
       <c r="Q113" s="13"/>
@@ -7901,8 +7905,8 @@
       <c r="J114" s="12"/>
       <c r="K114" s="14"/>
       <c r="L114" s="48"/>
-      <c r="M114" s="64"/>
-      <c r="N114" s="64"/>
+      <c r="M114" s="56"/>
+      <c r="N114" s="56"/>
       <c r="O114" s="1"/>
       <c r="P114" s="13"/>
       <c r="Q114" s="13"/>
@@ -7953,8 +7957,8 @@
       <c r="J115" s="12"/>
       <c r="K115" s="14"/>
       <c r="L115" s="48"/>
-      <c r="M115" s="64"/>
-      <c r="N115" s="64"/>
+      <c r="M115" s="56"/>
+      <c r="N115" s="56"/>
       <c r="O115" s="1"/>
       <c r="P115" s="13"/>
       <c r="Q115" s="13"/>
@@ -8005,8 +8009,8 @@
       <c r="J116" s="12"/>
       <c r="K116" s="14"/>
       <c r="L116" s="48"/>
-      <c r="M116" s="64"/>
-      <c r="N116" s="64"/>
+      <c r="M116" s="56"/>
+      <c r="N116" s="56"/>
       <c r="O116" s="4"/>
       <c r="P116" s="13"/>
       <c r="Q116" s="13"/>
@@ -8057,8 +8061,8 @@
       <c r="J117" s="15"/>
       <c r="K117" s="17"/>
       <c r="L117" s="49"/>
-      <c r="M117" s="64"/>
-      <c r="N117" s="64"/>
+      <c r="M117" s="56"/>
+      <c r="N117" s="56"/>
       <c r="O117" s="4"/>
       <c r="P117" s="13"/>
       <c r="Q117" s="13"/>
@@ -8840,68 +8844,68 @@
       <c r="M136" s="51"/>
       <c r="N136" s="52"/>
       <c r="O136" s="6"/>
-      <c r="P136" s="89" t="s">
+      <c r="P136" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="Q136" s="89"/>
-      <c r="R136" s="87" t="s">
+      <c r="Q136" s="74"/>
+      <c r="R136" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="S136" s="87"/>
-      <c r="T136" s="87" t="s">
+      <c r="S136" s="73"/>
+      <c r="T136" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="U136" s="87"/>
-      <c r="V136" s="87" t="s">
+      <c r="U136" s="73"/>
+      <c r="V136" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="W136" s="87"/>
-      <c r="X136" s="87" t="s">
+      <c r="W136" s="73"/>
+      <c r="X136" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="Y136" s="87"/>
-      <c r="Z136" s="87"/>
-      <c r="AA136" s="87"/>
-      <c r="AB136" s="87" t="s">
+      <c r="Y136" s="73"/>
+      <c r="Z136" s="73"/>
+      <c r="AA136" s="73"/>
+      <c r="AB136" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="AC136" s="87"/>
-      <c r="AD136" s="87"/>
-      <c r="AE136" s="87"/>
-      <c r="AF136" s="87"/>
-      <c r="AG136" s="87" t="s">
+      <c r="AC136" s="73"/>
+      <c r="AD136" s="73"/>
+      <c r="AE136" s="73"/>
+      <c r="AF136" s="73"/>
+      <c r="AG136" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="AH136" s="87"/>
-      <c r="AI136" s="87"/>
-      <c r="AJ136" s="87"/>
-      <c r="AK136" s="87"/>
-      <c r="AL136" s="87"/>
-      <c r="AM136" s="87" t="s">
+      <c r="AH136" s="73"/>
+      <c r="AI136" s="73"/>
+      <c r="AJ136" s="73"/>
+      <c r="AK136" s="73"/>
+      <c r="AL136" s="73"/>
+      <c r="AM136" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="AN136" s="87"/>
-      <c r="AO136" s="87" t="s">
+      <c r="AN136" s="73"/>
+      <c r="AO136" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="AP136" s="87"/>
-      <c r="AQ136" s="87"/>
-      <c r="AR136" s="87"/>
-      <c r="AS136" s="87"/>
-      <c r="AT136" s="87"/>
-      <c r="AU136" s="87" t="s">
+      <c r="AP136" s="73"/>
+      <c r="AQ136" s="73"/>
+      <c r="AR136" s="73"/>
+      <c r="AS136" s="73"/>
+      <c r="AT136" s="73"/>
+      <c r="AU136" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="AV136" s="87"/>
-      <c r="AW136" s="87"/>
-      <c r="AX136" s="87"/>
-      <c r="AY136" s="87"/>
-      <c r="AZ136" s="87"/>
-      <c r="BA136" s="87" t="s">
+      <c r="AV136" s="73"/>
+      <c r="AW136" s="73"/>
+      <c r="AX136" s="73"/>
+      <c r="AY136" s="73"/>
+      <c r="AZ136" s="73"/>
+      <c r="BA136" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="BB136" s="87"/>
-      <c r="BC136" s="87"/>
+      <c r="BB136" s="73"/>
+      <c r="BC136" s="73"/>
     </row>
     <row r="137" spans="6:55" x14ac:dyDescent="0.25">
       <c r="F137" s="53"/>
@@ -8914,46 +8918,46 @@
       <c r="M137" s="54"/>
       <c r="N137" s="55"/>
       <c r="O137" s="6"/>
-      <c r="P137" s="89"/>
-      <c r="Q137" s="89"/>
-      <c r="R137" s="87"/>
-      <c r="S137" s="87"/>
-      <c r="T137" s="87"/>
-      <c r="U137" s="87"/>
-      <c r="V137" s="87"/>
-      <c r="W137" s="87"/>
-      <c r="X137" s="87"/>
-      <c r="Y137" s="87"/>
-      <c r="Z137" s="87"/>
-      <c r="AA137" s="87"/>
-      <c r="AB137" s="87"/>
-      <c r="AC137" s="87"/>
-      <c r="AD137" s="87"/>
-      <c r="AE137" s="87"/>
-      <c r="AF137" s="87"/>
-      <c r="AG137" s="87"/>
-      <c r="AH137" s="87"/>
-      <c r="AI137" s="87"/>
-      <c r="AJ137" s="87"/>
-      <c r="AK137" s="87"/>
-      <c r="AL137" s="87"/>
-      <c r="AM137" s="87"/>
-      <c r="AN137" s="87"/>
-      <c r="AO137" s="87"/>
-      <c r="AP137" s="87"/>
-      <c r="AQ137" s="87"/>
-      <c r="AR137" s="87"/>
-      <c r="AS137" s="87"/>
-      <c r="AT137" s="87"/>
-      <c r="AU137" s="87"/>
-      <c r="AV137" s="87"/>
-      <c r="AW137" s="87"/>
-      <c r="AX137" s="87"/>
-      <c r="AY137" s="87"/>
-      <c r="AZ137" s="87"/>
-      <c r="BA137" s="87"/>
-      <c r="BB137" s="87"/>
-      <c r="BC137" s="87"/>
+      <c r="P137" s="74"/>
+      <c r="Q137" s="74"/>
+      <c r="R137" s="73"/>
+      <c r="S137" s="73"/>
+      <c r="T137" s="73"/>
+      <c r="U137" s="73"/>
+      <c r="V137" s="73"/>
+      <c r="W137" s="73"/>
+      <c r="X137" s="73"/>
+      <c r="Y137" s="73"/>
+      <c r="Z137" s="73"/>
+      <c r="AA137" s="73"/>
+      <c r="AB137" s="73"/>
+      <c r="AC137" s="73"/>
+      <c r="AD137" s="73"/>
+      <c r="AE137" s="73"/>
+      <c r="AF137" s="73"/>
+      <c r="AG137" s="73"/>
+      <c r="AH137" s="73"/>
+      <c r="AI137" s="73"/>
+      <c r="AJ137" s="73"/>
+      <c r="AK137" s="73"/>
+      <c r="AL137" s="73"/>
+      <c r="AM137" s="73"/>
+      <c r="AN137" s="73"/>
+      <c r="AO137" s="73"/>
+      <c r="AP137" s="73"/>
+      <c r="AQ137" s="73"/>
+      <c r="AR137" s="73"/>
+      <c r="AS137" s="73"/>
+      <c r="AT137" s="73"/>
+      <c r="AU137" s="73"/>
+      <c r="AV137" s="73"/>
+      <c r="AW137" s="73"/>
+      <c r="AX137" s="73"/>
+      <c r="AY137" s="73"/>
+      <c r="AZ137" s="73"/>
+      <c r="BA137" s="73"/>
+      <c r="BB137" s="73"/>
+      <c r="BC137" s="73"/>
     </row>
     <row r="138" spans="6:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F138" s="9" t="s">
@@ -8974,26 +8978,26 @@
       <c r="M138" s="10"/>
       <c r="N138" s="11"/>
       <c r="O138" s="1"/>
-      <c r="P138" s="64" t="s">
+      <c r="P138" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="Q138" s="64"/>
+      <c r="Q138" s="56"/>
       <c r="R138" s="32" t="s">
         <v>101</v>
       </c>
       <c r="S138" s="34"/>
-      <c r="T138" s="64" t="s">
+      <c r="T138" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="U138" s="64"/>
+      <c r="U138" s="56"/>
       <c r="V138" s="9"/>
       <c r="W138" s="11"/>
-      <c r="X138" s="64" t="s">
+      <c r="X138" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="Y138" s="64"/>
-      <c r="Z138" s="64"/>
-      <c r="AA138" s="64"/>
+      <c r="Y138" s="56"/>
+      <c r="Z138" s="56"/>
+      <c r="AA138" s="56"/>
       <c r="AB138" s="9" t="s">
         <v>96</v>
       </c>
@@ -9007,8 +9011,8 @@
       <c r="AJ138" s="10"/>
       <c r="AK138" s="10"/>
       <c r="AL138" s="11"/>
-      <c r="AM138" s="64"/>
-      <c r="AN138" s="64"/>
+      <c r="AM138" s="56"/>
+      <c r="AN138" s="56"/>
       <c r="AO138" s="9" t="s">
         <v>97</v>
       </c>
@@ -9042,18 +9046,18 @@
       <c r="M139" s="13"/>
       <c r="N139" s="14"/>
       <c r="O139" s="1"/>
-      <c r="P139" s="64"/>
-      <c r="Q139" s="64"/>
-      <c r="R139" s="90"/>
-      <c r="S139" s="91"/>
-      <c r="T139" s="64"/>
-      <c r="U139" s="64"/>
+      <c r="P139" s="56"/>
+      <c r="Q139" s="56"/>
+      <c r="R139" s="75"/>
+      <c r="S139" s="76"/>
+      <c r="T139" s="56"/>
+      <c r="U139" s="56"/>
       <c r="V139" s="12"/>
       <c r="W139" s="14"/>
-      <c r="X139" s="64"/>
-      <c r="Y139" s="64"/>
-      <c r="Z139" s="64"/>
-      <c r="AA139" s="64"/>
+      <c r="X139" s="56"/>
+      <c r="Y139" s="56"/>
+      <c r="Z139" s="56"/>
+      <c r="AA139" s="56"/>
       <c r="AB139" s="12"/>
       <c r="AC139" s="13"/>
       <c r="AD139" s="13"/>
@@ -9065,8 +9069,8 @@
       <c r="AJ139" s="13"/>
       <c r="AK139" s="13"/>
       <c r="AL139" s="14"/>
-      <c r="AM139" s="64"/>
-      <c r="AN139" s="64"/>
+      <c r="AM139" s="56"/>
+      <c r="AN139" s="56"/>
       <c r="AO139" s="12"/>
       <c r="AP139" s="13"/>
       <c r="AQ139" s="13"/>
@@ -9094,18 +9098,18 @@
       <c r="M140" s="13"/>
       <c r="N140" s="14"/>
       <c r="O140" s="1"/>
-      <c r="P140" s="64"/>
-      <c r="Q140" s="64"/>
-      <c r="R140" s="90"/>
-      <c r="S140" s="91"/>
-      <c r="T140" s="64"/>
-      <c r="U140" s="64"/>
+      <c r="P140" s="56"/>
+      <c r="Q140" s="56"/>
+      <c r="R140" s="75"/>
+      <c r="S140" s="76"/>
+      <c r="T140" s="56"/>
+      <c r="U140" s="56"/>
       <c r="V140" s="12"/>
       <c r="W140" s="14"/>
-      <c r="X140" s="64"/>
-      <c r="Y140" s="64"/>
-      <c r="Z140" s="64"/>
-      <c r="AA140" s="64"/>
+      <c r="X140" s="56"/>
+      <c r="Y140" s="56"/>
+      <c r="Z140" s="56"/>
+      <c r="AA140" s="56"/>
       <c r="AB140" s="12"/>
       <c r="AC140" s="13"/>
       <c r="AD140" s="13"/>
@@ -9117,8 +9121,8 @@
       <c r="AJ140" s="13"/>
       <c r="AK140" s="13"/>
       <c r="AL140" s="14"/>
-      <c r="AM140" s="64"/>
-      <c r="AN140" s="64"/>
+      <c r="AM140" s="56"/>
+      <c r="AN140" s="56"/>
       <c r="AO140" s="12"/>
       <c r="AP140" s="13"/>
       <c r="AQ140" s="13"/>
@@ -9146,18 +9150,18 @@
       <c r="M141" s="16"/>
       <c r="N141" s="17"/>
       <c r="O141" s="1"/>
-      <c r="P141" s="64"/>
-      <c r="Q141" s="64"/>
-      <c r="R141" s="90"/>
-      <c r="S141" s="91"/>
-      <c r="T141" s="64"/>
-      <c r="U141" s="64"/>
+      <c r="P141" s="56"/>
+      <c r="Q141" s="56"/>
+      <c r="R141" s="75"/>
+      <c r="S141" s="76"/>
+      <c r="T141" s="56"/>
+      <c r="U141" s="56"/>
       <c r="V141" s="12"/>
       <c r="W141" s="14"/>
-      <c r="X141" s="64"/>
-      <c r="Y141" s="64"/>
-      <c r="Z141" s="64"/>
-      <c r="AA141" s="64"/>
+      <c r="X141" s="56"/>
+      <c r="Y141" s="56"/>
+      <c r="Z141" s="56"/>
+      <c r="AA141" s="56"/>
       <c r="AB141" s="12"/>
       <c r="AC141" s="13"/>
       <c r="AD141" s="13"/>
@@ -9169,8 +9173,8 @@
       <c r="AJ141" s="13"/>
       <c r="AK141" s="13"/>
       <c r="AL141" s="14"/>
-      <c r="AM141" s="64"/>
-      <c r="AN141" s="64"/>
+      <c r="AM141" s="56"/>
+      <c r="AN141" s="56"/>
       <c r="AO141" s="12"/>
       <c r="AP141" s="13"/>
       <c r="AQ141" s="13"/>
@@ -9206,18 +9210,18 @@
       <c r="M142" s="10"/>
       <c r="N142" s="11"/>
       <c r="O142" s="1"/>
-      <c r="P142" s="64"/>
-      <c r="Q142" s="64"/>
-      <c r="R142" s="90"/>
-      <c r="S142" s="91"/>
-      <c r="T142" s="64"/>
-      <c r="U142" s="64"/>
+      <c r="P142" s="56"/>
+      <c r="Q142" s="56"/>
+      <c r="R142" s="75"/>
+      <c r="S142" s="76"/>
+      <c r="T142" s="56"/>
+      <c r="U142" s="56"/>
       <c r="V142" s="12"/>
       <c r="W142" s="14"/>
-      <c r="X142" s="64"/>
-      <c r="Y142" s="64"/>
-      <c r="Z142" s="64"/>
-      <c r="AA142" s="64"/>
+      <c r="X142" s="56"/>
+      <c r="Y142" s="56"/>
+      <c r="Z142" s="56"/>
+      <c r="AA142" s="56"/>
       <c r="AB142" s="12"/>
       <c r="AC142" s="13"/>
       <c r="AD142" s="13"/>
@@ -9229,8 +9233,8 @@
       <c r="AJ142" s="13"/>
       <c r="AK142" s="13"/>
       <c r="AL142" s="14"/>
-      <c r="AM142" s="64"/>
-      <c r="AN142" s="64"/>
+      <c r="AM142" s="56"/>
+      <c r="AN142" s="56"/>
       <c r="AO142" s="12"/>
       <c r="AP142" s="13"/>
       <c r="AQ142" s="13"/>
@@ -9258,18 +9262,18 @@
       <c r="M143" s="13"/>
       <c r="N143" s="14"/>
       <c r="O143" s="1"/>
-      <c r="P143" s="64"/>
-      <c r="Q143" s="64"/>
-      <c r="R143" s="90"/>
-      <c r="S143" s="91"/>
-      <c r="T143" s="64"/>
-      <c r="U143" s="64"/>
+      <c r="P143" s="56"/>
+      <c r="Q143" s="56"/>
+      <c r="R143" s="75"/>
+      <c r="S143" s="76"/>
+      <c r="T143" s="56"/>
+      <c r="U143" s="56"/>
       <c r="V143" s="12"/>
       <c r="W143" s="14"/>
-      <c r="X143" s="64"/>
-      <c r="Y143" s="64"/>
-      <c r="Z143" s="64"/>
-      <c r="AA143" s="64"/>
+      <c r="X143" s="56"/>
+      <c r="Y143" s="56"/>
+      <c r="Z143" s="56"/>
+      <c r="AA143" s="56"/>
       <c r="AB143" s="12"/>
       <c r="AC143" s="13"/>
       <c r="AD143" s="13"/>
@@ -9281,8 +9285,8 @@
       <c r="AJ143" s="13"/>
       <c r="AK143" s="13"/>
       <c r="AL143" s="14"/>
-      <c r="AM143" s="64"/>
-      <c r="AN143" s="64"/>
+      <c r="AM143" s="56"/>
+      <c r="AN143" s="56"/>
       <c r="AO143" s="12"/>
       <c r="AP143" s="13"/>
       <c r="AQ143" s="13"/>
@@ -9310,18 +9314,18 @@
       <c r="M144" s="13"/>
       <c r="N144" s="14"/>
       <c r="O144" s="1"/>
-      <c r="P144" s="64"/>
-      <c r="Q144" s="64"/>
-      <c r="R144" s="90"/>
-      <c r="S144" s="91"/>
-      <c r="T144" s="64"/>
-      <c r="U144" s="64"/>
+      <c r="P144" s="56"/>
+      <c r="Q144" s="56"/>
+      <c r="R144" s="75"/>
+      <c r="S144" s="76"/>
+      <c r="T144" s="56"/>
+      <c r="U144" s="56"/>
       <c r="V144" s="12"/>
       <c r="W144" s="14"/>
-      <c r="X144" s="64"/>
-      <c r="Y144" s="64"/>
-      <c r="Z144" s="64"/>
-      <c r="AA144" s="64"/>
+      <c r="X144" s="56"/>
+      <c r="Y144" s="56"/>
+      <c r="Z144" s="56"/>
+      <c r="AA144" s="56"/>
       <c r="AB144" s="12"/>
       <c r="AC144" s="13"/>
       <c r="AD144" s="13"/>
@@ -9333,8 +9337,8 @@
       <c r="AJ144" s="13"/>
       <c r="AK144" s="13"/>
       <c r="AL144" s="14"/>
-      <c r="AM144" s="64"/>
-      <c r="AN144" s="64"/>
+      <c r="AM144" s="56"/>
+      <c r="AN144" s="56"/>
       <c r="AO144" s="12"/>
       <c r="AP144" s="13"/>
       <c r="AQ144" s="13"/>
@@ -9362,18 +9366,18 @@
       <c r="M145" s="16"/>
       <c r="N145" s="17"/>
       <c r="O145" s="1"/>
-      <c r="P145" s="64"/>
-      <c r="Q145" s="64"/>
-      <c r="R145" s="90"/>
-      <c r="S145" s="91"/>
-      <c r="T145" s="64"/>
-      <c r="U145" s="64"/>
+      <c r="P145" s="56"/>
+      <c r="Q145" s="56"/>
+      <c r="R145" s="75"/>
+      <c r="S145" s="76"/>
+      <c r="T145" s="56"/>
+      <c r="U145" s="56"/>
       <c r="V145" s="12"/>
       <c r="W145" s="14"/>
-      <c r="X145" s="64"/>
-      <c r="Y145" s="64"/>
-      <c r="Z145" s="64"/>
-      <c r="AA145" s="64"/>
+      <c r="X145" s="56"/>
+      <c r="Y145" s="56"/>
+      <c r="Z145" s="56"/>
+      <c r="AA145" s="56"/>
       <c r="AB145" s="12"/>
       <c r="AC145" s="13"/>
       <c r="AD145" s="13"/>
@@ -9385,8 +9389,8 @@
       <c r="AJ145" s="13"/>
       <c r="AK145" s="13"/>
       <c r="AL145" s="14"/>
-      <c r="AM145" s="64"/>
-      <c r="AN145" s="64"/>
+      <c r="AM145" s="56"/>
+      <c r="AN145" s="56"/>
       <c r="AO145" s="12"/>
       <c r="AP145" s="13"/>
       <c r="AQ145" s="13"/>
@@ -9415,25 +9419,25 @@
       <c r="J146" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K146" s="64" t="s">
+      <c r="K146" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="L146" s="64"/>
-      <c r="M146" s="64"/>
-      <c r="N146" s="64"/>
+      <c r="L146" s="56"/>
+      <c r="M146" s="56"/>
+      <c r="N146" s="56"/>
       <c r="O146" s="1"/>
-      <c r="P146" s="64"/>
-      <c r="Q146" s="64"/>
-      <c r="R146" s="90"/>
-      <c r="S146" s="91"/>
-      <c r="T146" s="64"/>
-      <c r="U146" s="64"/>
+      <c r="P146" s="56"/>
+      <c r="Q146" s="56"/>
+      <c r="R146" s="75"/>
+      <c r="S146" s="76"/>
+      <c r="T146" s="56"/>
+      <c r="U146" s="56"/>
       <c r="V146" s="12"/>
       <c r="W146" s="14"/>
-      <c r="X146" s="64"/>
-      <c r="Y146" s="64"/>
-      <c r="Z146" s="64"/>
-      <c r="AA146" s="64"/>
+      <c r="X146" s="56"/>
+      <c r="Y146" s="56"/>
+      <c r="Z146" s="56"/>
+      <c r="AA146" s="56"/>
       <c r="AB146" s="12"/>
       <c r="AC146" s="13"/>
       <c r="AD146" s="13"/>
@@ -9445,8 +9449,8 @@
       <c r="AJ146" s="13"/>
       <c r="AK146" s="13"/>
       <c r="AL146" s="14"/>
-      <c r="AM146" s="64"/>
-      <c r="AN146" s="64"/>
+      <c r="AM146" s="56"/>
+      <c r="AN146" s="56"/>
       <c r="AO146" s="12"/>
       <c r="AP146" s="13"/>
       <c r="AQ146" s="13"/>
@@ -9469,23 +9473,23 @@
       <c r="H147" s="12"/>
       <c r="I147" s="14"/>
       <c r="J147" s="48"/>
-      <c r="K147" s="64"/>
-      <c r="L147" s="64"/>
-      <c r="M147" s="64"/>
-      <c r="N147" s="64"/>
+      <c r="K147" s="56"/>
+      <c r="L147" s="56"/>
+      <c r="M147" s="56"/>
+      <c r="N147" s="56"/>
       <c r="O147" s="1"/>
-      <c r="P147" s="64"/>
-      <c r="Q147" s="64"/>
-      <c r="R147" s="90"/>
-      <c r="S147" s="91"/>
-      <c r="T147" s="64"/>
-      <c r="U147" s="64"/>
+      <c r="P147" s="56"/>
+      <c r="Q147" s="56"/>
+      <c r="R147" s="75"/>
+      <c r="S147" s="76"/>
+      <c r="T147" s="56"/>
+      <c r="U147" s="56"/>
       <c r="V147" s="12"/>
       <c r="W147" s="14"/>
-      <c r="X147" s="64"/>
-      <c r="Y147" s="64"/>
-      <c r="Z147" s="64"/>
-      <c r="AA147" s="64"/>
+      <c r="X147" s="56"/>
+      <c r="Y147" s="56"/>
+      <c r="Z147" s="56"/>
+      <c r="AA147" s="56"/>
       <c r="AB147" s="12"/>
       <c r="AC147" s="13"/>
       <c r="AD147" s="13"/>
@@ -9497,8 +9501,8 @@
       <c r="AJ147" s="13"/>
       <c r="AK147" s="13"/>
       <c r="AL147" s="14"/>
-      <c r="AM147" s="64"/>
-      <c r="AN147" s="64"/>
+      <c r="AM147" s="56"/>
+      <c r="AN147" s="56"/>
       <c r="AO147" s="12"/>
       <c r="AP147" s="13"/>
       <c r="AQ147" s="13"/>
@@ -9521,23 +9525,23 @@
       <c r="H148" s="12"/>
       <c r="I148" s="14"/>
       <c r="J148" s="48"/>
-      <c r="K148" s="64"/>
-      <c r="L148" s="64"/>
-      <c r="M148" s="64"/>
-      <c r="N148" s="64"/>
+      <c r="K148" s="56"/>
+      <c r="L148" s="56"/>
+      <c r="M148" s="56"/>
+      <c r="N148" s="56"/>
       <c r="O148" s="1"/>
-      <c r="P148" s="64"/>
-      <c r="Q148" s="64"/>
-      <c r="R148" s="90"/>
-      <c r="S148" s="91"/>
-      <c r="T148" s="64"/>
-      <c r="U148" s="64"/>
+      <c r="P148" s="56"/>
+      <c r="Q148" s="56"/>
+      <c r="R148" s="75"/>
+      <c r="S148" s="76"/>
+      <c r="T148" s="56"/>
+      <c r="U148" s="56"/>
       <c r="V148" s="12"/>
       <c r="W148" s="14"/>
-      <c r="X148" s="64"/>
-      <c r="Y148" s="64"/>
-      <c r="Z148" s="64"/>
-      <c r="AA148" s="64"/>
+      <c r="X148" s="56"/>
+      <c r="Y148" s="56"/>
+      <c r="Z148" s="56"/>
+      <c r="AA148" s="56"/>
       <c r="AB148" s="12"/>
       <c r="AC148" s="13"/>
       <c r="AD148" s="13"/>
@@ -9549,8 +9553,8 @@
       <c r="AJ148" s="13"/>
       <c r="AK148" s="13"/>
       <c r="AL148" s="14"/>
-      <c r="AM148" s="64"/>
-      <c r="AN148" s="64"/>
+      <c r="AM148" s="56"/>
+      <c r="AN148" s="56"/>
       <c r="AO148" s="12"/>
       <c r="AP148" s="13"/>
       <c r="AQ148" s="13"/>
@@ -9573,23 +9577,23 @@
       <c r="H149" s="15"/>
       <c r="I149" s="17"/>
       <c r="J149" s="49"/>
-      <c r="K149" s="64"/>
-      <c r="L149" s="64"/>
-      <c r="M149" s="64"/>
-      <c r="N149" s="64"/>
+      <c r="K149" s="56"/>
+      <c r="L149" s="56"/>
+      <c r="M149" s="56"/>
+      <c r="N149" s="56"/>
       <c r="O149" s="1"/>
-      <c r="P149" s="64"/>
-      <c r="Q149" s="64"/>
-      <c r="R149" s="90"/>
-      <c r="S149" s="91"/>
-      <c r="T149" s="64"/>
-      <c r="U149" s="64"/>
+      <c r="P149" s="56"/>
+      <c r="Q149" s="56"/>
+      <c r="R149" s="75"/>
+      <c r="S149" s="76"/>
+      <c r="T149" s="56"/>
+      <c r="U149" s="56"/>
       <c r="V149" s="12"/>
       <c r="W149" s="14"/>
-      <c r="X149" s="64"/>
-      <c r="Y149" s="64"/>
-      <c r="Z149" s="64"/>
-      <c r="AA149" s="64"/>
+      <c r="X149" s="56"/>
+      <c r="Y149" s="56"/>
+      <c r="Z149" s="56"/>
+      <c r="AA149" s="56"/>
       <c r="AB149" s="12"/>
       <c r="AC149" s="13"/>
       <c r="AD149" s="13"/>
@@ -9601,8 +9605,8 @@
       <c r="AJ149" s="13"/>
       <c r="AK149" s="13"/>
       <c r="AL149" s="14"/>
-      <c r="AM149" s="64"/>
-      <c r="AN149" s="64"/>
+      <c r="AM149" s="56"/>
+      <c r="AN149" s="56"/>
       <c r="AO149" s="12"/>
       <c r="AP149" s="13"/>
       <c r="AQ149" s="13"/>
@@ -9620,18 +9624,18 @@
       <c r="BC149" s="14"/>
     </row>
     <row r="150" spans="6:55" x14ac:dyDescent="0.25">
-      <c r="P150" s="64"/>
-      <c r="Q150" s="64"/>
+      <c r="P150" s="56"/>
+      <c r="Q150" s="56"/>
       <c r="R150" s="35"/>
       <c r="S150" s="37"/>
-      <c r="T150" s="64"/>
-      <c r="U150" s="64"/>
+      <c r="T150" s="56"/>
+      <c r="U150" s="56"/>
       <c r="V150" s="15"/>
       <c r="W150" s="17"/>
-      <c r="X150" s="64"/>
-      <c r="Y150" s="64"/>
-      <c r="Z150" s="64"/>
-      <c r="AA150" s="64"/>
+      <c r="X150" s="56"/>
+      <c r="Y150" s="56"/>
+      <c r="Z150" s="56"/>
+      <c r="AA150" s="56"/>
       <c r="AB150" s="15"/>
       <c r="AC150" s="16"/>
       <c r="AD150" s="16"/>
@@ -9643,8 +9647,8 @@
       <c r="AJ150" s="16"/>
       <c r="AK150" s="16"/>
       <c r="AL150" s="17"/>
-      <c r="AM150" s="64"/>
-      <c r="AN150" s="64"/>
+      <c r="AM150" s="56"/>
+      <c r="AN150" s="56"/>
       <c r="AO150" s="15"/>
       <c r="AP150" s="16"/>
       <c r="AQ150" s="16"/>
@@ -9699,14 +9703,14 @@
         <v>106</v>
       </c>
       <c r="AN151" s="11"/>
-      <c r="AO151" s="64" t="s">
+      <c r="AO151" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AP151" s="64"/>
-      <c r="AQ151" s="64"/>
-      <c r="AR151" s="64"/>
-      <c r="AS151" s="64"/>
-      <c r="AT151" s="64"/>
+      <c r="AP151" s="56"/>
+      <c r="AQ151" s="56"/>
+      <c r="AR151" s="56"/>
+      <c r="AS151" s="56"/>
+      <c r="AT151" s="56"/>
       <c r="AU151" s="9"/>
       <c r="AV151" s="10"/>
       <c r="AW151" s="10"/>
@@ -9722,8 +9726,8 @@
     <row r="152" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P152" s="12"/>
       <c r="Q152" s="14"/>
-      <c r="R152" s="90"/>
-      <c r="S152" s="91"/>
+      <c r="R152" s="75"/>
+      <c r="S152" s="76"/>
       <c r="T152" s="12"/>
       <c r="U152" s="14"/>
       <c r="V152" s="12"/>
@@ -9745,12 +9749,12 @@
       <c r="AL152" s="14"/>
       <c r="AM152" s="12"/>
       <c r="AN152" s="14"/>
-      <c r="AO152" s="64"/>
-      <c r="AP152" s="64"/>
-      <c r="AQ152" s="64"/>
-      <c r="AR152" s="64"/>
-      <c r="AS152" s="64"/>
-      <c r="AT152" s="64"/>
+      <c r="AO152" s="56"/>
+      <c r="AP152" s="56"/>
+      <c r="AQ152" s="56"/>
+      <c r="AR152" s="56"/>
+      <c r="AS152" s="56"/>
+      <c r="AT152" s="56"/>
       <c r="AU152" s="12"/>
       <c r="AV152" s="13"/>
       <c r="AW152" s="13"/>
@@ -9764,8 +9768,8 @@
     <row r="153" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P153" s="12"/>
       <c r="Q153" s="14"/>
-      <c r="R153" s="90"/>
-      <c r="S153" s="91"/>
+      <c r="R153" s="75"/>
+      <c r="S153" s="76"/>
       <c r="T153" s="12"/>
       <c r="U153" s="14"/>
       <c r="V153" s="12"/>
@@ -9787,12 +9791,12 @@
       <c r="AL153" s="14"/>
       <c r="AM153" s="12"/>
       <c r="AN153" s="14"/>
-      <c r="AO153" s="64"/>
-      <c r="AP153" s="64"/>
-      <c r="AQ153" s="64"/>
-      <c r="AR153" s="64"/>
-      <c r="AS153" s="64"/>
-      <c r="AT153" s="64"/>
+      <c r="AO153" s="56"/>
+      <c r="AP153" s="56"/>
+      <c r="AQ153" s="56"/>
+      <c r="AR153" s="56"/>
+      <c r="AS153" s="56"/>
+      <c r="AT153" s="56"/>
       <c r="AU153" s="12"/>
       <c r="AV153" s="13"/>
       <c r="AW153" s="13"/>
@@ -9806,8 +9810,8 @@
     <row r="154" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P154" s="12"/>
       <c r="Q154" s="14"/>
-      <c r="R154" s="90"/>
-      <c r="S154" s="91"/>
+      <c r="R154" s="75"/>
+      <c r="S154" s="76"/>
       <c r="T154" s="12"/>
       <c r="U154" s="14"/>
       <c r="V154" s="12"/>
@@ -9829,12 +9833,12 @@
       <c r="AL154" s="14"/>
       <c r="AM154" s="12"/>
       <c r="AN154" s="14"/>
-      <c r="AO154" s="64"/>
-      <c r="AP154" s="64"/>
-      <c r="AQ154" s="64"/>
-      <c r="AR154" s="64"/>
-      <c r="AS154" s="64"/>
-      <c r="AT154" s="64"/>
+      <c r="AO154" s="56"/>
+      <c r="AP154" s="56"/>
+      <c r="AQ154" s="56"/>
+      <c r="AR154" s="56"/>
+      <c r="AS154" s="56"/>
+      <c r="AT154" s="56"/>
       <c r="AU154" s="12"/>
       <c r="AV154" s="13"/>
       <c r="AW154" s="13"/>
@@ -9848,8 +9852,8 @@
     <row r="155" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P155" s="12"/>
       <c r="Q155" s="14"/>
-      <c r="R155" s="90"/>
-      <c r="S155" s="91"/>
+      <c r="R155" s="75"/>
+      <c r="S155" s="76"/>
       <c r="T155" s="12"/>
       <c r="U155" s="14"/>
       <c r="V155" s="12"/>
@@ -9871,12 +9875,12 @@
       <c r="AL155" s="14"/>
       <c r="AM155" s="12"/>
       <c r="AN155" s="14"/>
-      <c r="AO155" s="64"/>
-      <c r="AP155" s="64"/>
-      <c r="AQ155" s="64"/>
-      <c r="AR155" s="64"/>
-      <c r="AS155" s="64"/>
-      <c r="AT155" s="64"/>
+      <c r="AO155" s="56"/>
+      <c r="AP155" s="56"/>
+      <c r="AQ155" s="56"/>
+      <c r="AR155" s="56"/>
+      <c r="AS155" s="56"/>
+      <c r="AT155" s="56"/>
       <c r="AU155" s="12"/>
       <c r="AV155" s="13"/>
       <c r="AW155" s="13"/>
@@ -9890,8 +9894,8 @@
     <row r="156" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P156" s="12"/>
       <c r="Q156" s="14"/>
-      <c r="R156" s="90"/>
-      <c r="S156" s="91"/>
+      <c r="R156" s="75"/>
+      <c r="S156" s="76"/>
       <c r="T156" s="12"/>
       <c r="U156" s="14"/>
       <c r="V156" s="12"/>
@@ -9913,12 +9917,12 @@
       <c r="AL156" s="14"/>
       <c r="AM156" s="12"/>
       <c r="AN156" s="14"/>
-      <c r="AO156" s="64"/>
-      <c r="AP156" s="64"/>
-      <c r="AQ156" s="64"/>
-      <c r="AR156" s="64"/>
-      <c r="AS156" s="64"/>
-      <c r="AT156" s="64"/>
+      <c r="AO156" s="56"/>
+      <c r="AP156" s="56"/>
+      <c r="AQ156" s="56"/>
+      <c r="AR156" s="56"/>
+      <c r="AS156" s="56"/>
+      <c r="AT156" s="56"/>
       <c r="AU156" s="12"/>
       <c r="AV156" s="13"/>
       <c r="AW156" s="13"/>
@@ -9932,8 +9936,8 @@
     <row r="157" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P157" s="12"/>
       <c r="Q157" s="14"/>
-      <c r="R157" s="90"/>
-      <c r="S157" s="91"/>
+      <c r="R157" s="75"/>
+      <c r="S157" s="76"/>
       <c r="T157" s="12"/>
       <c r="U157" s="14"/>
       <c r="V157" s="12"/>
@@ -9955,12 +9959,12 @@
       <c r="AL157" s="14"/>
       <c r="AM157" s="12"/>
       <c r="AN157" s="14"/>
-      <c r="AO157" s="64"/>
-      <c r="AP157" s="64"/>
-      <c r="AQ157" s="64"/>
-      <c r="AR157" s="64"/>
-      <c r="AS157" s="64"/>
-      <c r="AT157" s="64"/>
+      <c r="AO157" s="56"/>
+      <c r="AP157" s="56"/>
+      <c r="AQ157" s="56"/>
+      <c r="AR157" s="56"/>
+      <c r="AS157" s="56"/>
+      <c r="AT157" s="56"/>
       <c r="AU157" s="12"/>
       <c r="AV157" s="13"/>
       <c r="AW157" s="13"/>
@@ -9974,8 +9978,8 @@
     <row r="158" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P158" s="12"/>
       <c r="Q158" s="14"/>
-      <c r="R158" s="90"/>
-      <c r="S158" s="91"/>
+      <c r="R158" s="75"/>
+      <c r="S158" s="76"/>
       <c r="T158" s="12"/>
       <c r="U158" s="14"/>
       <c r="V158" s="12"/>
@@ -9997,12 +10001,12 @@
       <c r="AL158" s="14"/>
       <c r="AM158" s="12"/>
       <c r="AN158" s="14"/>
-      <c r="AO158" s="64"/>
-      <c r="AP158" s="64"/>
-      <c r="AQ158" s="64"/>
-      <c r="AR158" s="64"/>
-      <c r="AS158" s="64"/>
-      <c r="AT158" s="64"/>
+      <c r="AO158" s="56"/>
+      <c r="AP158" s="56"/>
+      <c r="AQ158" s="56"/>
+      <c r="AR158" s="56"/>
+      <c r="AS158" s="56"/>
+      <c r="AT158" s="56"/>
       <c r="AU158" s="12"/>
       <c r="AV158" s="13"/>
       <c r="AW158" s="13"/>
@@ -10016,8 +10020,8 @@
     <row r="159" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P159" s="12"/>
       <c r="Q159" s="14"/>
-      <c r="R159" s="90"/>
-      <c r="S159" s="91"/>
+      <c r="R159" s="75"/>
+      <c r="S159" s="76"/>
       <c r="T159" s="12"/>
       <c r="U159" s="14"/>
       <c r="V159" s="12"/>
@@ -10039,12 +10043,12 @@
       <c r="AL159" s="14"/>
       <c r="AM159" s="12"/>
       <c r="AN159" s="14"/>
-      <c r="AO159" s="64"/>
-      <c r="AP159" s="64"/>
-      <c r="AQ159" s="64"/>
-      <c r="AR159" s="64"/>
-      <c r="AS159" s="64"/>
-      <c r="AT159" s="64"/>
+      <c r="AO159" s="56"/>
+      <c r="AP159" s="56"/>
+      <c r="AQ159" s="56"/>
+      <c r="AR159" s="56"/>
+      <c r="AS159" s="56"/>
+      <c r="AT159" s="56"/>
       <c r="AU159" s="12"/>
       <c r="AV159" s="13"/>
       <c r="AW159" s="13"/>
@@ -10058,8 +10062,8 @@
     <row r="160" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P160" s="12"/>
       <c r="Q160" s="14"/>
-      <c r="R160" s="90"/>
-      <c r="S160" s="91"/>
+      <c r="R160" s="75"/>
+      <c r="S160" s="76"/>
       <c r="T160" s="12"/>
       <c r="U160" s="14"/>
       <c r="V160" s="12"/>
@@ -10081,12 +10085,12 @@
       <c r="AL160" s="14"/>
       <c r="AM160" s="12"/>
       <c r="AN160" s="14"/>
-      <c r="AO160" s="64"/>
-      <c r="AP160" s="64"/>
-      <c r="AQ160" s="64"/>
-      <c r="AR160" s="64"/>
-      <c r="AS160" s="64"/>
-      <c r="AT160" s="64"/>
+      <c r="AO160" s="56"/>
+      <c r="AP160" s="56"/>
+      <c r="AQ160" s="56"/>
+      <c r="AR160" s="56"/>
+      <c r="AS160" s="56"/>
+      <c r="AT160" s="56"/>
       <c r="AU160" s="12"/>
       <c r="AV160" s="13"/>
       <c r="AW160" s="13"/>
@@ -10100,8 +10104,8 @@
     <row r="161" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P161" s="12"/>
       <c r="Q161" s="14"/>
-      <c r="R161" s="90"/>
-      <c r="S161" s="91"/>
+      <c r="R161" s="75"/>
+      <c r="S161" s="76"/>
       <c r="T161" s="12"/>
       <c r="U161" s="14"/>
       <c r="V161" s="12"/>
@@ -10123,12 +10127,12 @@
       <c r="AL161" s="14"/>
       <c r="AM161" s="12"/>
       <c r="AN161" s="14"/>
-      <c r="AO161" s="64"/>
-      <c r="AP161" s="64"/>
-      <c r="AQ161" s="64"/>
-      <c r="AR161" s="64"/>
-      <c r="AS161" s="64"/>
-      <c r="AT161" s="64"/>
+      <c r="AO161" s="56"/>
+      <c r="AP161" s="56"/>
+      <c r="AQ161" s="56"/>
+      <c r="AR161" s="56"/>
+      <c r="AS161" s="56"/>
+      <c r="AT161" s="56"/>
       <c r="AU161" s="12"/>
       <c r="AV161" s="13"/>
       <c r="AW161" s="13"/>
@@ -10142,8 +10146,8 @@
     <row r="162" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P162" s="12"/>
       <c r="Q162" s="14"/>
-      <c r="R162" s="90"/>
-      <c r="S162" s="91"/>
+      <c r="R162" s="75"/>
+      <c r="S162" s="76"/>
       <c r="T162" s="12"/>
       <c r="U162" s="14"/>
       <c r="V162" s="12"/>
@@ -10165,12 +10169,12 @@
       <c r="AL162" s="14"/>
       <c r="AM162" s="12"/>
       <c r="AN162" s="14"/>
-      <c r="AO162" s="64"/>
-      <c r="AP162" s="64"/>
-      <c r="AQ162" s="64"/>
-      <c r="AR162" s="64"/>
-      <c r="AS162" s="64"/>
-      <c r="AT162" s="64"/>
+      <c r="AO162" s="56"/>
+      <c r="AP162" s="56"/>
+      <c r="AQ162" s="56"/>
+      <c r="AR162" s="56"/>
+      <c r="AS162" s="56"/>
+      <c r="AT162" s="56"/>
       <c r="AU162" s="12"/>
       <c r="AV162" s="13"/>
       <c r="AW162" s="13"/>
@@ -10184,8 +10188,8 @@
     <row r="163" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P163" s="12"/>
       <c r="Q163" s="14"/>
-      <c r="R163" s="90"/>
-      <c r="S163" s="91"/>
+      <c r="R163" s="75"/>
+      <c r="S163" s="76"/>
       <c r="T163" s="12"/>
       <c r="U163" s="14"/>
       <c r="V163" s="12"/>
@@ -10207,12 +10211,12 @@
       <c r="AL163" s="14"/>
       <c r="AM163" s="12"/>
       <c r="AN163" s="14"/>
-      <c r="AO163" s="64"/>
-      <c r="AP163" s="64"/>
-      <c r="AQ163" s="64"/>
-      <c r="AR163" s="64"/>
-      <c r="AS163" s="64"/>
-      <c r="AT163" s="64"/>
+      <c r="AO163" s="56"/>
+      <c r="AP163" s="56"/>
+      <c r="AQ163" s="56"/>
+      <c r="AR163" s="56"/>
+      <c r="AS163" s="56"/>
+      <c r="AT163" s="56"/>
       <c r="AU163" s="12"/>
       <c r="AV163" s="13"/>
       <c r="AW163" s="13"/>
@@ -10226,8 +10230,8 @@
     <row r="164" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P164" s="12"/>
       <c r="Q164" s="14"/>
-      <c r="R164" s="90"/>
-      <c r="S164" s="91"/>
+      <c r="R164" s="75"/>
+      <c r="S164" s="76"/>
       <c r="T164" s="12"/>
       <c r="U164" s="14"/>
       <c r="V164" s="12"/>
@@ -10249,12 +10253,12 @@
       <c r="AL164" s="14"/>
       <c r="AM164" s="12"/>
       <c r="AN164" s="14"/>
-      <c r="AO164" s="64"/>
-      <c r="AP164" s="64"/>
-      <c r="AQ164" s="64"/>
-      <c r="AR164" s="64"/>
-      <c r="AS164" s="64"/>
-      <c r="AT164" s="64"/>
+      <c r="AO164" s="56"/>
+      <c r="AP164" s="56"/>
+      <c r="AQ164" s="56"/>
+      <c r="AR164" s="56"/>
+      <c r="AS164" s="56"/>
+      <c r="AT164" s="56"/>
       <c r="AU164" s="12"/>
       <c r="AV164" s="13"/>
       <c r="AW164" s="13"/>
@@ -10268,8 +10272,8 @@
     <row r="165" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P165" s="12"/>
       <c r="Q165" s="14"/>
-      <c r="R165" s="90"/>
-      <c r="S165" s="91"/>
+      <c r="R165" s="75"/>
+      <c r="S165" s="76"/>
       <c r="T165" s="12"/>
       <c r="U165" s="14"/>
       <c r="V165" s="12"/>
@@ -10291,12 +10295,12 @@
       <c r="AL165" s="14"/>
       <c r="AM165" s="12"/>
       <c r="AN165" s="14"/>
-      <c r="AO165" s="64"/>
-      <c r="AP165" s="64"/>
-      <c r="AQ165" s="64"/>
-      <c r="AR165" s="64"/>
-      <c r="AS165" s="64"/>
-      <c r="AT165" s="64"/>
+      <c r="AO165" s="56"/>
+      <c r="AP165" s="56"/>
+      <c r="AQ165" s="56"/>
+      <c r="AR165" s="56"/>
+      <c r="AS165" s="56"/>
+      <c r="AT165" s="56"/>
       <c r="AU165" s="12"/>
       <c r="AV165" s="13"/>
       <c r="AW165" s="13"/>
@@ -10310,8 +10314,8 @@
     <row r="166" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P166" s="12"/>
       <c r="Q166" s="14"/>
-      <c r="R166" s="90"/>
-      <c r="S166" s="91"/>
+      <c r="R166" s="75"/>
+      <c r="S166" s="76"/>
       <c r="T166" s="12"/>
       <c r="U166" s="14"/>
       <c r="V166" s="12"/>
@@ -10333,12 +10337,12 @@
       <c r="AL166" s="14"/>
       <c r="AM166" s="12"/>
       <c r="AN166" s="14"/>
-      <c r="AO166" s="64"/>
-      <c r="AP166" s="64"/>
-      <c r="AQ166" s="64"/>
-      <c r="AR166" s="64"/>
-      <c r="AS166" s="64"/>
-      <c r="AT166" s="64"/>
+      <c r="AO166" s="56"/>
+      <c r="AP166" s="56"/>
+      <c r="AQ166" s="56"/>
+      <c r="AR166" s="56"/>
+      <c r="AS166" s="56"/>
+      <c r="AT166" s="56"/>
       <c r="AU166" s="12"/>
       <c r="AV166" s="13"/>
       <c r="AW166" s="13"/>
@@ -10352,8 +10356,8 @@
     <row r="167" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P167" s="12"/>
       <c r="Q167" s="14"/>
-      <c r="R167" s="90"/>
-      <c r="S167" s="91"/>
+      <c r="R167" s="75"/>
+      <c r="S167" s="76"/>
       <c r="T167" s="15"/>
       <c r="U167" s="17"/>
       <c r="V167" s="15"/>
@@ -10375,12 +10379,12 @@
       <c r="AL167" s="17"/>
       <c r="AM167" s="15"/>
       <c r="AN167" s="17"/>
-      <c r="AO167" s="64"/>
-      <c r="AP167" s="64"/>
-      <c r="AQ167" s="64"/>
-      <c r="AR167" s="64"/>
-      <c r="AS167" s="64"/>
-      <c r="AT167" s="64"/>
+      <c r="AO167" s="56"/>
+      <c r="AP167" s="56"/>
+      <c r="AQ167" s="56"/>
+      <c r="AR167" s="56"/>
+      <c r="AS167" s="56"/>
+      <c r="AT167" s="56"/>
       <c r="AU167" s="15"/>
       <c r="AV167" s="16"/>
       <c r="AW167" s="16"/>
@@ -10477,8 +10481,6 @@
     </row>
   </sheetData>
   <mergeCells count="277">
-    <mergeCell ref="L102:L105"/>
-    <mergeCell ref="M102:N105"/>
     <mergeCell ref="F104:G105"/>
     <mergeCell ref="AG138:AL150"/>
     <mergeCell ref="AM138:AN150"/>
@@ -10499,6 +10501,8 @@
     <mergeCell ref="K138:N141"/>
     <mergeCell ref="K142:N145"/>
     <mergeCell ref="K146:N149"/>
+    <mergeCell ref="J138:J141"/>
+    <mergeCell ref="J142:J145"/>
     <mergeCell ref="F2:F13"/>
     <mergeCell ref="G2:G13"/>
     <mergeCell ref="H2:H13"/>
@@ -10518,6 +10522,11 @@
     <mergeCell ref="M24:N41"/>
     <mergeCell ref="F56:N57"/>
     <mergeCell ref="F20:I21"/>
+    <mergeCell ref="J20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="F16:N17"/>
+    <mergeCell ref="F18:N19"/>
+    <mergeCell ref="M20:N23"/>
     <mergeCell ref="AU151:AZ167"/>
     <mergeCell ref="BA151:BC167"/>
     <mergeCell ref="AO151:AT167"/>
@@ -10591,11 +10600,6 @@
     <mergeCell ref="AU68:AZ77"/>
     <mergeCell ref="AU88:AZ97"/>
     <mergeCell ref="AO100:AT101"/>
-    <mergeCell ref="J20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="F16:N17"/>
-    <mergeCell ref="F18:N19"/>
-    <mergeCell ref="M20:N23"/>
     <mergeCell ref="F24:G32"/>
     <mergeCell ref="F33:G41"/>
     <mergeCell ref="H24:I32"/>
@@ -10606,8 +10610,6 @@
     <mergeCell ref="J33:K41"/>
     <mergeCell ref="L24:L32"/>
     <mergeCell ref="L33:L41"/>
-    <mergeCell ref="J138:J141"/>
-    <mergeCell ref="J142:J145"/>
     <mergeCell ref="J146:J149"/>
     <mergeCell ref="H136:I137"/>
     <mergeCell ref="J136:J137"/>
@@ -10630,6 +10632,8 @@
     <mergeCell ref="R100:S101"/>
     <mergeCell ref="F102:I103"/>
     <mergeCell ref="J102:K105"/>
+    <mergeCell ref="L102:L105"/>
+    <mergeCell ref="M102:N105"/>
     <mergeCell ref="T88:U97"/>
     <mergeCell ref="V88:W97"/>
     <mergeCell ref="X88:AA97"/>

</xml_diff>

<commit_message>
Revert "Add Nombre Cientifico plaga"
This reverts commit 5f015fb9b6d2900e64e9200785193700794cb825.
</commit_message>
<xml_diff>
--- a/Matriz Cacao, Cafe y Arroz/MATRIZ FINAL DEL CAFÉ.xlsx
+++ b/Matriz Cacao, Cafe y Arroz/MATRIZ FINAL DEL CAFÉ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\proyecto\Matriz Cacao, Cafe y Arroz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38CD72F8-248A-4F19-B0E4-BD41511F3404}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="7575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="7575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="156">
   <si>
     <r>
       <rPr>
@@ -740,14 +741,11 @@
   <si>
     <t>Pratylenchus (lesionadores) y Meloidogyne (agalladores)</t>
   </si>
-  <si>
-    <t>Hemileia vastatrix Berkeley y Broome</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1234,33 +1232,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,12 +1280,57 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1360,15 +1403,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1385,42 +1419,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1463,7 +1461,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1524,7 +1522,7 @@
         <xdr:cNvPr id="3" name="Imagen 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1585,7 +1583,7 @@
         <xdr:cNvPr id="4" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1646,7 +1644,7 @@
         <xdr:cNvPr id="9" name="8 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1690,7 +1688,7 @@
         <xdr:cNvPr id="11" name="10 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1740,7 +1738,7 @@
         <xdr:cNvPr id="13" name="Imagen 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2070,11 +2068,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:N13"/>
+      <selection activeCell="C7" sqref="C7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,331 +2323,331 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:BC174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:I41"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100:N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="6:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="H2" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="101" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="89" t="str">
+      <c r="J2" s="104" t="str">
         <f>[1]Hoja1!$B$6</f>
         <v xml:space="preserve">EL café tiene su origen en África – Etiopia luego paso a Europa y después de algunos siglos llego al continente americano.
 Al Ecuador el café llego en los años 1800 y desde entonces ha tenido importantes aportaciones como fuente de empleo y de divisas al país
 El café se siembra y se cosecha en el litoral ecuatoriano y parte del oriente, la provincia de Manabí fue uno de preponderante del cultivo del Café, a partir del año 1860 ya se cultivaba el producto en este sector
 </v>
       </c>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="91"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="106"/>
     </row>
     <row r="3" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F3" s="78"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="93"/>
-      <c r="T3" s="93"/>
-      <c r="U3" s="93"/>
-      <c r="V3" s="93"/>
-      <c r="W3" s="93"/>
-      <c r="X3" s="94"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="109"/>
     </row>
     <row r="4" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F4" s="78"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="94"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="108"/>
+      <c r="W4" s="108"/>
+      <c r="X4" s="109"/>
     </row>
     <row r="5" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F5" s="78"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
-      <c r="S5" s="93"/>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="94"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="109"/>
     </row>
     <row r="6" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F6" s="78"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="93"/>
-      <c r="S6" s="93"/>
-      <c r="T6" s="93"/>
-      <c r="U6" s="93"/>
-      <c r="V6" s="93"/>
-      <c r="W6" s="93"/>
-      <c r="X6" s="94"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="108"/>
+      <c r="T6" s="108"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="108"/>
+      <c r="X6" s="109"/>
     </row>
     <row r="7" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F7" s="78"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="93"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="93"/>
-      <c r="S7" s="93"/>
-      <c r="T7" s="93"/>
-      <c r="U7" s="93"/>
-      <c r="V7" s="93"/>
-      <c r="W7" s="93"/>
-      <c r="X7" s="94"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="108"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="109"/>
     </row>
     <row r="8" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F8" s="78"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93"/>
-      <c r="U8" s="93"/>
-      <c r="V8" s="93"/>
-      <c r="W8" s="93"/>
-      <c r="X8" s="94"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="108"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="108"/>
+      <c r="U8" s="108"/>
+      <c r="V8" s="108"/>
+      <c r="W8" s="108"/>
+      <c r="X8" s="109"/>
     </row>
     <row r="9" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F9" s="78"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="93"/>
-      <c r="N9" s="93"/>
-      <c r="O9" s="93"/>
-      <c r="P9" s="93"/>
-      <c r="Q9" s="93"/>
-      <c r="R9" s="93"/>
-      <c r="S9" s="93"/>
-      <c r="T9" s="93"/>
-      <c r="U9" s="93"/>
-      <c r="V9" s="93"/>
-      <c r="W9" s="93"/>
-      <c r="X9" s="94"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108"/>
+      <c r="U9" s="108"/>
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="109"/>
     </row>
     <row r="10" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="78"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="93"/>
-      <c r="N10" s="93"/>
-      <c r="O10" s="93"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="93"/>
-      <c r="R10" s="93"/>
-      <c r="S10" s="93"/>
-      <c r="T10" s="93"/>
-      <c r="U10" s="93"/>
-      <c r="V10" s="93"/>
-      <c r="W10" s="93"/>
-      <c r="X10" s="94"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="108"/>
+      <c r="L10" s="108"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="108"/>
+      <c r="O10" s="108"/>
+      <c r="P10" s="108"/>
+      <c r="Q10" s="108"/>
+      <c r="R10" s="108"/>
+      <c r="S10" s="108"/>
+      <c r="T10" s="108"/>
+      <c r="U10" s="108"/>
+      <c r="V10" s="108"/>
+      <c r="W10" s="108"/>
+      <c r="X10" s="109"/>
     </row>
     <row r="11" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="78"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="93"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
-      <c r="Q11" s="93"/>
-      <c r="R11" s="93"/>
-      <c r="S11" s="93"/>
-      <c r="T11" s="93"/>
-      <c r="U11" s="93"/>
-      <c r="V11" s="93"/>
-      <c r="W11" s="93"/>
-      <c r="X11" s="94"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="108"/>
+      <c r="L11" s="108"/>
+      <c r="M11" s="108"/>
+      <c r="N11" s="108"/>
+      <c r="O11" s="108"/>
+      <c r="P11" s="108"/>
+      <c r="Q11" s="108"/>
+      <c r="R11" s="108"/>
+      <c r="S11" s="108"/>
+      <c r="T11" s="108"/>
+      <c r="U11" s="108"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="108"/>
+      <c r="X11" s="109"/>
     </row>
     <row r="12" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="78"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="93"/>
-      <c r="N12" s="93"/>
-      <c r="O12" s="93"/>
-      <c r="P12" s="93"/>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="93"/>
-      <c r="T12" s="93"/>
-      <c r="U12" s="93"/>
-      <c r="V12" s="93"/>
-      <c r="W12" s="93"/>
-      <c r="X12" s="94"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="108"/>
+      <c r="L12" s="108"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="108"/>
+      <c r="T12" s="108"/>
+      <c r="U12" s="108"/>
+      <c r="V12" s="108"/>
+      <c r="W12" s="108"/>
+      <c r="X12" s="109"/>
     </row>
     <row r="13" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="79"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="96"/>
-      <c r="O13" s="96"/>
-      <c r="P13" s="96"/>
-      <c r="Q13" s="96"/>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="96"/>
-      <c r="V13" s="96"/>
-      <c r="W13" s="96"/>
-      <c r="X13" s="97"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="111"/>
+      <c r="T13" s="111"/>
+      <c r="U13" s="111"/>
+      <c r="V13" s="111"/>
+      <c r="W13" s="111"/>
+      <c r="X13" s="112"/>
     </row>
     <row r="16" spans="6:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="107" t="s">
+      <c r="F16" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="108"/>
-      <c r="L16" s="108"/>
-      <c r="M16" s="108"/>
-      <c r="N16" s="109"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="77"/>
       <c r="O16" s="6"/>
     </row>
     <row r="17" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F17" s="110"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="111"/>
-      <c r="L17" s="111"/>
-      <c r="M17" s="111"/>
-      <c r="N17" s="112"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="80"/>
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="113" t="s">
+      <c r="F18" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
-      <c r="L18" s="114"/>
-      <c r="M18" s="114"/>
-      <c r="N18" s="115"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="83"/>
       <c r="O18" s="6"/>
     </row>
     <row r="19" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F19" s="116"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="117"/>
-      <c r="J19" s="117"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
-      <c r="N19" s="118"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="86"/>
       <c r="O19" s="6"/>
     </row>
     <row r="20" spans="2:55" x14ac:dyDescent="0.25">
@@ -2663,7 +2661,7 @@
         <v>19</v>
       </c>
       <c r="K20" s="52"/>
-      <c r="L20" s="98" t="s">
+      <c r="L20" s="72" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="50" t="s">
@@ -2679,7 +2677,7 @@
       <c r="I21" s="55"/>
       <c r="J21" s="65"/>
       <c r="K21" s="67"/>
-      <c r="L21" s="99"/>
+      <c r="L21" s="73"/>
       <c r="M21" s="65"/>
       <c r="N21" s="67"/>
       <c r="O21" s="6"/>
@@ -2701,14 +2699,14 @@
       <c r="I22" s="52"/>
       <c r="J22" s="65"/>
       <c r="K22" s="67"/>
-      <c r="L22" s="99"/>
+      <c r="L22" s="73"/>
       <c r="M22" s="65"/>
       <c r="N22" s="67"/>
       <c r="O22" s="6"/>
-      <c r="P22" s="57" t="s">
+      <c r="P22" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="Q22" s="58"/>
+      <c r="Q22" s="57"/>
       <c r="R22" s="50" t="s">
         <v>68</v>
       </c>
@@ -2779,12 +2777,12 @@
       <c r="I23" s="55"/>
       <c r="J23" s="53"/>
       <c r="K23" s="55"/>
-      <c r="L23" s="100"/>
+      <c r="L23" s="74"/>
       <c r="M23" s="53"/>
       <c r="N23" s="55"/>
       <c r="O23" s="6"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="60"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="59"/>
       <c r="R23" s="53"/>
       <c r="S23" s="55"/>
       <c r="T23" s="53"/>
@@ -3355,10 +3353,8 @@
         <v>115</v>
       </c>
       <c r="G33" s="11"/>
-      <c r="H33" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="I33" s="56"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
       <c r="J33" s="9" t="s">
         <v>117</v>
       </c>
@@ -3425,8 +3421,8 @@
       <c r="E34" s="43"/>
       <c r="F34" s="12"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
       <c r="J34" s="12"/>
       <c r="K34" s="14"/>
       <c r="L34" s="48"/>
@@ -3481,8 +3477,8 @@
       <c r="E35" s="43"/>
       <c r="F35" s="12"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
       <c r="J35" s="12"/>
       <c r="K35" s="14"/>
       <c r="L35" s="48"/>
@@ -3537,8 +3533,8 @@
       <c r="E36" s="43"/>
       <c r="F36" s="12"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
       <c r="J36" s="12"/>
       <c r="K36" s="14"/>
       <c r="L36" s="48"/>
@@ -3593,8 +3589,8 @@
       <c r="E37" s="43"/>
       <c r="F37" s="12"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
       <c r="J37" s="12"/>
       <c r="K37" s="14"/>
       <c r="L37" s="48"/>
@@ -3649,8 +3645,8 @@
       <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
       <c r="J38" s="12"/>
       <c r="K38" s="14"/>
       <c r="L38" s="48"/>
@@ -3705,8 +3701,8 @@
       <c r="E39" s="43"/>
       <c r="F39" s="12"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
       <c r="J39" s="12"/>
       <c r="K39" s="14"/>
       <c r="L39" s="48"/>
@@ -3761,8 +3757,8 @@
       <c r="E40" s="43"/>
       <c r="F40" s="12"/>
       <c r="G40" s="14"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
       <c r="J40" s="12"/>
       <c r="K40" s="14"/>
       <c r="L40" s="48"/>
@@ -3817,8 +3813,8 @@
       <c r="E41" s="46"/>
       <c r="F41" s="15"/>
       <c r="G41" s="17"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
       <c r="J41" s="15"/>
       <c r="K41" s="17"/>
       <c r="L41" s="49"/>
@@ -4222,9 +4218,9 @@
       <c r="AX47" s="10"/>
       <c r="AY47" s="10"/>
       <c r="AZ47" s="11"/>
-      <c r="BA47" s="56"/>
-      <c r="BB47" s="56"/>
-      <c r="BC47" s="56"/>
+      <c r="BA47" s="64"/>
+      <c r="BB47" s="64"/>
+      <c r="BC47" s="64"/>
     </row>
     <row r="48" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B48" s="41"/>
@@ -4278,9 +4274,9 @@
       <c r="AX48" s="13"/>
       <c r="AY48" s="13"/>
       <c r="AZ48" s="14"/>
-      <c r="BA48" s="56"/>
-      <c r="BB48" s="56"/>
-      <c r="BC48" s="56"/>
+      <c r="BA48" s="64"/>
+      <c r="BB48" s="64"/>
+      <c r="BC48" s="64"/>
     </row>
     <row r="49" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B49" s="41"/>
@@ -4334,9 +4330,9 @@
       <c r="AX49" s="13"/>
       <c r="AY49" s="13"/>
       <c r="AZ49" s="14"/>
-      <c r="BA49" s="56"/>
-      <c r="BB49" s="56"/>
-      <c r="BC49" s="56"/>
+      <c r="BA49" s="64"/>
+      <c r="BB49" s="64"/>
+      <c r="BC49" s="64"/>
     </row>
     <row r="50" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B50" s="41"/>
@@ -4390,9 +4386,9 @@
       <c r="AX50" s="13"/>
       <c r="AY50" s="13"/>
       <c r="AZ50" s="14"/>
-      <c r="BA50" s="56"/>
-      <c r="BB50" s="56"/>
-      <c r="BC50" s="56"/>
+      <c r="BA50" s="64"/>
+      <c r="BB50" s="64"/>
+      <c r="BC50" s="64"/>
     </row>
     <row r="51" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B51" s="41"/>
@@ -4446,9 +4442,9 @@
       <c r="AX51" s="13"/>
       <c r="AY51" s="13"/>
       <c r="AZ51" s="14"/>
-      <c r="BA51" s="56"/>
-      <c r="BB51" s="56"/>
-      <c r="BC51" s="56"/>
+      <c r="BA51" s="64"/>
+      <c r="BB51" s="64"/>
+      <c r="BC51" s="64"/>
     </row>
     <row r="52" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B52" s="41"/>
@@ -4502,9 +4498,9 @@
       <c r="AX52" s="13"/>
       <c r="AY52" s="13"/>
       <c r="AZ52" s="14"/>
-      <c r="BA52" s="56"/>
-      <c r="BB52" s="56"/>
-      <c r="BC52" s="56"/>
+      <c r="BA52" s="64"/>
+      <c r="BB52" s="64"/>
+      <c r="BC52" s="64"/>
     </row>
     <row r="53" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B53" s="44"/>
@@ -4558,9 +4554,9 @@
       <c r="AX53" s="13"/>
       <c r="AY53" s="13"/>
       <c r="AZ53" s="14"/>
-      <c r="BA53" s="56"/>
-      <c r="BB53" s="56"/>
-      <c r="BC53" s="56"/>
+      <c r="BA53" s="64"/>
+      <c r="BB53" s="64"/>
+      <c r="BC53" s="64"/>
     </row>
     <row r="54" spans="2:55" x14ac:dyDescent="0.25">
       <c r="O54" s="4"/>
@@ -4601,9 +4597,9 @@
       <c r="AX54" s="13"/>
       <c r="AY54" s="13"/>
       <c r="AZ54" s="14"/>
-      <c r="BA54" s="56"/>
-      <c r="BB54" s="56"/>
-      <c r="BC54" s="56"/>
+      <c r="BA54" s="64"/>
+      <c r="BB54" s="64"/>
+      <c r="BC54" s="64"/>
     </row>
     <row r="55" spans="2:55" x14ac:dyDescent="0.25">
       <c r="F55" s="4"/>
@@ -4653,22 +4649,22 @@
       <c r="AX55" s="13"/>
       <c r="AY55" s="13"/>
       <c r="AZ55" s="14"/>
-      <c r="BA55" s="56"/>
-      <c r="BB55" s="56"/>
-      <c r="BC55" s="56"/>
+      <c r="BA55" s="64"/>
+      <c r="BB55" s="64"/>
+      <c r="BC55" s="64"/>
     </row>
     <row r="56" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F56" s="101" t="s">
+      <c r="F56" s="113" t="s">
         <v>134</v>
       </c>
-      <c r="G56" s="102"/>
-      <c r="H56" s="102"/>
-      <c r="I56" s="102"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="102"/>
-      <c r="L56" s="102"/>
-      <c r="M56" s="102"/>
-      <c r="N56" s="103"/>
+      <c r="G56" s="114"/>
+      <c r="H56" s="114"/>
+      <c r="I56" s="114"/>
+      <c r="J56" s="114"/>
+      <c r="K56" s="114"/>
+      <c r="L56" s="114"/>
+      <c r="M56" s="114"/>
+      <c r="N56" s="115"/>
       <c r="O56" s="4"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="14"/>
@@ -4707,20 +4703,20 @@
       <c r="AX56" s="13"/>
       <c r="AY56" s="13"/>
       <c r="AZ56" s="14"/>
-      <c r="BA56" s="56"/>
-      <c r="BB56" s="56"/>
-      <c r="BC56" s="56"/>
+      <c r="BA56" s="64"/>
+      <c r="BB56" s="64"/>
+      <c r="BC56" s="64"/>
     </row>
     <row r="57" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F57" s="104"/>
-      <c r="G57" s="105"/>
-      <c r="H57" s="105"/>
-      <c r="I57" s="105"/>
-      <c r="J57" s="105"/>
-      <c r="K57" s="105"/>
-      <c r="L57" s="105"/>
-      <c r="M57" s="105"/>
-      <c r="N57" s="106"/>
+      <c r="F57" s="116"/>
+      <c r="G57" s="117"/>
+      <c r="H57" s="117"/>
+      <c r="I57" s="117"/>
+      <c r="J57" s="117"/>
+      <c r="K57" s="117"/>
+      <c r="L57" s="117"/>
+      <c r="M57" s="117"/>
+      <c r="N57" s="118"/>
       <c r="O57" s="4"/>
       <c r="P57" s="15"/>
       <c r="Q57" s="17"/>
@@ -4759,9 +4755,9 @@
       <c r="AX57" s="16"/>
       <c r="AY57" s="16"/>
       <c r="AZ57" s="17"/>
-      <c r="BA57" s="56"/>
-      <c r="BB57" s="56"/>
-      <c r="BC57" s="56"/>
+      <c r="BA57" s="64"/>
+      <c r="BB57" s="64"/>
+      <c r="BC57" s="64"/>
     </row>
     <row r="58" spans="2:55" x14ac:dyDescent="0.25">
       <c r="F58" s="50" t="s">
@@ -4774,7 +4770,7 @@
         <v>19</v>
       </c>
       <c r="K58" s="52"/>
-      <c r="L58" s="98" t="s">
+      <c r="L58" s="72" t="s">
         <v>20</v>
       </c>
       <c r="M58" s="50" t="s">
@@ -4830,7 +4826,7 @@
       <c r="I59" s="55"/>
       <c r="J59" s="65"/>
       <c r="K59" s="67"/>
-      <c r="L59" s="99"/>
+      <c r="L59" s="73"/>
       <c r="M59" s="65"/>
       <c r="N59" s="67"/>
       <c r="O59" s="4"/>
@@ -4892,14 +4888,14 @@
       <c r="I60" s="52"/>
       <c r="J60" s="65"/>
       <c r="K60" s="67"/>
-      <c r="L60" s="99"/>
+      <c r="L60" s="73"/>
       <c r="M60" s="65"/>
       <c r="N60" s="67"/>
       <c r="O60" s="6"/>
-      <c r="P60" s="61" t="s">
+      <c r="P60" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="Q60" s="62"/>
+      <c r="Q60" s="61"/>
       <c r="R60" s="65" t="s">
         <v>68</v>
       </c>
@@ -4970,12 +4966,12 @@
       <c r="I61" s="55"/>
       <c r="J61" s="53"/>
       <c r="K61" s="55"/>
-      <c r="L61" s="100"/>
+      <c r="L61" s="74"/>
       <c r="M61" s="53"/>
       <c r="N61" s="55"/>
       <c r="O61" s="6"/>
-      <c r="P61" s="63"/>
-      <c r="Q61" s="64"/>
+      <c r="P61" s="62"/>
+      <c r="Q61" s="63"/>
       <c r="R61" s="53"/>
       <c r="S61" s="55"/>
       <c r="T61" s="53"/>
@@ -5020,19 +5016,19 @@
       <c r="C62" s="39"/>
       <c r="D62" s="39"/>
       <c r="E62" s="40"/>
-      <c r="F62" s="56" t="s">
+      <c r="F62" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="G62" s="56"/>
+      <c r="G62" s="64"/>
       <c r="H62" s="9" t="s">
         <v>119</v>
       </c>
       <c r="I62" s="11"/>
-      <c r="J62" s="56" t="s">
+      <c r="J62" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="K62" s="56"/>
-      <c r="L62" s="56"/>
+      <c r="K62" s="64"/>
+      <c r="L62" s="64"/>
       <c r="M62" s="9" t="s">
         <v>121</v>
       </c>
@@ -5079,14 +5075,14 @@
         <v>82</v>
       </c>
       <c r="AN62" s="11"/>
-      <c r="AO62" s="56" t="s">
+      <c r="AO62" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="AP62" s="56"/>
-      <c r="AQ62" s="56"/>
-      <c r="AR62" s="56"/>
-      <c r="AS62" s="56"/>
-      <c r="AT62" s="56"/>
+      <c r="AP62" s="64"/>
+      <c r="AQ62" s="64"/>
+      <c r="AR62" s="64"/>
+      <c r="AS62" s="64"/>
+      <c r="AT62" s="64"/>
       <c r="AU62" s="9" t="s">
         <v>150</v>
       </c>
@@ -5106,13 +5102,13 @@
       <c r="C63" s="42"/>
       <c r="D63" s="42"/>
       <c r="E63" s="43"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="12"/>
       <c r="I63" s="14"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
+      <c r="J63" s="64"/>
+      <c r="K63" s="64"/>
+      <c r="L63" s="64"/>
       <c r="M63" s="12"/>
       <c r="N63" s="14"/>
       <c r="O63" s="1"/>
@@ -5141,12 +5137,12 @@
       <c r="AL63" s="14"/>
       <c r="AM63" s="12"/>
       <c r="AN63" s="14"/>
-      <c r="AO63" s="56"/>
-      <c r="AP63" s="56"/>
-      <c r="AQ63" s="56"/>
-      <c r="AR63" s="56"/>
-      <c r="AS63" s="56"/>
-      <c r="AT63" s="56"/>
+      <c r="AO63" s="64"/>
+      <c r="AP63" s="64"/>
+      <c r="AQ63" s="64"/>
+      <c r="AR63" s="64"/>
+      <c r="AS63" s="64"/>
+      <c r="AT63" s="64"/>
       <c r="AU63" s="12"/>
       <c r="AV63" s="13"/>
       <c r="AW63" s="13"/>
@@ -5162,13 +5158,13 @@
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="43"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="12"/>
       <c r="I64" s="14"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
-      <c r="L64" s="56"/>
+      <c r="J64" s="64"/>
+      <c r="K64" s="64"/>
+      <c r="L64" s="64"/>
       <c r="M64" s="12"/>
       <c r="N64" s="14"/>
       <c r="O64" s="1"/>
@@ -5197,12 +5193,12 @@
       <c r="AL64" s="14"/>
       <c r="AM64" s="12"/>
       <c r="AN64" s="14"/>
-      <c r="AO64" s="56"/>
-      <c r="AP64" s="56"/>
-      <c r="AQ64" s="56"/>
-      <c r="AR64" s="56"/>
-      <c r="AS64" s="56"/>
-      <c r="AT64" s="56"/>
+      <c r="AO64" s="64"/>
+      <c r="AP64" s="64"/>
+      <c r="AQ64" s="64"/>
+      <c r="AR64" s="64"/>
+      <c r="AS64" s="64"/>
+      <c r="AT64" s="64"/>
       <c r="AU64" s="12"/>
       <c r="AV64" s="13"/>
       <c r="AW64" s="13"/>
@@ -5218,13 +5214,13 @@
       <c r="C65" s="42"/>
       <c r="D65" s="42"/>
       <c r="E65" s="43"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="12"/>
       <c r="I65" s="14"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="56"/>
-      <c r="L65" s="56"/>
+      <c r="J65" s="64"/>
+      <c r="K65" s="64"/>
+      <c r="L65" s="64"/>
       <c r="M65" s="12"/>
       <c r="N65" s="14"/>
       <c r="O65" s="1"/>
@@ -5253,12 +5249,12 @@
       <c r="AL65" s="14"/>
       <c r="AM65" s="12"/>
       <c r="AN65" s="14"/>
-      <c r="AO65" s="56"/>
-      <c r="AP65" s="56"/>
-      <c r="AQ65" s="56"/>
-      <c r="AR65" s="56"/>
-      <c r="AS65" s="56"/>
-      <c r="AT65" s="56"/>
+      <c r="AO65" s="64"/>
+      <c r="AP65" s="64"/>
+      <c r="AQ65" s="64"/>
+      <c r="AR65" s="64"/>
+      <c r="AS65" s="64"/>
+      <c r="AT65" s="64"/>
       <c r="AU65" s="12"/>
       <c r="AV65" s="13"/>
       <c r="AW65" s="13"/>
@@ -5274,13 +5270,13 @@
       <c r="C66" s="42"/>
       <c r="D66" s="42"/>
       <c r="E66" s="43"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="12"/>
       <c r="I66" s="14"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="56"/>
-      <c r="L66" s="56"/>
+      <c r="J66" s="64"/>
+      <c r="K66" s="64"/>
+      <c r="L66" s="64"/>
       <c r="M66" s="12"/>
       <c r="N66" s="14"/>
       <c r="O66" s="1"/>
@@ -5309,12 +5305,12 @@
       <c r="AL66" s="14"/>
       <c r="AM66" s="12"/>
       <c r="AN66" s="14"/>
-      <c r="AO66" s="56"/>
-      <c r="AP66" s="56"/>
-      <c r="AQ66" s="56"/>
-      <c r="AR66" s="56"/>
-      <c r="AS66" s="56"/>
-      <c r="AT66" s="56"/>
+      <c r="AO66" s="64"/>
+      <c r="AP66" s="64"/>
+      <c r="AQ66" s="64"/>
+      <c r="AR66" s="64"/>
+      <c r="AS66" s="64"/>
+      <c r="AT66" s="64"/>
       <c r="AU66" s="12"/>
       <c r="AV66" s="13"/>
       <c r="AW66" s="13"/>
@@ -5330,13 +5326,13 @@
       <c r="C67" s="45"/>
       <c r="D67" s="45"/>
       <c r="E67" s="46"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="15"/>
       <c r="I67" s="17"/>
-      <c r="J67" s="56"/>
-      <c r="K67" s="56"/>
-      <c r="L67" s="56"/>
+      <c r="J67" s="64"/>
+      <c r="K67" s="64"/>
+      <c r="L67" s="64"/>
       <c r="M67" s="15"/>
       <c r="N67" s="17"/>
       <c r="O67" s="1"/>
@@ -5365,12 +5361,12 @@
       <c r="AL67" s="17"/>
       <c r="AM67" s="15"/>
       <c r="AN67" s="17"/>
-      <c r="AO67" s="56"/>
-      <c r="AP67" s="56"/>
-      <c r="AQ67" s="56"/>
-      <c r="AR67" s="56"/>
-      <c r="AS67" s="56"/>
-      <c r="AT67" s="56"/>
+      <c r="AO67" s="64"/>
+      <c r="AP67" s="64"/>
+      <c r="AQ67" s="64"/>
+      <c r="AR67" s="64"/>
+      <c r="AS67" s="64"/>
+      <c r="AT67" s="64"/>
       <c r="AU67" s="15"/>
       <c r="AV67" s="16"/>
       <c r="AW67" s="16"/>
@@ -5401,8 +5397,8 @@
       <c r="L68" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="M68" s="56"/>
-      <c r="N68" s="56"/>
+      <c r="M68" s="64"/>
+      <c r="N68" s="64"/>
       <c r="O68" s="1"/>
       <c r="P68" s="9" t="s">
         <v>22</v>
@@ -5441,26 +5437,26 @@
       <c r="AJ68" s="10"/>
       <c r="AK68" s="10"/>
       <c r="AL68" s="11"/>
-      <c r="AM68" s="56" t="s">
+      <c r="AM68" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="AN68" s="56"/>
-      <c r="AO68" s="56" t="s">
+      <c r="AN68" s="64"/>
+      <c r="AO68" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="AP68" s="56"/>
-      <c r="AQ68" s="56"/>
-      <c r="AR68" s="56"/>
-      <c r="AS68" s="56"/>
-      <c r="AT68" s="56"/>
-      <c r="AU68" s="56" t="s">
+      <c r="AP68" s="64"/>
+      <c r="AQ68" s="64"/>
+      <c r="AR68" s="64"/>
+      <c r="AS68" s="64"/>
+      <c r="AT68" s="64"/>
+      <c r="AU68" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="AV68" s="56"/>
-      <c r="AW68" s="56"/>
-      <c r="AX68" s="56"/>
-      <c r="AY68" s="56"/>
-      <c r="AZ68" s="56"/>
+      <c r="AV68" s="64"/>
+      <c r="AW68" s="64"/>
+      <c r="AX68" s="64"/>
+      <c r="AY68" s="64"/>
+      <c r="AZ68" s="64"/>
       <c r="BA68" s="9" t="s">
         <v>77</v>
       </c>
@@ -5479,8 +5475,8 @@
       <c r="J69" s="12"/>
       <c r="K69" s="14"/>
       <c r="L69" s="48"/>
-      <c r="M69" s="56"/>
-      <c r="N69" s="56"/>
+      <c r="M69" s="64"/>
+      <c r="N69" s="64"/>
       <c r="O69" s="1"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="14"/>
@@ -5505,20 +5501,20 @@
       <c r="AJ69" s="13"/>
       <c r="AK69" s="13"/>
       <c r="AL69" s="14"/>
-      <c r="AM69" s="56"/>
-      <c r="AN69" s="56"/>
-      <c r="AO69" s="56"/>
-      <c r="AP69" s="56"/>
-      <c r="AQ69" s="56"/>
-      <c r="AR69" s="56"/>
-      <c r="AS69" s="56"/>
-      <c r="AT69" s="56"/>
-      <c r="AU69" s="56"/>
-      <c r="AV69" s="56"/>
-      <c r="AW69" s="56"/>
-      <c r="AX69" s="56"/>
-      <c r="AY69" s="56"/>
-      <c r="AZ69" s="56"/>
+      <c r="AM69" s="64"/>
+      <c r="AN69" s="64"/>
+      <c r="AO69" s="64"/>
+      <c r="AP69" s="64"/>
+      <c r="AQ69" s="64"/>
+      <c r="AR69" s="64"/>
+      <c r="AS69" s="64"/>
+      <c r="AT69" s="64"/>
+      <c r="AU69" s="64"/>
+      <c r="AV69" s="64"/>
+      <c r="AW69" s="64"/>
+      <c r="AX69" s="64"/>
+      <c r="AY69" s="64"/>
+      <c r="AZ69" s="64"/>
       <c r="BA69" s="12"/>
       <c r="BB69" s="13"/>
       <c r="BC69" s="14"/>
@@ -5535,8 +5531,8 @@
       <c r="J70" s="12"/>
       <c r="K70" s="14"/>
       <c r="L70" s="48"/>
-      <c r="M70" s="56"/>
-      <c r="N70" s="56"/>
+      <c r="M70" s="64"/>
+      <c r="N70" s="64"/>
       <c r="O70" s="1"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="14"/>
@@ -5561,20 +5557,20 @@
       <c r="AJ70" s="13"/>
       <c r="AK70" s="13"/>
       <c r="AL70" s="14"/>
-      <c r="AM70" s="56"/>
-      <c r="AN70" s="56"/>
-      <c r="AO70" s="56"/>
-      <c r="AP70" s="56"/>
-      <c r="AQ70" s="56"/>
-      <c r="AR70" s="56"/>
-      <c r="AS70" s="56"/>
-      <c r="AT70" s="56"/>
-      <c r="AU70" s="56"/>
-      <c r="AV70" s="56"/>
-      <c r="AW70" s="56"/>
-      <c r="AX70" s="56"/>
-      <c r="AY70" s="56"/>
-      <c r="AZ70" s="56"/>
+      <c r="AM70" s="64"/>
+      <c r="AN70" s="64"/>
+      <c r="AO70" s="64"/>
+      <c r="AP70" s="64"/>
+      <c r="AQ70" s="64"/>
+      <c r="AR70" s="64"/>
+      <c r="AS70" s="64"/>
+      <c r="AT70" s="64"/>
+      <c r="AU70" s="64"/>
+      <c r="AV70" s="64"/>
+      <c r="AW70" s="64"/>
+      <c r="AX70" s="64"/>
+      <c r="AY70" s="64"/>
+      <c r="AZ70" s="64"/>
       <c r="BA70" s="12"/>
       <c r="BB70" s="13"/>
       <c r="BC70" s="14"/>
@@ -5591,8 +5587,8 @@
       <c r="J71" s="12"/>
       <c r="K71" s="14"/>
       <c r="L71" s="48"/>
-      <c r="M71" s="56"/>
-      <c r="N71" s="56"/>
+      <c r="M71" s="64"/>
+      <c r="N71" s="64"/>
       <c r="O71" s="1"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="14"/>
@@ -5617,20 +5613,20 @@
       <c r="AJ71" s="13"/>
       <c r="AK71" s="13"/>
       <c r="AL71" s="14"/>
-      <c r="AM71" s="56"/>
-      <c r="AN71" s="56"/>
-      <c r="AO71" s="56"/>
-      <c r="AP71" s="56"/>
-      <c r="AQ71" s="56"/>
-      <c r="AR71" s="56"/>
-      <c r="AS71" s="56"/>
-      <c r="AT71" s="56"/>
-      <c r="AU71" s="56"/>
-      <c r="AV71" s="56"/>
-      <c r="AW71" s="56"/>
-      <c r="AX71" s="56"/>
-      <c r="AY71" s="56"/>
-      <c r="AZ71" s="56"/>
+      <c r="AM71" s="64"/>
+      <c r="AN71" s="64"/>
+      <c r="AO71" s="64"/>
+      <c r="AP71" s="64"/>
+      <c r="AQ71" s="64"/>
+      <c r="AR71" s="64"/>
+      <c r="AS71" s="64"/>
+      <c r="AT71" s="64"/>
+      <c r="AU71" s="64"/>
+      <c r="AV71" s="64"/>
+      <c r="AW71" s="64"/>
+      <c r="AX71" s="64"/>
+      <c r="AY71" s="64"/>
+      <c r="AZ71" s="64"/>
       <c r="BA71" s="12"/>
       <c r="BB71" s="13"/>
       <c r="BC71" s="14"/>
@@ -5647,8 +5643,8 @@
       <c r="J72" s="12"/>
       <c r="K72" s="14"/>
       <c r="L72" s="48"/>
-      <c r="M72" s="56"/>
-      <c r="N72" s="56"/>
+      <c r="M72" s="64"/>
+      <c r="N72" s="64"/>
       <c r="O72" s="1"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="14"/>
@@ -5673,20 +5669,20 @@
       <c r="AJ72" s="13"/>
       <c r="AK72" s="13"/>
       <c r="AL72" s="14"/>
-      <c r="AM72" s="56"/>
-      <c r="AN72" s="56"/>
-      <c r="AO72" s="56"/>
-      <c r="AP72" s="56"/>
-      <c r="AQ72" s="56"/>
-      <c r="AR72" s="56"/>
-      <c r="AS72" s="56"/>
-      <c r="AT72" s="56"/>
-      <c r="AU72" s="56"/>
-      <c r="AV72" s="56"/>
-      <c r="AW72" s="56"/>
-      <c r="AX72" s="56"/>
-      <c r="AY72" s="56"/>
-      <c r="AZ72" s="56"/>
+      <c r="AM72" s="64"/>
+      <c r="AN72" s="64"/>
+      <c r="AO72" s="64"/>
+      <c r="AP72" s="64"/>
+      <c r="AQ72" s="64"/>
+      <c r="AR72" s="64"/>
+      <c r="AS72" s="64"/>
+      <c r="AT72" s="64"/>
+      <c r="AU72" s="64"/>
+      <c r="AV72" s="64"/>
+      <c r="AW72" s="64"/>
+      <c r="AX72" s="64"/>
+      <c r="AY72" s="64"/>
+      <c r="AZ72" s="64"/>
       <c r="BA72" s="12"/>
       <c r="BB72" s="13"/>
       <c r="BC72" s="14"/>
@@ -5703,8 +5699,8 @@
       <c r="J73" s="12"/>
       <c r="K73" s="14"/>
       <c r="L73" s="48"/>
-      <c r="M73" s="56"/>
-      <c r="N73" s="56"/>
+      <c r="M73" s="64"/>
+      <c r="N73" s="64"/>
       <c r="O73" s="1"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="14"/>
@@ -5729,20 +5725,20 @@
       <c r="AJ73" s="13"/>
       <c r="AK73" s="13"/>
       <c r="AL73" s="14"/>
-      <c r="AM73" s="56"/>
-      <c r="AN73" s="56"/>
-      <c r="AO73" s="56"/>
-      <c r="AP73" s="56"/>
-      <c r="AQ73" s="56"/>
-      <c r="AR73" s="56"/>
-      <c r="AS73" s="56"/>
-      <c r="AT73" s="56"/>
-      <c r="AU73" s="56"/>
-      <c r="AV73" s="56"/>
-      <c r="AW73" s="56"/>
-      <c r="AX73" s="56"/>
-      <c r="AY73" s="56"/>
-      <c r="AZ73" s="56"/>
+      <c r="AM73" s="64"/>
+      <c r="AN73" s="64"/>
+      <c r="AO73" s="64"/>
+      <c r="AP73" s="64"/>
+      <c r="AQ73" s="64"/>
+      <c r="AR73" s="64"/>
+      <c r="AS73" s="64"/>
+      <c r="AT73" s="64"/>
+      <c r="AU73" s="64"/>
+      <c r="AV73" s="64"/>
+      <c r="AW73" s="64"/>
+      <c r="AX73" s="64"/>
+      <c r="AY73" s="64"/>
+      <c r="AZ73" s="64"/>
       <c r="BA73" s="12"/>
       <c r="BB73" s="13"/>
       <c r="BC73" s="14"/>
@@ -5759,8 +5755,8 @@
       <c r="J74" s="12"/>
       <c r="K74" s="14"/>
       <c r="L74" s="48"/>
-      <c r="M74" s="56"/>
-      <c r="N74" s="56"/>
+      <c r="M74" s="64"/>
+      <c r="N74" s="64"/>
       <c r="O74" s="1"/>
       <c r="P74" s="12"/>
       <c r="Q74" s="14"/>
@@ -5785,20 +5781,20 @@
       <c r="AJ74" s="13"/>
       <c r="AK74" s="13"/>
       <c r="AL74" s="14"/>
-      <c r="AM74" s="56"/>
-      <c r="AN74" s="56"/>
-      <c r="AO74" s="56"/>
-      <c r="AP74" s="56"/>
-      <c r="AQ74" s="56"/>
-      <c r="AR74" s="56"/>
-      <c r="AS74" s="56"/>
-      <c r="AT74" s="56"/>
-      <c r="AU74" s="56"/>
-      <c r="AV74" s="56"/>
-      <c r="AW74" s="56"/>
-      <c r="AX74" s="56"/>
-      <c r="AY74" s="56"/>
-      <c r="AZ74" s="56"/>
+      <c r="AM74" s="64"/>
+      <c r="AN74" s="64"/>
+      <c r="AO74" s="64"/>
+      <c r="AP74" s="64"/>
+      <c r="AQ74" s="64"/>
+      <c r="AR74" s="64"/>
+      <c r="AS74" s="64"/>
+      <c r="AT74" s="64"/>
+      <c r="AU74" s="64"/>
+      <c r="AV74" s="64"/>
+      <c r="AW74" s="64"/>
+      <c r="AX74" s="64"/>
+      <c r="AY74" s="64"/>
+      <c r="AZ74" s="64"/>
       <c r="BA74" s="12"/>
       <c r="BB74" s="13"/>
       <c r="BC74" s="14"/>
@@ -5815,8 +5811,8 @@
       <c r="J75" s="12"/>
       <c r="K75" s="14"/>
       <c r="L75" s="48"/>
-      <c r="M75" s="56"/>
-      <c r="N75" s="56"/>
+      <c r="M75" s="64"/>
+      <c r="N75" s="64"/>
       <c r="O75" s="1"/>
       <c r="P75" s="12"/>
       <c r="Q75" s="14"/>
@@ -5841,20 +5837,20 @@
       <c r="AJ75" s="13"/>
       <c r="AK75" s="13"/>
       <c r="AL75" s="14"/>
-      <c r="AM75" s="56"/>
-      <c r="AN75" s="56"/>
-      <c r="AO75" s="56"/>
-      <c r="AP75" s="56"/>
-      <c r="AQ75" s="56"/>
-      <c r="AR75" s="56"/>
-      <c r="AS75" s="56"/>
-      <c r="AT75" s="56"/>
-      <c r="AU75" s="56"/>
-      <c r="AV75" s="56"/>
-      <c r="AW75" s="56"/>
-      <c r="AX75" s="56"/>
-      <c r="AY75" s="56"/>
-      <c r="AZ75" s="56"/>
+      <c r="AM75" s="64"/>
+      <c r="AN75" s="64"/>
+      <c r="AO75" s="64"/>
+      <c r="AP75" s="64"/>
+      <c r="AQ75" s="64"/>
+      <c r="AR75" s="64"/>
+      <c r="AS75" s="64"/>
+      <c r="AT75" s="64"/>
+      <c r="AU75" s="64"/>
+      <c r="AV75" s="64"/>
+      <c r="AW75" s="64"/>
+      <c r="AX75" s="64"/>
+      <c r="AY75" s="64"/>
+      <c r="AZ75" s="64"/>
       <c r="BA75" s="12"/>
       <c r="BB75" s="13"/>
       <c r="BC75" s="14"/>
@@ -5871,8 +5867,8 @@
       <c r="J76" s="12"/>
       <c r="K76" s="14"/>
       <c r="L76" s="48"/>
-      <c r="M76" s="56"/>
-      <c r="N76" s="56"/>
+      <c r="M76" s="64"/>
+      <c r="N76" s="64"/>
       <c r="O76" s="1"/>
       <c r="P76" s="12"/>
       <c r="Q76" s="14"/>
@@ -5897,20 +5893,20 @@
       <c r="AJ76" s="13"/>
       <c r="AK76" s="13"/>
       <c r="AL76" s="14"/>
-      <c r="AM76" s="56"/>
-      <c r="AN76" s="56"/>
-      <c r="AO76" s="56"/>
-      <c r="AP76" s="56"/>
-      <c r="AQ76" s="56"/>
-      <c r="AR76" s="56"/>
-      <c r="AS76" s="56"/>
-      <c r="AT76" s="56"/>
-      <c r="AU76" s="56"/>
-      <c r="AV76" s="56"/>
-      <c r="AW76" s="56"/>
-      <c r="AX76" s="56"/>
-      <c r="AY76" s="56"/>
-      <c r="AZ76" s="56"/>
+      <c r="AM76" s="64"/>
+      <c r="AN76" s="64"/>
+      <c r="AO76" s="64"/>
+      <c r="AP76" s="64"/>
+      <c r="AQ76" s="64"/>
+      <c r="AR76" s="64"/>
+      <c r="AS76" s="64"/>
+      <c r="AT76" s="64"/>
+      <c r="AU76" s="64"/>
+      <c r="AV76" s="64"/>
+      <c r="AW76" s="64"/>
+      <c r="AX76" s="64"/>
+      <c r="AY76" s="64"/>
+      <c r="AZ76" s="64"/>
       <c r="BA76" s="12"/>
       <c r="BB76" s="13"/>
       <c r="BC76" s="14"/>
@@ -5927,8 +5923,8 @@
       <c r="J77" s="15"/>
       <c r="K77" s="17"/>
       <c r="L77" s="49"/>
-      <c r="M77" s="56"/>
-      <c r="N77" s="56"/>
+      <c r="M77" s="64"/>
+      <c r="N77" s="64"/>
       <c r="O77" s="1"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="14"/>
@@ -5996,66 +5992,66 @@
       </c>
       <c r="N78" s="11"/>
       <c r="O78" s="1"/>
-      <c r="P78" s="56" t="s">
+      <c r="P78" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="Q78" s="56"/>
+      <c r="Q78" s="64"/>
       <c r="R78" s="68" t="s">
         <v>63</v>
       </c>
       <c r="S78" s="68"/>
-      <c r="T78" s="56" t="s">
+      <c r="T78" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="U78" s="56"/>
-      <c r="V78" s="56" t="s">
+      <c r="U78" s="64"/>
+      <c r="V78" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="W78" s="56"/>
-      <c r="X78" s="56" t="s">
+      <c r="W78" s="64"/>
+      <c r="X78" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="Y78" s="56"/>
-      <c r="Z78" s="56"/>
-      <c r="AA78" s="56"/>
-      <c r="AB78" s="56" t="s">
+      <c r="Y78" s="64"/>
+      <c r="Z78" s="64"/>
+      <c r="AA78" s="64"/>
+      <c r="AB78" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="AC78" s="56"/>
-      <c r="AD78" s="56"/>
-      <c r="AE78" s="56"/>
-      <c r="AF78" s="56"/>
-      <c r="AG78" s="56" t="s">
+      <c r="AC78" s="64"/>
+      <c r="AD78" s="64"/>
+      <c r="AE78" s="64"/>
+      <c r="AF78" s="64"/>
+      <c r="AG78" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="AH78" s="56"/>
-      <c r="AI78" s="56"/>
-      <c r="AJ78" s="56"/>
-      <c r="AK78" s="56"/>
-      <c r="AL78" s="56"/>
-      <c r="AM78" s="56" t="s">
+      <c r="AH78" s="64"/>
+      <c r="AI78" s="64"/>
+      <c r="AJ78" s="64"/>
+      <c r="AK78" s="64"/>
+      <c r="AL78" s="64"/>
+      <c r="AM78" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="AN78" s="56"/>
-      <c r="AO78" s="56" t="s">
+      <c r="AN78" s="64"/>
+      <c r="AO78" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="AP78" s="56"/>
-      <c r="AQ78" s="56"/>
-      <c r="AR78" s="56"/>
-      <c r="AS78" s="56"/>
-      <c r="AT78" s="56"/>
-      <c r="AU78" s="56"/>
-      <c r="AV78" s="56"/>
-      <c r="AW78" s="56"/>
-      <c r="AX78" s="56"/>
-      <c r="AY78" s="56"/>
-      <c r="AZ78" s="56"/>
-      <c r="BA78" s="56" t="s">
+      <c r="AP78" s="64"/>
+      <c r="AQ78" s="64"/>
+      <c r="AR78" s="64"/>
+      <c r="AS78" s="64"/>
+      <c r="AT78" s="64"/>
+      <c r="AU78" s="64"/>
+      <c r="AV78" s="64"/>
+      <c r="AW78" s="64"/>
+      <c r="AX78" s="64"/>
+      <c r="AY78" s="64"/>
+      <c r="AZ78" s="64"/>
+      <c r="BA78" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="BB78" s="56"/>
-      <c r="BC78" s="56"/>
+      <c r="BB78" s="64"/>
+      <c r="BC78" s="64"/>
     </row>
     <row r="79" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B79" s="41"/>
@@ -6072,46 +6068,46 @@
       <c r="M79" s="12"/>
       <c r="N79" s="14"/>
       <c r="O79" s="1"/>
-      <c r="P79" s="56"/>
-      <c r="Q79" s="56"/>
+      <c r="P79" s="64"/>
+      <c r="Q79" s="64"/>
       <c r="R79" s="68"/>
       <c r="S79" s="68"/>
-      <c r="T79" s="56"/>
-      <c r="U79" s="56"/>
-      <c r="V79" s="56"/>
-      <c r="W79" s="56"/>
-      <c r="X79" s="56"/>
-      <c r="Y79" s="56"/>
-      <c r="Z79" s="56"/>
-      <c r="AA79" s="56"/>
-      <c r="AB79" s="56"/>
-      <c r="AC79" s="56"/>
-      <c r="AD79" s="56"/>
-      <c r="AE79" s="56"/>
-      <c r="AF79" s="56"/>
-      <c r="AG79" s="56"/>
-      <c r="AH79" s="56"/>
-      <c r="AI79" s="56"/>
-      <c r="AJ79" s="56"/>
-      <c r="AK79" s="56"/>
-      <c r="AL79" s="56"/>
-      <c r="AM79" s="56"/>
-      <c r="AN79" s="56"/>
-      <c r="AO79" s="56"/>
-      <c r="AP79" s="56"/>
-      <c r="AQ79" s="56"/>
-      <c r="AR79" s="56"/>
-      <c r="AS79" s="56"/>
-      <c r="AT79" s="56"/>
-      <c r="AU79" s="56"/>
-      <c r="AV79" s="56"/>
-      <c r="AW79" s="56"/>
-      <c r="AX79" s="56"/>
-      <c r="AY79" s="56"/>
-      <c r="AZ79" s="56"/>
-      <c r="BA79" s="56"/>
-      <c r="BB79" s="56"/>
-      <c r="BC79" s="56"/>
+      <c r="T79" s="64"/>
+      <c r="U79" s="64"/>
+      <c r="V79" s="64"/>
+      <c r="W79" s="64"/>
+      <c r="X79" s="64"/>
+      <c r="Y79" s="64"/>
+      <c r="Z79" s="64"/>
+      <c r="AA79" s="64"/>
+      <c r="AB79" s="64"/>
+      <c r="AC79" s="64"/>
+      <c r="AD79" s="64"/>
+      <c r="AE79" s="64"/>
+      <c r="AF79" s="64"/>
+      <c r="AG79" s="64"/>
+      <c r="AH79" s="64"/>
+      <c r="AI79" s="64"/>
+      <c r="AJ79" s="64"/>
+      <c r="AK79" s="64"/>
+      <c r="AL79" s="64"/>
+      <c r="AM79" s="64"/>
+      <c r="AN79" s="64"/>
+      <c r="AO79" s="64"/>
+      <c r="AP79" s="64"/>
+      <c r="AQ79" s="64"/>
+      <c r="AR79" s="64"/>
+      <c r="AS79" s="64"/>
+      <c r="AT79" s="64"/>
+      <c r="AU79" s="64"/>
+      <c r="AV79" s="64"/>
+      <c r="AW79" s="64"/>
+      <c r="AX79" s="64"/>
+      <c r="AY79" s="64"/>
+      <c r="AZ79" s="64"/>
+      <c r="BA79" s="64"/>
+      <c r="BB79" s="64"/>
+      <c r="BC79" s="64"/>
     </row>
     <row r="80" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B80" s="41"/>
@@ -6128,46 +6124,46 @@
       <c r="M80" s="12"/>
       <c r="N80" s="14"/>
       <c r="O80" s="1"/>
-      <c r="P80" s="56"/>
-      <c r="Q80" s="56"/>
+      <c r="P80" s="64"/>
+      <c r="Q80" s="64"/>
       <c r="R80" s="68"/>
       <c r="S80" s="68"/>
-      <c r="T80" s="56"/>
-      <c r="U80" s="56"/>
-      <c r="V80" s="56"/>
-      <c r="W80" s="56"/>
-      <c r="X80" s="56"/>
-      <c r="Y80" s="56"/>
-      <c r="Z80" s="56"/>
-      <c r="AA80" s="56"/>
-      <c r="AB80" s="56"/>
-      <c r="AC80" s="56"/>
-      <c r="AD80" s="56"/>
-      <c r="AE80" s="56"/>
-      <c r="AF80" s="56"/>
-      <c r="AG80" s="56"/>
-      <c r="AH80" s="56"/>
-      <c r="AI80" s="56"/>
-      <c r="AJ80" s="56"/>
-      <c r="AK80" s="56"/>
-      <c r="AL80" s="56"/>
-      <c r="AM80" s="56"/>
-      <c r="AN80" s="56"/>
-      <c r="AO80" s="56"/>
-      <c r="AP80" s="56"/>
-      <c r="AQ80" s="56"/>
-      <c r="AR80" s="56"/>
-      <c r="AS80" s="56"/>
-      <c r="AT80" s="56"/>
-      <c r="AU80" s="56"/>
-      <c r="AV80" s="56"/>
-      <c r="AW80" s="56"/>
-      <c r="AX80" s="56"/>
-      <c r="AY80" s="56"/>
-      <c r="AZ80" s="56"/>
-      <c r="BA80" s="56"/>
-      <c r="BB80" s="56"/>
-      <c r="BC80" s="56"/>
+      <c r="T80" s="64"/>
+      <c r="U80" s="64"/>
+      <c r="V80" s="64"/>
+      <c r="W80" s="64"/>
+      <c r="X80" s="64"/>
+      <c r="Y80" s="64"/>
+      <c r="Z80" s="64"/>
+      <c r="AA80" s="64"/>
+      <c r="AB80" s="64"/>
+      <c r="AC80" s="64"/>
+      <c r="AD80" s="64"/>
+      <c r="AE80" s="64"/>
+      <c r="AF80" s="64"/>
+      <c r="AG80" s="64"/>
+      <c r="AH80" s="64"/>
+      <c r="AI80" s="64"/>
+      <c r="AJ80" s="64"/>
+      <c r="AK80" s="64"/>
+      <c r="AL80" s="64"/>
+      <c r="AM80" s="64"/>
+      <c r="AN80" s="64"/>
+      <c r="AO80" s="64"/>
+      <c r="AP80" s="64"/>
+      <c r="AQ80" s="64"/>
+      <c r="AR80" s="64"/>
+      <c r="AS80" s="64"/>
+      <c r="AT80" s="64"/>
+      <c r="AU80" s="64"/>
+      <c r="AV80" s="64"/>
+      <c r="AW80" s="64"/>
+      <c r="AX80" s="64"/>
+      <c r="AY80" s="64"/>
+      <c r="AZ80" s="64"/>
+      <c r="BA80" s="64"/>
+      <c r="BB80" s="64"/>
+      <c r="BC80" s="64"/>
     </row>
     <row r="81" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B81" s="41"/>
@@ -6184,46 +6180,46 @@
       <c r="M81" s="12"/>
       <c r="N81" s="14"/>
       <c r="O81" s="1"/>
-      <c r="P81" s="56"/>
-      <c r="Q81" s="56"/>
+      <c r="P81" s="64"/>
+      <c r="Q81" s="64"/>
       <c r="R81" s="68"/>
       <c r="S81" s="68"/>
-      <c r="T81" s="56"/>
-      <c r="U81" s="56"/>
-      <c r="V81" s="56"/>
-      <c r="W81" s="56"/>
-      <c r="X81" s="56"/>
-      <c r="Y81" s="56"/>
-      <c r="Z81" s="56"/>
-      <c r="AA81" s="56"/>
-      <c r="AB81" s="56"/>
-      <c r="AC81" s="56"/>
-      <c r="AD81" s="56"/>
-      <c r="AE81" s="56"/>
-      <c r="AF81" s="56"/>
-      <c r="AG81" s="56"/>
-      <c r="AH81" s="56"/>
-      <c r="AI81" s="56"/>
-      <c r="AJ81" s="56"/>
-      <c r="AK81" s="56"/>
-      <c r="AL81" s="56"/>
-      <c r="AM81" s="56"/>
-      <c r="AN81" s="56"/>
-      <c r="AO81" s="56"/>
-      <c r="AP81" s="56"/>
-      <c r="AQ81" s="56"/>
-      <c r="AR81" s="56"/>
-      <c r="AS81" s="56"/>
-      <c r="AT81" s="56"/>
-      <c r="AU81" s="56"/>
-      <c r="AV81" s="56"/>
-      <c r="AW81" s="56"/>
-      <c r="AX81" s="56"/>
-      <c r="AY81" s="56"/>
-      <c r="AZ81" s="56"/>
-      <c r="BA81" s="56"/>
-      <c r="BB81" s="56"/>
-      <c r="BC81" s="56"/>
+      <c r="T81" s="64"/>
+      <c r="U81" s="64"/>
+      <c r="V81" s="64"/>
+      <c r="W81" s="64"/>
+      <c r="X81" s="64"/>
+      <c r="Y81" s="64"/>
+      <c r="Z81" s="64"/>
+      <c r="AA81" s="64"/>
+      <c r="AB81" s="64"/>
+      <c r="AC81" s="64"/>
+      <c r="AD81" s="64"/>
+      <c r="AE81" s="64"/>
+      <c r="AF81" s="64"/>
+      <c r="AG81" s="64"/>
+      <c r="AH81" s="64"/>
+      <c r="AI81" s="64"/>
+      <c r="AJ81" s="64"/>
+      <c r="AK81" s="64"/>
+      <c r="AL81" s="64"/>
+      <c r="AM81" s="64"/>
+      <c r="AN81" s="64"/>
+      <c r="AO81" s="64"/>
+      <c r="AP81" s="64"/>
+      <c r="AQ81" s="64"/>
+      <c r="AR81" s="64"/>
+      <c r="AS81" s="64"/>
+      <c r="AT81" s="64"/>
+      <c r="AU81" s="64"/>
+      <c r="AV81" s="64"/>
+      <c r="AW81" s="64"/>
+      <c r="AX81" s="64"/>
+      <c r="AY81" s="64"/>
+      <c r="AZ81" s="64"/>
+      <c r="BA81" s="64"/>
+      <c r="BB81" s="64"/>
+      <c r="BC81" s="64"/>
     </row>
     <row r="82" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B82" s="41"/>
@@ -6240,46 +6236,46 @@
       <c r="M82" s="12"/>
       <c r="N82" s="14"/>
       <c r="O82" s="1"/>
-      <c r="P82" s="56"/>
-      <c r="Q82" s="56"/>
+      <c r="P82" s="64"/>
+      <c r="Q82" s="64"/>
       <c r="R82" s="68"/>
       <c r="S82" s="68"/>
-      <c r="T82" s="56"/>
-      <c r="U82" s="56"/>
-      <c r="V82" s="56"/>
-      <c r="W82" s="56"/>
-      <c r="X82" s="56"/>
-      <c r="Y82" s="56"/>
-      <c r="Z82" s="56"/>
-      <c r="AA82" s="56"/>
-      <c r="AB82" s="56"/>
-      <c r="AC82" s="56"/>
-      <c r="AD82" s="56"/>
-      <c r="AE82" s="56"/>
-      <c r="AF82" s="56"/>
-      <c r="AG82" s="56"/>
-      <c r="AH82" s="56"/>
-      <c r="AI82" s="56"/>
-      <c r="AJ82" s="56"/>
-      <c r="AK82" s="56"/>
-      <c r="AL82" s="56"/>
-      <c r="AM82" s="56"/>
-      <c r="AN82" s="56"/>
-      <c r="AO82" s="56"/>
-      <c r="AP82" s="56"/>
-      <c r="AQ82" s="56"/>
-      <c r="AR82" s="56"/>
-      <c r="AS82" s="56"/>
-      <c r="AT82" s="56"/>
-      <c r="AU82" s="56"/>
-      <c r="AV82" s="56"/>
-      <c r="AW82" s="56"/>
-      <c r="AX82" s="56"/>
-      <c r="AY82" s="56"/>
-      <c r="AZ82" s="56"/>
-      <c r="BA82" s="56"/>
-      <c r="BB82" s="56"/>
-      <c r="BC82" s="56"/>
+      <c r="T82" s="64"/>
+      <c r="U82" s="64"/>
+      <c r="V82" s="64"/>
+      <c r="W82" s="64"/>
+      <c r="X82" s="64"/>
+      <c r="Y82" s="64"/>
+      <c r="Z82" s="64"/>
+      <c r="AA82" s="64"/>
+      <c r="AB82" s="64"/>
+      <c r="AC82" s="64"/>
+      <c r="AD82" s="64"/>
+      <c r="AE82" s="64"/>
+      <c r="AF82" s="64"/>
+      <c r="AG82" s="64"/>
+      <c r="AH82" s="64"/>
+      <c r="AI82" s="64"/>
+      <c r="AJ82" s="64"/>
+      <c r="AK82" s="64"/>
+      <c r="AL82" s="64"/>
+      <c r="AM82" s="64"/>
+      <c r="AN82" s="64"/>
+      <c r="AO82" s="64"/>
+      <c r="AP82" s="64"/>
+      <c r="AQ82" s="64"/>
+      <c r="AR82" s="64"/>
+      <c r="AS82" s="64"/>
+      <c r="AT82" s="64"/>
+      <c r="AU82" s="64"/>
+      <c r="AV82" s="64"/>
+      <c r="AW82" s="64"/>
+      <c r="AX82" s="64"/>
+      <c r="AY82" s="64"/>
+      <c r="AZ82" s="64"/>
+      <c r="BA82" s="64"/>
+      <c r="BB82" s="64"/>
+      <c r="BC82" s="64"/>
     </row>
     <row r="83" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B83" s="41"/>
@@ -6296,46 +6292,46 @@
       <c r="M83" s="12"/>
       <c r="N83" s="14"/>
       <c r="O83" s="1"/>
-      <c r="P83" s="56"/>
-      <c r="Q83" s="56"/>
+      <c r="P83" s="64"/>
+      <c r="Q83" s="64"/>
       <c r="R83" s="68"/>
       <c r="S83" s="68"/>
-      <c r="T83" s="56"/>
-      <c r="U83" s="56"/>
-      <c r="V83" s="56"/>
-      <c r="W83" s="56"/>
-      <c r="X83" s="56"/>
-      <c r="Y83" s="56"/>
-      <c r="Z83" s="56"/>
-      <c r="AA83" s="56"/>
-      <c r="AB83" s="56"/>
-      <c r="AC83" s="56"/>
-      <c r="AD83" s="56"/>
-      <c r="AE83" s="56"/>
-      <c r="AF83" s="56"/>
-      <c r="AG83" s="56"/>
-      <c r="AH83" s="56"/>
-      <c r="AI83" s="56"/>
-      <c r="AJ83" s="56"/>
-      <c r="AK83" s="56"/>
-      <c r="AL83" s="56"/>
-      <c r="AM83" s="56"/>
-      <c r="AN83" s="56"/>
-      <c r="AO83" s="56"/>
-      <c r="AP83" s="56"/>
-      <c r="AQ83" s="56"/>
-      <c r="AR83" s="56"/>
-      <c r="AS83" s="56"/>
-      <c r="AT83" s="56"/>
-      <c r="AU83" s="56"/>
-      <c r="AV83" s="56"/>
-      <c r="AW83" s="56"/>
-      <c r="AX83" s="56"/>
-      <c r="AY83" s="56"/>
-      <c r="AZ83" s="56"/>
-      <c r="BA83" s="56"/>
-      <c r="BB83" s="56"/>
-      <c r="BC83" s="56"/>
+      <c r="T83" s="64"/>
+      <c r="U83" s="64"/>
+      <c r="V83" s="64"/>
+      <c r="W83" s="64"/>
+      <c r="X83" s="64"/>
+      <c r="Y83" s="64"/>
+      <c r="Z83" s="64"/>
+      <c r="AA83" s="64"/>
+      <c r="AB83" s="64"/>
+      <c r="AC83" s="64"/>
+      <c r="AD83" s="64"/>
+      <c r="AE83" s="64"/>
+      <c r="AF83" s="64"/>
+      <c r="AG83" s="64"/>
+      <c r="AH83" s="64"/>
+      <c r="AI83" s="64"/>
+      <c r="AJ83" s="64"/>
+      <c r="AK83" s="64"/>
+      <c r="AL83" s="64"/>
+      <c r="AM83" s="64"/>
+      <c r="AN83" s="64"/>
+      <c r="AO83" s="64"/>
+      <c r="AP83" s="64"/>
+      <c r="AQ83" s="64"/>
+      <c r="AR83" s="64"/>
+      <c r="AS83" s="64"/>
+      <c r="AT83" s="64"/>
+      <c r="AU83" s="64"/>
+      <c r="AV83" s="64"/>
+      <c r="AW83" s="64"/>
+      <c r="AX83" s="64"/>
+      <c r="AY83" s="64"/>
+      <c r="AZ83" s="64"/>
+      <c r="BA83" s="64"/>
+      <c r="BB83" s="64"/>
+      <c r="BC83" s="64"/>
     </row>
     <row r="84" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B84" s="41"/>
@@ -6352,46 +6348,46 @@
       <c r="M84" s="12"/>
       <c r="N84" s="14"/>
       <c r="O84" s="1"/>
-      <c r="P84" s="56"/>
-      <c r="Q84" s="56"/>
+      <c r="P84" s="64"/>
+      <c r="Q84" s="64"/>
       <c r="R84" s="68"/>
       <c r="S84" s="68"/>
-      <c r="T84" s="56"/>
-      <c r="U84" s="56"/>
-      <c r="V84" s="56"/>
-      <c r="W84" s="56"/>
-      <c r="X84" s="56"/>
-      <c r="Y84" s="56"/>
-      <c r="Z84" s="56"/>
-      <c r="AA84" s="56"/>
-      <c r="AB84" s="56"/>
-      <c r="AC84" s="56"/>
-      <c r="AD84" s="56"/>
-      <c r="AE84" s="56"/>
-      <c r="AF84" s="56"/>
-      <c r="AG84" s="56"/>
-      <c r="AH84" s="56"/>
-      <c r="AI84" s="56"/>
-      <c r="AJ84" s="56"/>
-      <c r="AK84" s="56"/>
-      <c r="AL84" s="56"/>
-      <c r="AM84" s="56"/>
-      <c r="AN84" s="56"/>
-      <c r="AO84" s="56"/>
-      <c r="AP84" s="56"/>
-      <c r="AQ84" s="56"/>
-      <c r="AR84" s="56"/>
-      <c r="AS84" s="56"/>
-      <c r="AT84" s="56"/>
-      <c r="AU84" s="56"/>
-      <c r="AV84" s="56"/>
-      <c r="AW84" s="56"/>
-      <c r="AX84" s="56"/>
-      <c r="AY84" s="56"/>
-      <c r="AZ84" s="56"/>
-      <c r="BA84" s="56"/>
-      <c r="BB84" s="56"/>
-      <c r="BC84" s="56"/>
+      <c r="T84" s="64"/>
+      <c r="U84" s="64"/>
+      <c r="V84" s="64"/>
+      <c r="W84" s="64"/>
+      <c r="X84" s="64"/>
+      <c r="Y84" s="64"/>
+      <c r="Z84" s="64"/>
+      <c r="AA84" s="64"/>
+      <c r="AB84" s="64"/>
+      <c r="AC84" s="64"/>
+      <c r="AD84" s="64"/>
+      <c r="AE84" s="64"/>
+      <c r="AF84" s="64"/>
+      <c r="AG84" s="64"/>
+      <c r="AH84" s="64"/>
+      <c r="AI84" s="64"/>
+      <c r="AJ84" s="64"/>
+      <c r="AK84" s="64"/>
+      <c r="AL84" s="64"/>
+      <c r="AM84" s="64"/>
+      <c r="AN84" s="64"/>
+      <c r="AO84" s="64"/>
+      <c r="AP84" s="64"/>
+      <c r="AQ84" s="64"/>
+      <c r="AR84" s="64"/>
+      <c r="AS84" s="64"/>
+      <c r="AT84" s="64"/>
+      <c r="AU84" s="64"/>
+      <c r="AV84" s="64"/>
+      <c r="AW84" s="64"/>
+      <c r="AX84" s="64"/>
+      <c r="AY84" s="64"/>
+      <c r="AZ84" s="64"/>
+      <c r="BA84" s="64"/>
+      <c r="BB84" s="64"/>
+      <c r="BC84" s="64"/>
     </row>
     <row r="85" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B85" s="41"/>
@@ -6408,46 +6404,46 @@
       <c r="M85" s="12"/>
       <c r="N85" s="14"/>
       <c r="O85" s="1"/>
-      <c r="P85" s="56"/>
-      <c r="Q85" s="56"/>
+      <c r="P85" s="64"/>
+      <c r="Q85" s="64"/>
       <c r="R85" s="68"/>
       <c r="S85" s="68"/>
-      <c r="T85" s="56"/>
-      <c r="U85" s="56"/>
-      <c r="V85" s="56"/>
-      <c r="W85" s="56"/>
-      <c r="X85" s="56"/>
-      <c r="Y85" s="56"/>
-      <c r="Z85" s="56"/>
-      <c r="AA85" s="56"/>
-      <c r="AB85" s="56"/>
-      <c r="AC85" s="56"/>
-      <c r="AD85" s="56"/>
-      <c r="AE85" s="56"/>
-      <c r="AF85" s="56"/>
-      <c r="AG85" s="56"/>
-      <c r="AH85" s="56"/>
-      <c r="AI85" s="56"/>
-      <c r="AJ85" s="56"/>
-      <c r="AK85" s="56"/>
-      <c r="AL85" s="56"/>
-      <c r="AM85" s="56"/>
-      <c r="AN85" s="56"/>
-      <c r="AO85" s="56"/>
-      <c r="AP85" s="56"/>
-      <c r="AQ85" s="56"/>
-      <c r="AR85" s="56"/>
-      <c r="AS85" s="56"/>
-      <c r="AT85" s="56"/>
-      <c r="AU85" s="56"/>
-      <c r="AV85" s="56"/>
-      <c r="AW85" s="56"/>
-      <c r="AX85" s="56"/>
-      <c r="AY85" s="56"/>
-      <c r="AZ85" s="56"/>
-      <c r="BA85" s="56"/>
-      <c r="BB85" s="56"/>
-      <c r="BC85" s="56"/>
+      <c r="T85" s="64"/>
+      <c r="U85" s="64"/>
+      <c r="V85" s="64"/>
+      <c r="W85" s="64"/>
+      <c r="X85" s="64"/>
+      <c r="Y85" s="64"/>
+      <c r="Z85" s="64"/>
+      <c r="AA85" s="64"/>
+      <c r="AB85" s="64"/>
+      <c r="AC85" s="64"/>
+      <c r="AD85" s="64"/>
+      <c r="AE85" s="64"/>
+      <c r="AF85" s="64"/>
+      <c r="AG85" s="64"/>
+      <c r="AH85" s="64"/>
+      <c r="AI85" s="64"/>
+      <c r="AJ85" s="64"/>
+      <c r="AK85" s="64"/>
+      <c r="AL85" s="64"/>
+      <c r="AM85" s="64"/>
+      <c r="AN85" s="64"/>
+      <c r="AO85" s="64"/>
+      <c r="AP85" s="64"/>
+      <c r="AQ85" s="64"/>
+      <c r="AR85" s="64"/>
+      <c r="AS85" s="64"/>
+      <c r="AT85" s="64"/>
+      <c r="AU85" s="64"/>
+      <c r="AV85" s="64"/>
+      <c r="AW85" s="64"/>
+      <c r="AX85" s="64"/>
+      <c r="AY85" s="64"/>
+      <c r="AZ85" s="64"/>
+      <c r="BA85" s="64"/>
+      <c r="BB85" s="64"/>
+      <c r="BC85" s="64"/>
     </row>
     <row r="86" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B86" s="41"/>
@@ -6464,46 +6460,46 @@
       <c r="M86" s="12"/>
       <c r="N86" s="14"/>
       <c r="O86" s="1"/>
-      <c r="P86" s="56"/>
-      <c r="Q86" s="56"/>
+      <c r="P86" s="64"/>
+      <c r="Q86" s="64"/>
       <c r="R86" s="68"/>
       <c r="S86" s="68"/>
-      <c r="T86" s="56"/>
-      <c r="U86" s="56"/>
-      <c r="V86" s="56"/>
-      <c r="W86" s="56"/>
-      <c r="X86" s="56"/>
-      <c r="Y86" s="56"/>
-      <c r="Z86" s="56"/>
-      <c r="AA86" s="56"/>
-      <c r="AB86" s="56"/>
-      <c r="AC86" s="56"/>
-      <c r="AD86" s="56"/>
-      <c r="AE86" s="56"/>
-      <c r="AF86" s="56"/>
-      <c r="AG86" s="56"/>
-      <c r="AH86" s="56"/>
-      <c r="AI86" s="56"/>
-      <c r="AJ86" s="56"/>
-      <c r="AK86" s="56"/>
-      <c r="AL86" s="56"/>
-      <c r="AM86" s="56"/>
-      <c r="AN86" s="56"/>
-      <c r="AO86" s="56"/>
-      <c r="AP86" s="56"/>
-      <c r="AQ86" s="56"/>
-      <c r="AR86" s="56"/>
-      <c r="AS86" s="56"/>
-      <c r="AT86" s="56"/>
-      <c r="AU86" s="56"/>
-      <c r="AV86" s="56"/>
-      <c r="AW86" s="56"/>
-      <c r="AX86" s="56"/>
-      <c r="AY86" s="56"/>
-      <c r="AZ86" s="56"/>
-      <c r="BA86" s="56"/>
-      <c r="BB86" s="56"/>
-      <c r="BC86" s="56"/>
+      <c r="T86" s="64"/>
+      <c r="U86" s="64"/>
+      <c r="V86" s="64"/>
+      <c r="W86" s="64"/>
+      <c r="X86" s="64"/>
+      <c r="Y86" s="64"/>
+      <c r="Z86" s="64"/>
+      <c r="AA86" s="64"/>
+      <c r="AB86" s="64"/>
+      <c r="AC86" s="64"/>
+      <c r="AD86" s="64"/>
+      <c r="AE86" s="64"/>
+      <c r="AF86" s="64"/>
+      <c r="AG86" s="64"/>
+      <c r="AH86" s="64"/>
+      <c r="AI86" s="64"/>
+      <c r="AJ86" s="64"/>
+      <c r="AK86" s="64"/>
+      <c r="AL86" s="64"/>
+      <c r="AM86" s="64"/>
+      <c r="AN86" s="64"/>
+      <c r="AO86" s="64"/>
+      <c r="AP86" s="64"/>
+      <c r="AQ86" s="64"/>
+      <c r="AR86" s="64"/>
+      <c r="AS86" s="64"/>
+      <c r="AT86" s="64"/>
+      <c r="AU86" s="64"/>
+      <c r="AV86" s="64"/>
+      <c r="AW86" s="64"/>
+      <c r="AX86" s="64"/>
+      <c r="AY86" s="64"/>
+      <c r="AZ86" s="64"/>
+      <c r="BA86" s="64"/>
+      <c r="BB86" s="64"/>
+      <c r="BC86" s="64"/>
     </row>
     <row r="87" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B87" s="44"/>
@@ -6520,46 +6516,46 @@
       <c r="M87" s="15"/>
       <c r="N87" s="17"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="56"/>
-      <c r="Q87" s="56"/>
+      <c r="P87" s="64"/>
+      <c r="Q87" s="64"/>
       <c r="R87" s="68"/>
       <c r="S87" s="68"/>
-      <c r="T87" s="56"/>
-      <c r="U87" s="56"/>
-      <c r="V87" s="56"/>
-      <c r="W87" s="56"/>
-      <c r="X87" s="56"/>
-      <c r="Y87" s="56"/>
-      <c r="Z87" s="56"/>
-      <c r="AA87" s="56"/>
-      <c r="AB87" s="56"/>
-      <c r="AC87" s="56"/>
-      <c r="AD87" s="56"/>
-      <c r="AE87" s="56"/>
-      <c r="AF87" s="56"/>
-      <c r="AG87" s="56"/>
-      <c r="AH87" s="56"/>
-      <c r="AI87" s="56"/>
-      <c r="AJ87" s="56"/>
-      <c r="AK87" s="56"/>
-      <c r="AL87" s="56"/>
-      <c r="AM87" s="56"/>
-      <c r="AN87" s="56"/>
-      <c r="AO87" s="56"/>
-      <c r="AP87" s="56"/>
-      <c r="AQ87" s="56"/>
-      <c r="AR87" s="56"/>
-      <c r="AS87" s="56"/>
-      <c r="AT87" s="56"/>
-      <c r="AU87" s="56"/>
-      <c r="AV87" s="56"/>
-      <c r="AW87" s="56"/>
-      <c r="AX87" s="56"/>
-      <c r="AY87" s="56"/>
-      <c r="AZ87" s="56"/>
-      <c r="BA87" s="56"/>
-      <c r="BB87" s="56"/>
-      <c r="BC87" s="56"/>
+      <c r="T87" s="64"/>
+      <c r="U87" s="64"/>
+      <c r="V87" s="64"/>
+      <c r="W87" s="64"/>
+      <c r="X87" s="64"/>
+      <c r="Y87" s="64"/>
+      <c r="Z87" s="64"/>
+      <c r="AA87" s="64"/>
+      <c r="AB87" s="64"/>
+      <c r="AC87" s="64"/>
+      <c r="AD87" s="64"/>
+      <c r="AE87" s="64"/>
+      <c r="AF87" s="64"/>
+      <c r="AG87" s="64"/>
+      <c r="AH87" s="64"/>
+      <c r="AI87" s="64"/>
+      <c r="AJ87" s="64"/>
+      <c r="AK87" s="64"/>
+      <c r="AL87" s="64"/>
+      <c r="AM87" s="64"/>
+      <c r="AN87" s="64"/>
+      <c r="AO87" s="64"/>
+      <c r="AP87" s="64"/>
+      <c r="AQ87" s="64"/>
+      <c r="AR87" s="64"/>
+      <c r="AS87" s="64"/>
+      <c r="AT87" s="64"/>
+      <c r="AU87" s="64"/>
+      <c r="AV87" s="64"/>
+      <c r="AW87" s="64"/>
+      <c r="AX87" s="64"/>
+      <c r="AY87" s="64"/>
+      <c r="AZ87" s="64"/>
+      <c r="BA87" s="64"/>
+      <c r="BB87" s="64"/>
+      <c r="BC87" s="64"/>
     </row>
     <row r="88" spans="2:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O88" s="1"/>
@@ -7108,68 +7104,68 @@
       <c r="M100" s="71"/>
       <c r="N100" s="71"/>
       <c r="O100" s="4"/>
-      <c r="P100" s="72" t="s">
+      <c r="P100" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="Q100" s="72"/>
-      <c r="R100" s="73" t="s">
+      <c r="Q100" s="88"/>
+      <c r="R100" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="S100" s="73"/>
-      <c r="T100" s="73" t="s">
+      <c r="S100" s="87"/>
+      <c r="T100" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="U100" s="73"/>
-      <c r="V100" s="73" t="s">
+      <c r="U100" s="87"/>
+      <c r="V100" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="W100" s="73"/>
-      <c r="X100" s="73" t="s">
+      <c r="W100" s="87"/>
+      <c r="X100" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="Y100" s="73"/>
-      <c r="Z100" s="73"/>
-      <c r="AA100" s="73"/>
-      <c r="AB100" s="73" t="s">
+      <c r="Y100" s="87"/>
+      <c r="Z100" s="87"/>
+      <c r="AA100" s="87"/>
+      <c r="AB100" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AC100" s="73"/>
-      <c r="AD100" s="73"/>
-      <c r="AE100" s="73"/>
-      <c r="AF100" s="73"/>
-      <c r="AG100" s="73" t="s">
+      <c r="AC100" s="87"/>
+      <c r="AD100" s="87"/>
+      <c r="AE100" s="87"/>
+      <c r="AF100" s="87"/>
+      <c r="AG100" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="AH100" s="73"/>
-      <c r="AI100" s="73"/>
-      <c r="AJ100" s="73"/>
-      <c r="AK100" s="73"/>
-      <c r="AL100" s="73"/>
-      <c r="AM100" s="73" t="s">
+      <c r="AH100" s="87"/>
+      <c r="AI100" s="87"/>
+      <c r="AJ100" s="87"/>
+      <c r="AK100" s="87"/>
+      <c r="AL100" s="87"/>
+      <c r="AM100" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="AN100" s="73"/>
-      <c r="AO100" s="73" t="s">
+      <c r="AN100" s="87"/>
+      <c r="AO100" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="AP100" s="73"/>
-      <c r="AQ100" s="73"/>
-      <c r="AR100" s="73"/>
-      <c r="AS100" s="73"/>
-      <c r="AT100" s="73"/>
-      <c r="AU100" s="73" t="s">
+      <c r="AP100" s="87"/>
+      <c r="AQ100" s="87"/>
+      <c r="AR100" s="87"/>
+      <c r="AS100" s="87"/>
+      <c r="AT100" s="87"/>
+      <c r="AU100" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AV100" s="73"/>
-      <c r="AW100" s="73"/>
-      <c r="AX100" s="73"/>
-      <c r="AY100" s="73"/>
-      <c r="AZ100" s="73"/>
-      <c r="BA100" s="73" t="s">
+      <c r="AV100" s="87"/>
+      <c r="AW100" s="87"/>
+      <c r="AX100" s="87"/>
+      <c r="AY100" s="87"/>
+      <c r="AZ100" s="87"/>
+      <c r="BA100" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="BB100" s="73"/>
-      <c r="BC100" s="73"/>
+      <c r="BB100" s="87"/>
+      <c r="BC100" s="87"/>
     </row>
     <row r="101" spans="6:55" x14ac:dyDescent="0.25">
       <c r="F101" s="71"/>
@@ -7182,46 +7178,46 @@
       <c r="M101" s="71"/>
       <c r="N101" s="71"/>
       <c r="O101" s="4"/>
-      <c r="P101" s="72"/>
-      <c r="Q101" s="72"/>
-      <c r="R101" s="73"/>
-      <c r="S101" s="73"/>
-      <c r="T101" s="73"/>
-      <c r="U101" s="73"/>
-      <c r="V101" s="73"/>
-      <c r="W101" s="73"/>
-      <c r="X101" s="73"/>
-      <c r="Y101" s="73"/>
-      <c r="Z101" s="73"/>
-      <c r="AA101" s="73"/>
-      <c r="AB101" s="73"/>
-      <c r="AC101" s="73"/>
-      <c r="AD101" s="73"/>
-      <c r="AE101" s="73"/>
-      <c r="AF101" s="73"/>
-      <c r="AG101" s="73"/>
-      <c r="AH101" s="73"/>
-      <c r="AI101" s="73"/>
-      <c r="AJ101" s="73"/>
-      <c r="AK101" s="73"/>
-      <c r="AL101" s="73"/>
-      <c r="AM101" s="73"/>
-      <c r="AN101" s="73"/>
-      <c r="AO101" s="73"/>
-      <c r="AP101" s="73"/>
-      <c r="AQ101" s="73"/>
-      <c r="AR101" s="73"/>
-      <c r="AS101" s="73"/>
-      <c r="AT101" s="73"/>
-      <c r="AU101" s="73"/>
-      <c r="AV101" s="73"/>
-      <c r="AW101" s="73"/>
-      <c r="AX101" s="73"/>
-      <c r="AY101" s="73"/>
-      <c r="AZ101" s="73"/>
-      <c r="BA101" s="73"/>
-      <c r="BB101" s="73"/>
-      <c r="BC101" s="73"/>
+      <c r="P101" s="88"/>
+      <c r="Q101" s="88"/>
+      <c r="R101" s="87"/>
+      <c r="S101" s="87"/>
+      <c r="T101" s="87"/>
+      <c r="U101" s="87"/>
+      <c r="V101" s="87"/>
+      <c r="W101" s="87"/>
+      <c r="X101" s="87"/>
+      <c r="Y101" s="87"/>
+      <c r="Z101" s="87"/>
+      <c r="AA101" s="87"/>
+      <c r="AB101" s="87"/>
+      <c r="AC101" s="87"/>
+      <c r="AD101" s="87"/>
+      <c r="AE101" s="87"/>
+      <c r="AF101" s="87"/>
+      <c r="AG101" s="87"/>
+      <c r="AH101" s="87"/>
+      <c r="AI101" s="87"/>
+      <c r="AJ101" s="87"/>
+      <c r="AK101" s="87"/>
+      <c r="AL101" s="87"/>
+      <c r="AM101" s="87"/>
+      <c r="AN101" s="87"/>
+      <c r="AO101" s="87"/>
+      <c r="AP101" s="87"/>
+      <c r="AQ101" s="87"/>
+      <c r="AR101" s="87"/>
+      <c r="AS101" s="87"/>
+      <c r="AT101" s="87"/>
+      <c r="AU101" s="87"/>
+      <c r="AV101" s="87"/>
+      <c r="AW101" s="87"/>
+      <c r="AX101" s="87"/>
+      <c r="AY101" s="87"/>
+      <c r="AZ101" s="87"/>
+      <c r="BA101" s="87"/>
+      <c r="BB101" s="87"/>
+      <c r="BC101" s="87"/>
     </row>
     <row r="102" spans="6:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F102" s="50" t="s">
@@ -7234,7 +7230,7 @@
         <v>19</v>
       </c>
       <c r="K102" s="52"/>
-      <c r="L102" s="98" t="s">
+      <c r="L102" s="72" t="s">
         <v>20</v>
       </c>
       <c r="M102" s="50" t="s">
@@ -7310,7 +7306,7 @@
       <c r="I103" s="55"/>
       <c r="J103" s="65"/>
       <c r="K103" s="67"/>
-      <c r="L103" s="99"/>
+      <c r="L103" s="73"/>
       <c r="M103" s="65"/>
       <c r="N103" s="67"/>
       <c r="O103" s="4"/>
@@ -7366,7 +7362,7 @@
       <c r="I104" s="52"/>
       <c r="J104" s="65"/>
       <c r="K104" s="67"/>
-      <c r="L104" s="99"/>
+      <c r="L104" s="73"/>
       <c r="M104" s="65"/>
       <c r="N104" s="67"/>
       <c r="O104" s="4"/>
@@ -7418,7 +7414,7 @@
       <c r="I105" s="55"/>
       <c r="J105" s="53"/>
       <c r="K105" s="55"/>
-      <c r="L105" s="100"/>
+      <c r="L105" s="74"/>
       <c r="M105" s="53"/>
       <c r="N105" s="55"/>
       <c r="O105" s="4"/>
@@ -7479,10 +7475,10 @@
       <c r="L106" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="M106" s="56" t="s">
+      <c r="M106" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="N106" s="56"/>
+      <c r="N106" s="64"/>
       <c r="O106" s="6"/>
       <c r="P106" s="12"/>
       <c r="Q106" s="14"/>
@@ -7533,8 +7529,8 @@
       <c r="J107" s="12"/>
       <c r="K107" s="14"/>
       <c r="L107" s="48"/>
-      <c r="M107" s="56"/>
-      <c r="N107" s="56"/>
+      <c r="M107" s="64"/>
+      <c r="N107" s="64"/>
       <c r="O107" s="6"/>
       <c r="P107" s="12"/>
       <c r="Q107" s="14"/>
@@ -7585,8 +7581,8 @@
       <c r="J108" s="12"/>
       <c r="K108" s="14"/>
       <c r="L108" s="48"/>
-      <c r="M108" s="56"/>
-      <c r="N108" s="56"/>
+      <c r="M108" s="64"/>
+      <c r="N108" s="64"/>
       <c r="O108" s="1"/>
       <c r="P108" s="12"/>
       <c r="Q108" s="14"/>
@@ -7637,8 +7633,8 @@
       <c r="J109" s="12"/>
       <c r="K109" s="14"/>
       <c r="L109" s="48"/>
-      <c r="M109" s="56"/>
-      <c r="N109" s="56"/>
+      <c r="M109" s="64"/>
+      <c r="N109" s="64"/>
       <c r="O109" s="1"/>
       <c r="P109" s="12"/>
       <c r="Q109" s="14"/>
@@ -7689,8 +7685,8 @@
       <c r="J110" s="12"/>
       <c r="K110" s="14"/>
       <c r="L110" s="48"/>
-      <c r="M110" s="56"/>
-      <c r="N110" s="56"/>
+      <c r="M110" s="64"/>
+      <c r="N110" s="64"/>
       <c r="O110" s="1"/>
       <c r="P110" s="12"/>
       <c r="Q110" s="14"/>
@@ -7741,8 +7737,8 @@
       <c r="J111" s="12"/>
       <c r="K111" s="14"/>
       <c r="L111" s="48"/>
-      <c r="M111" s="56"/>
-      <c r="N111" s="56"/>
+      <c r="M111" s="64"/>
+      <c r="N111" s="64"/>
       <c r="O111" s="1"/>
       <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
@@ -7801,8 +7797,8 @@
       <c r="L112" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="M112" s="56"/>
-      <c r="N112" s="56"/>
+      <c r="M112" s="64"/>
+      <c r="N112" s="64"/>
       <c r="O112" s="1"/>
       <c r="P112" s="13"/>
       <c r="Q112" s="13"/>
@@ -7853,8 +7849,8 @@
       <c r="J113" s="12"/>
       <c r="K113" s="14"/>
       <c r="L113" s="48"/>
-      <c r="M113" s="56"/>
-      <c r="N113" s="56"/>
+      <c r="M113" s="64"/>
+      <c r="N113" s="64"/>
       <c r="O113" s="1"/>
       <c r="P113" s="13"/>
       <c r="Q113" s="13"/>
@@ -7905,8 +7901,8 @@
       <c r="J114" s="12"/>
       <c r="K114" s="14"/>
       <c r="L114" s="48"/>
-      <c r="M114" s="56"/>
-      <c r="N114" s="56"/>
+      <c r="M114" s="64"/>
+      <c r="N114" s="64"/>
       <c r="O114" s="1"/>
       <c r="P114" s="13"/>
       <c r="Q114" s="13"/>
@@ -7957,8 +7953,8 @@
       <c r="J115" s="12"/>
       <c r="K115" s="14"/>
       <c r="L115" s="48"/>
-      <c r="M115" s="56"/>
-      <c r="N115" s="56"/>
+      <c r="M115" s="64"/>
+      <c r="N115" s="64"/>
       <c r="O115" s="1"/>
       <c r="P115" s="13"/>
       <c r="Q115" s="13"/>
@@ -8009,8 +8005,8 @@
       <c r="J116" s="12"/>
       <c r="K116" s="14"/>
       <c r="L116" s="48"/>
-      <c r="M116" s="56"/>
-      <c r="N116" s="56"/>
+      <c r="M116" s="64"/>
+      <c r="N116" s="64"/>
       <c r="O116" s="4"/>
       <c r="P116" s="13"/>
       <c r="Q116" s="13"/>
@@ -8061,8 +8057,8 @@
       <c r="J117" s="15"/>
       <c r="K117" s="17"/>
       <c r="L117" s="49"/>
-      <c r="M117" s="56"/>
-      <c r="N117" s="56"/>
+      <c r="M117" s="64"/>
+      <c r="N117" s="64"/>
       <c r="O117" s="4"/>
       <c r="P117" s="13"/>
       <c r="Q117" s="13"/>
@@ -8844,68 +8840,68 @@
       <c r="M136" s="51"/>
       <c r="N136" s="52"/>
       <c r="O136" s="6"/>
-      <c r="P136" s="74" t="s">
+      <c r="P136" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="Q136" s="74"/>
-      <c r="R136" s="73" t="s">
+      <c r="Q136" s="89"/>
+      <c r="R136" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="S136" s="73"/>
-      <c r="T136" s="73" t="s">
+      <c r="S136" s="87"/>
+      <c r="T136" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="U136" s="73"/>
-      <c r="V136" s="73" t="s">
+      <c r="U136" s="87"/>
+      <c r="V136" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="W136" s="73"/>
-      <c r="X136" s="73" t="s">
+      <c r="W136" s="87"/>
+      <c r="X136" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="Y136" s="73"/>
-      <c r="Z136" s="73"/>
-      <c r="AA136" s="73"/>
-      <c r="AB136" s="73" t="s">
+      <c r="Y136" s="87"/>
+      <c r="Z136" s="87"/>
+      <c r="AA136" s="87"/>
+      <c r="AB136" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AC136" s="73"/>
-      <c r="AD136" s="73"/>
-      <c r="AE136" s="73"/>
-      <c r="AF136" s="73"/>
-      <c r="AG136" s="73" t="s">
+      <c r="AC136" s="87"/>
+      <c r="AD136" s="87"/>
+      <c r="AE136" s="87"/>
+      <c r="AF136" s="87"/>
+      <c r="AG136" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="AH136" s="73"/>
-      <c r="AI136" s="73"/>
-      <c r="AJ136" s="73"/>
-      <c r="AK136" s="73"/>
-      <c r="AL136" s="73"/>
-      <c r="AM136" s="73" t="s">
+      <c r="AH136" s="87"/>
+      <c r="AI136" s="87"/>
+      <c r="AJ136" s="87"/>
+      <c r="AK136" s="87"/>
+      <c r="AL136" s="87"/>
+      <c r="AM136" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="AN136" s="73"/>
-      <c r="AO136" s="73" t="s">
+      <c r="AN136" s="87"/>
+      <c r="AO136" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="AP136" s="73"/>
-      <c r="AQ136" s="73"/>
-      <c r="AR136" s="73"/>
-      <c r="AS136" s="73"/>
-      <c r="AT136" s="73"/>
-      <c r="AU136" s="73" t="s">
+      <c r="AP136" s="87"/>
+      <c r="AQ136" s="87"/>
+      <c r="AR136" s="87"/>
+      <c r="AS136" s="87"/>
+      <c r="AT136" s="87"/>
+      <c r="AU136" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AV136" s="73"/>
-      <c r="AW136" s="73"/>
-      <c r="AX136" s="73"/>
-      <c r="AY136" s="73"/>
-      <c r="AZ136" s="73"/>
-      <c r="BA136" s="73" t="s">
+      <c r="AV136" s="87"/>
+      <c r="AW136" s="87"/>
+      <c r="AX136" s="87"/>
+      <c r="AY136" s="87"/>
+      <c r="AZ136" s="87"/>
+      <c r="BA136" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="BB136" s="73"/>
-      <c r="BC136" s="73"/>
+      <c r="BB136" s="87"/>
+      <c r="BC136" s="87"/>
     </row>
     <row r="137" spans="6:55" x14ac:dyDescent="0.25">
       <c r="F137" s="53"/>
@@ -8918,46 +8914,46 @@
       <c r="M137" s="54"/>
       <c r="N137" s="55"/>
       <c r="O137" s="6"/>
-      <c r="P137" s="74"/>
-      <c r="Q137" s="74"/>
-      <c r="R137" s="73"/>
-      <c r="S137" s="73"/>
-      <c r="T137" s="73"/>
-      <c r="U137" s="73"/>
-      <c r="V137" s="73"/>
-      <c r="W137" s="73"/>
-      <c r="X137" s="73"/>
-      <c r="Y137" s="73"/>
-      <c r="Z137" s="73"/>
-      <c r="AA137" s="73"/>
-      <c r="AB137" s="73"/>
-      <c r="AC137" s="73"/>
-      <c r="AD137" s="73"/>
-      <c r="AE137" s="73"/>
-      <c r="AF137" s="73"/>
-      <c r="AG137" s="73"/>
-      <c r="AH137" s="73"/>
-      <c r="AI137" s="73"/>
-      <c r="AJ137" s="73"/>
-      <c r="AK137" s="73"/>
-      <c r="AL137" s="73"/>
-      <c r="AM137" s="73"/>
-      <c r="AN137" s="73"/>
-      <c r="AO137" s="73"/>
-      <c r="AP137" s="73"/>
-      <c r="AQ137" s="73"/>
-      <c r="AR137" s="73"/>
-      <c r="AS137" s="73"/>
-      <c r="AT137" s="73"/>
-      <c r="AU137" s="73"/>
-      <c r="AV137" s="73"/>
-      <c r="AW137" s="73"/>
-      <c r="AX137" s="73"/>
-      <c r="AY137" s="73"/>
-      <c r="AZ137" s="73"/>
-      <c r="BA137" s="73"/>
-      <c r="BB137" s="73"/>
-      <c r="BC137" s="73"/>
+      <c r="P137" s="89"/>
+      <c r="Q137" s="89"/>
+      <c r="R137" s="87"/>
+      <c r="S137" s="87"/>
+      <c r="T137" s="87"/>
+      <c r="U137" s="87"/>
+      <c r="V137" s="87"/>
+      <c r="W137" s="87"/>
+      <c r="X137" s="87"/>
+      <c r="Y137" s="87"/>
+      <c r="Z137" s="87"/>
+      <c r="AA137" s="87"/>
+      <c r="AB137" s="87"/>
+      <c r="AC137" s="87"/>
+      <c r="AD137" s="87"/>
+      <c r="AE137" s="87"/>
+      <c r="AF137" s="87"/>
+      <c r="AG137" s="87"/>
+      <c r="AH137" s="87"/>
+      <c r="AI137" s="87"/>
+      <c r="AJ137" s="87"/>
+      <c r="AK137" s="87"/>
+      <c r="AL137" s="87"/>
+      <c r="AM137" s="87"/>
+      <c r="AN137" s="87"/>
+      <c r="AO137" s="87"/>
+      <c r="AP137" s="87"/>
+      <c r="AQ137" s="87"/>
+      <c r="AR137" s="87"/>
+      <c r="AS137" s="87"/>
+      <c r="AT137" s="87"/>
+      <c r="AU137" s="87"/>
+      <c r="AV137" s="87"/>
+      <c r="AW137" s="87"/>
+      <c r="AX137" s="87"/>
+      <c r="AY137" s="87"/>
+      <c r="AZ137" s="87"/>
+      <c r="BA137" s="87"/>
+      <c r="BB137" s="87"/>
+      <c r="BC137" s="87"/>
     </row>
     <row r="138" spans="6:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F138" s="9" t="s">
@@ -8978,26 +8974,26 @@
       <c r="M138" s="10"/>
       <c r="N138" s="11"/>
       <c r="O138" s="1"/>
-      <c r="P138" s="56" t="s">
+      <c r="P138" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="Q138" s="56"/>
+      <c r="Q138" s="64"/>
       <c r="R138" s="32" t="s">
         <v>101</v>
       </c>
       <c r="S138" s="34"/>
-      <c r="T138" s="56" t="s">
+      <c r="T138" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="U138" s="56"/>
+      <c r="U138" s="64"/>
       <c r="V138" s="9"/>
       <c r="W138" s="11"/>
-      <c r="X138" s="56" t="s">
+      <c r="X138" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="Y138" s="56"/>
-      <c r="Z138" s="56"/>
-      <c r="AA138" s="56"/>
+      <c r="Y138" s="64"/>
+      <c r="Z138" s="64"/>
+      <c r="AA138" s="64"/>
       <c r="AB138" s="9" t="s">
         <v>96</v>
       </c>
@@ -9011,8 +9007,8 @@
       <c r="AJ138" s="10"/>
       <c r="AK138" s="10"/>
       <c r="AL138" s="11"/>
-      <c r="AM138" s="56"/>
-      <c r="AN138" s="56"/>
+      <c r="AM138" s="64"/>
+      <c r="AN138" s="64"/>
       <c r="AO138" s="9" t="s">
         <v>97</v>
       </c>
@@ -9046,18 +9042,18 @@
       <c r="M139" s="13"/>
       <c r="N139" s="14"/>
       <c r="O139" s="1"/>
-      <c r="P139" s="56"/>
-      <c r="Q139" s="56"/>
-      <c r="R139" s="75"/>
-      <c r="S139" s="76"/>
-      <c r="T139" s="56"/>
-      <c r="U139" s="56"/>
+      <c r="P139" s="64"/>
+      <c r="Q139" s="64"/>
+      <c r="R139" s="90"/>
+      <c r="S139" s="91"/>
+      <c r="T139" s="64"/>
+      <c r="U139" s="64"/>
       <c r="V139" s="12"/>
       <c r="W139" s="14"/>
-      <c r="X139" s="56"/>
-      <c r="Y139" s="56"/>
-      <c r="Z139" s="56"/>
-      <c r="AA139" s="56"/>
+      <c r="X139" s="64"/>
+      <c r="Y139" s="64"/>
+      <c r="Z139" s="64"/>
+      <c r="AA139" s="64"/>
       <c r="AB139" s="12"/>
       <c r="AC139" s="13"/>
       <c r="AD139" s="13"/>
@@ -9069,8 +9065,8 @@
       <c r="AJ139" s="13"/>
       <c r="AK139" s="13"/>
       <c r="AL139" s="14"/>
-      <c r="AM139" s="56"/>
-      <c r="AN139" s="56"/>
+      <c r="AM139" s="64"/>
+      <c r="AN139" s="64"/>
       <c r="AO139" s="12"/>
       <c r="AP139" s="13"/>
       <c r="AQ139" s="13"/>
@@ -9098,18 +9094,18 @@
       <c r="M140" s="13"/>
       <c r="N140" s="14"/>
       <c r="O140" s="1"/>
-      <c r="P140" s="56"/>
-      <c r="Q140" s="56"/>
-      <c r="R140" s="75"/>
-      <c r="S140" s="76"/>
-      <c r="T140" s="56"/>
-      <c r="U140" s="56"/>
+      <c r="P140" s="64"/>
+      <c r="Q140" s="64"/>
+      <c r="R140" s="90"/>
+      <c r="S140" s="91"/>
+      <c r="T140" s="64"/>
+      <c r="U140" s="64"/>
       <c r="V140" s="12"/>
       <c r="W140" s="14"/>
-      <c r="X140" s="56"/>
-      <c r="Y140" s="56"/>
-      <c r="Z140" s="56"/>
-      <c r="AA140" s="56"/>
+      <c r="X140" s="64"/>
+      <c r="Y140" s="64"/>
+      <c r="Z140" s="64"/>
+      <c r="AA140" s="64"/>
       <c r="AB140" s="12"/>
       <c r="AC140" s="13"/>
       <c r="AD140" s="13"/>
@@ -9121,8 +9117,8 @@
       <c r="AJ140" s="13"/>
       <c r="AK140" s="13"/>
       <c r="AL140" s="14"/>
-      <c r="AM140" s="56"/>
-      <c r="AN140" s="56"/>
+      <c r="AM140" s="64"/>
+      <c r="AN140" s="64"/>
       <c r="AO140" s="12"/>
       <c r="AP140" s="13"/>
       <c r="AQ140" s="13"/>
@@ -9150,18 +9146,18 @@
       <c r="M141" s="16"/>
       <c r="N141" s="17"/>
       <c r="O141" s="1"/>
-      <c r="P141" s="56"/>
-      <c r="Q141" s="56"/>
-      <c r="R141" s="75"/>
-      <c r="S141" s="76"/>
-      <c r="T141" s="56"/>
-      <c r="U141" s="56"/>
+      <c r="P141" s="64"/>
+      <c r="Q141" s="64"/>
+      <c r="R141" s="90"/>
+      <c r="S141" s="91"/>
+      <c r="T141" s="64"/>
+      <c r="U141" s="64"/>
       <c r="V141" s="12"/>
       <c r="W141" s="14"/>
-      <c r="X141" s="56"/>
-      <c r="Y141" s="56"/>
-      <c r="Z141" s="56"/>
-      <c r="AA141" s="56"/>
+      <c r="X141" s="64"/>
+      <c r="Y141" s="64"/>
+      <c r="Z141" s="64"/>
+      <c r="AA141" s="64"/>
       <c r="AB141" s="12"/>
       <c r="AC141" s="13"/>
       <c r="AD141" s="13"/>
@@ -9173,8 +9169,8 @@
       <c r="AJ141" s="13"/>
       <c r="AK141" s="13"/>
       <c r="AL141" s="14"/>
-      <c r="AM141" s="56"/>
-      <c r="AN141" s="56"/>
+      <c r="AM141" s="64"/>
+      <c r="AN141" s="64"/>
       <c r="AO141" s="12"/>
       <c r="AP141" s="13"/>
       <c r="AQ141" s="13"/>
@@ -9210,18 +9206,18 @@
       <c r="M142" s="10"/>
       <c r="N142" s="11"/>
       <c r="O142" s="1"/>
-      <c r="P142" s="56"/>
-      <c r="Q142" s="56"/>
-      <c r="R142" s="75"/>
-      <c r="S142" s="76"/>
-      <c r="T142" s="56"/>
-      <c r="U142" s="56"/>
+      <c r="P142" s="64"/>
+      <c r="Q142" s="64"/>
+      <c r="R142" s="90"/>
+      <c r="S142" s="91"/>
+      <c r="T142" s="64"/>
+      <c r="U142" s="64"/>
       <c r="V142" s="12"/>
       <c r="W142" s="14"/>
-      <c r="X142" s="56"/>
-      <c r="Y142" s="56"/>
-      <c r="Z142" s="56"/>
-      <c r="AA142" s="56"/>
+      <c r="X142" s="64"/>
+      <c r="Y142" s="64"/>
+      <c r="Z142" s="64"/>
+      <c r="AA142" s="64"/>
       <c r="AB142" s="12"/>
       <c r="AC142" s="13"/>
       <c r="AD142" s="13"/>
@@ -9233,8 +9229,8 @@
       <c r="AJ142" s="13"/>
       <c r="AK142" s="13"/>
       <c r="AL142" s="14"/>
-      <c r="AM142" s="56"/>
-      <c r="AN142" s="56"/>
+      <c r="AM142" s="64"/>
+      <c r="AN142" s="64"/>
       <c r="AO142" s="12"/>
       <c r="AP142" s="13"/>
       <c r="AQ142" s="13"/>
@@ -9262,18 +9258,18 @@
       <c r="M143" s="13"/>
       <c r="N143" s="14"/>
       <c r="O143" s="1"/>
-      <c r="P143" s="56"/>
-      <c r="Q143" s="56"/>
-      <c r="R143" s="75"/>
-      <c r="S143" s="76"/>
-      <c r="T143" s="56"/>
-      <c r="U143" s="56"/>
+      <c r="P143" s="64"/>
+      <c r="Q143" s="64"/>
+      <c r="R143" s="90"/>
+      <c r="S143" s="91"/>
+      <c r="T143" s="64"/>
+      <c r="U143" s="64"/>
       <c r="V143" s="12"/>
       <c r="W143" s="14"/>
-      <c r="X143" s="56"/>
-      <c r="Y143" s="56"/>
-      <c r="Z143" s="56"/>
-      <c r="AA143" s="56"/>
+      <c r="X143" s="64"/>
+      <c r="Y143" s="64"/>
+      <c r="Z143" s="64"/>
+      <c r="AA143" s="64"/>
       <c r="AB143" s="12"/>
       <c r="AC143" s="13"/>
       <c r="AD143" s="13"/>
@@ -9285,8 +9281,8 @@
       <c r="AJ143" s="13"/>
       <c r="AK143" s="13"/>
       <c r="AL143" s="14"/>
-      <c r="AM143" s="56"/>
-      <c r="AN143" s="56"/>
+      <c r="AM143" s="64"/>
+      <c r="AN143" s="64"/>
       <c r="AO143" s="12"/>
       <c r="AP143" s="13"/>
       <c r="AQ143" s="13"/>
@@ -9314,18 +9310,18 @@
       <c r="M144" s="13"/>
       <c r="N144" s="14"/>
       <c r="O144" s="1"/>
-      <c r="P144" s="56"/>
-      <c r="Q144" s="56"/>
-      <c r="R144" s="75"/>
-      <c r="S144" s="76"/>
-      <c r="T144" s="56"/>
-      <c r="U144" s="56"/>
+      <c r="P144" s="64"/>
+      <c r="Q144" s="64"/>
+      <c r="R144" s="90"/>
+      <c r="S144" s="91"/>
+      <c r="T144" s="64"/>
+      <c r="U144" s="64"/>
       <c r="V144" s="12"/>
       <c r="W144" s="14"/>
-      <c r="X144" s="56"/>
-      <c r="Y144" s="56"/>
-      <c r="Z144" s="56"/>
-      <c r="AA144" s="56"/>
+      <c r="X144" s="64"/>
+      <c r="Y144" s="64"/>
+      <c r="Z144" s="64"/>
+      <c r="AA144" s="64"/>
       <c r="AB144" s="12"/>
       <c r="AC144" s="13"/>
       <c r="AD144" s="13"/>
@@ -9337,8 +9333,8 @@
       <c r="AJ144" s="13"/>
       <c r="AK144" s="13"/>
       <c r="AL144" s="14"/>
-      <c r="AM144" s="56"/>
-      <c r="AN144" s="56"/>
+      <c r="AM144" s="64"/>
+      <c r="AN144" s="64"/>
       <c r="AO144" s="12"/>
       <c r="AP144" s="13"/>
       <c r="AQ144" s="13"/>
@@ -9366,18 +9362,18 @@
       <c r="M145" s="16"/>
       <c r="N145" s="17"/>
       <c r="O145" s="1"/>
-      <c r="P145" s="56"/>
-      <c r="Q145" s="56"/>
-      <c r="R145" s="75"/>
-      <c r="S145" s="76"/>
-      <c r="T145" s="56"/>
-      <c r="U145" s="56"/>
+      <c r="P145" s="64"/>
+      <c r="Q145" s="64"/>
+      <c r="R145" s="90"/>
+      <c r="S145" s="91"/>
+      <c r="T145" s="64"/>
+      <c r="U145" s="64"/>
       <c r="V145" s="12"/>
       <c r="W145" s="14"/>
-      <c r="X145" s="56"/>
-      <c r="Y145" s="56"/>
-      <c r="Z145" s="56"/>
-      <c r="AA145" s="56"/>
+      <c r="X145" s="64"/>
+      <c r="Y145" s="64"/>
+      <c r="Z145" s="64"/>
+      <c r="AA145" s="64"/>
       <c r="AB145" s="12"/>
       <c r="AC145" s="13"/>
       <c r="AD145" s="13"/>
@@ -9389,8 +9385,8 @@
       <c r="AJ145" s="13"/>
       <c r="AK145" s="13"/>
       <c r="AL145" s="14"/>
-      <c r="AM145" s="56"/>
-      <c r="AN145" s="56"/>
+      <c r="AM145" s="64"/>
+      <c r="AN145" s="64"/>
       <c r="AO145" s="12"/>
       <c r="AP145" s="13"/>
       <c r="AQ145" s="13"/>
@@ -9419,25 +9415,25 @@
       <c r="J146" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K146" s="56" t="s">
+      <c r="K146" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="L146" s="56"/>
-      <c r="M146" s="56"/>
-      <c r="N146" s="56"/>
+      <c r="L146" s="64"/>
+      <c r="M146" s="64"/>
+      <c r="N146" s="64"/>
       <c r="O146" s="1"/>
-      <c r="P146" s="56"/>
-      <c r="Q146" s="56"/>
-      <c r="R146" s="75"/>
-      <c r="S146" s="76"/>
-      <c r="T146" s="56"/>
-      <c r="U146" s="56"/>
+      <c r="P146" s="64"/>
+      <c r="Q146" s="64"/>
+      <c r="R146" s="90"/>
+      <c r="S146" s="91"/>
+      <c r="T146" s="64"/>
+      <c r="U146" s="64"/>
       <c r="V146" s="12"/>
       <c r="W146" s="14"/>
-      <c r="X146" s="56"/>
-      <c r="Y146" s="56"/>
-      <c r="Z146" s="56"/>
-      <c r="AA146" s="56"/>
+      <c r="X146" s="64"/>
+      <c r="Y146" s="64"/>
+      <c r="Z146" s="64"/>
+      <c r="AA146" s="64"/>
       <c r="AB146" s="12"/>
       <c r="AC146" s="13"/>
       <c r="AD146" s="13"/>
@@ -9449,8 +9445,8 @@
       <c r="AJ146" s="13"/>
       <c r="AK146" s="13"/>
       <c r="AL146" s="14"/>
-      <c r="AM146" s="56"/>
-      <c r="AN146" s="56"/>
+      <c r="AM146" s="64"/>
+      <c r="AN146" s="64"/>
       <c r="AO146" s="12"/>
       <c r="AP146" s="13"/>
       <c r="AQ146" s="13"/>
@@ -9473,23 +9469,23 @@
       <c r="H147" s="12"/>
       <c r="I147" s="14"/>
       <c r="J147" s="48"/>
-      <c r="K147" s="56"/>
-      <c r="L147" s="56"/>
-      <c r="M147" s="56"/>
-      <c r="N147" s="56"/>
+      <c r="K147" s="64"/>
+      <c r="L147" s="64"/>
+      <c r="M147" s="64"/>
+      <c r="N147" s="64"/>
       <c r="O147" s="1"/>
-      <c r="P147" s="56"/>
-      <c r="Q147" s="56"/>
-      <c r="R147" s="75"/>
-      <c r="S147" s="76"/>
-      <c r="T147" s="56"/>
-      <c r="U147" s="56"/>
+      <c r="P147" s="64"/>
+      <c r="Q147" s="64"/>
+      <c r="R147" s="90"/>
+      <c r="S147" s="91"/>
+      <c r="T147" s="64"/>
+      <c r="U147" s="64"/>
       <c r="V147" s="12"/>
       <c r="W147" s="14"/>
-      <c r="X147" s="56"/>
-      <c r="Y147" s="56"/>
-      <c r="Z147" s="56"/>
-      <c r="AA147" s="56"/>
+      <c r="X147" s="64"/>
+      <c r="Y147" s="64"/>
+      <c r="Z147" s="64"/>
+      <c r="AA147" s="64"/>
       <c r="AB147" s="12"/>
       <c r="AC147" s="13"/>
       <c r="AD147" s="13"/>
@@ -9501,8 +9497,8 @@
       <c r="AJ147" s="13"/>
       <c r="AK147" s="13"/>
       <c r="AL147" s="14"/>
-      <c r="AM147" s="56"/>
-      <c r="AN147" s="56"/>
+      <c r="AM147" s="64"/>
+      <c r="AN147" s="64"/>
       <c r="AO147" s="12"/>
       <c r="AP147" s="13"/>
       <c r="AQ147" s="13"/>
@@ -9525,23 +9521,23 @@
       <c r="H148" s="12"/>
       <c r="I148" s="14"/>
       <c r="J148" s="48"/>
-      <c r="K148" s="56"/>
-      <c r="L148" s="56"/>
-      <c r="M148" s="56"/>
-      <c r="N148" s="56"/>
+      <c r="K148" s="64"/>
+      <c r="L148" s="64"/>
+      <c r="M148" s="64"/>
+      <c r="N148" s="64"/>
       <c r="O148" s="1"/>
-      <c r="P148" s="56"/>
-      <c r="Q148" s="56"/>
-      <c r="R148" s="75"/>
-      <c r="S148" s="76"/>
-      <c r="T148" s="56"/>
-      <c r="U148" s="56"/>
+      <c r="P148" s="64"/>
+      <c r="Q148" s="64"/>
+      <c r="R148" s="90"/>
+      <c r="S148" s="91"/>
+      <c r="T148" s="64"/>
+      <c r="U148" s="64"/>
       <c r="V148" s="12"/>
       <c r="W148" s="14"/>
-      <c r="X148" s="56"/>
-      <c r="Y148" s="56"/>
-      <c r="Z148" s="56"/>
-      <c r="AA148" s="56"/>
+      <c r="X148" s="64"/>
+      <c r="Y148" s="64"/>
+      <c r="Z148" s="64"/>
+      <c r="AA148" s="64"/>
       <c r="AB148" s="12"/>
       <c r="AC148" s="13"/>
       <c r="AD148" s="13"/>
@@ -9553,8 +9549,8 @@
       <c r="AJ148" s="13"/>
       <c r="AK148" s="13"/>
       <c r="AL148" s="14"/>
-      <c r="AM148" s="56"/>
-      <c r="AN148" s="56"/>
+      <c r="AM148" s="64"/>
+      <c r="AN148" s="64"/>
       <c r="AO148" s="12"/>
       <c r="AP148" s="13"/>
       <c r="AQ148" s="13"/>
@@ -9577,23 +9573,23 @@
       <c r="H149" s="15"/>
       <c r="I149" s="17"/>
       <c r="J149" s="49"/>
-      <c r="K149" s="56"/>
-      <c r="L149" s="56"/>
-      <c r="M149" s="56"/>
-      <c r="N149" s="56"/>
+      <c r="K149" s="64"/>
+      <c r="L149" s="64"/>
+      <c r="M149" s="64"/>
+      <c r="N149" s="64"/>
       <c r="O149" s="1"/>
-      <c r="P149" s="56"/>
-      <c r="Q149" s="56"/>
-      <c r="R149" s="75"/>
-      <c r="S149" s="76"/>
-      <c r="T149" s="56"/>
-      <c r="U149" s="56"/>
+      <c r="P149" s="64"/>
+      <c r="Q149" s="64"/>
+      <c r="R149" s="90"/>
+      <c r="S149" s="91"/>
+      <c r="T149" s="64"/>
+      <c r="U149" s="64"/>
       <c r="V149" s="12"/>
       <c r="W149" s="14"/>
-      <c r="X149" s="56"/>
-      <c r="Y149" s="56"/>
-      <c r="Z149" s="56"/>
-      <c r="AA149" s="56"/>
+      <c r="X149" s="64"/>
+      <c r="Y149" s="64"/>
+      <c r="Z149" s="64"/>
+      <c r="AA149" s="64"/>
       <c r="AB149" s="12"/>
       <c r="AC149" s="13"/>
       <c r="AD149" s="13"/>
@@ -9605,8 +9601,8 @@
       <c r="AJ149" s="13"/>
       <c r="AK149" s="13"/>
       <c r="AL149" s="14"/>
-      <c r="AM149" s="56"/>
-      <c r="AN149" s="56"/>
+      <c r="AM149" s="64"/>
+      <c r="AN149" s="64"/>
       <c r="AO149" s="12"/>
       <c r="AP149" s="13"/>
       <c r="AQ149" s="13"/>
@@ -9624,18 +9620,18 @@
       <c r="BC149" s="14"/>
     </row>
     <row r="150" spans="6:55" x14ac:dyDescent="0.25">
-      <c r="P150" s="56"/>
-      <c r="Q150" s="56"/>
+      <c r="P150" s="64"/>
+      <c r="Q150" s="64"/>
       <c r="R150" s="35"/>
       <c r="S150" s="37"/>
-      <c r="T150" s="56"/>
-      <c r="U150" s="56"/>
+      <c r="T150" s="64"/>
+      <c r="U150" s="64"/>
       <c r="V150" s="15"/>
       <c r="W150" s="17"/>
-      <c r="X150" s="56"/>
-      <c r="Y150" s="56"/>
-      <c r="Z150" s="56"/>
-      <c r="AA150" s="56"/>
+      <c r="X150" s="64"/>
+      <c r="Y150" s="64"/>
+      <c r="Z150" s="64"/>
+      <c r="AA150" s="64"/>
       <c r="AB150" s="15"/>
       <c r="AC150" s="16"/>
       <c r="AD150" s="16"/>
@@ -9647,8 +9643,8 @@
       <c r="AJ150" s="16"/>
       <c r="AK150" s="16"/>
       <c r="AL150" s="17"/>
-      <c r="AM150" s="56"/>
-      <c r="AN150" s="56"/>
+      <c r="AM150" s="64"/>
+      <c r="AN150" s="64"/>
       <c r="AO150" s="15"/>
       <c r="AP150" s="16"/>
       <c r="AQ150" s="16"/>
@@ -9703,14 +9699,14 @@
         <v>106</v>
       </c>
       <c r="AN151" s="11"/>
-      <c r="AO151" s="56" t="s">
+      <c r="AO151" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="AP151" s="56"/>
-      <c r="AQ151" s="56"/>
-      <c r="AR151" s="56"/>
-      <c r="AS151" s="56"/>
-      <c r="AT151" s="56"/>
+      <c r="AP151" s="64"/>
+      <c r="AQ151" s="64"/>
+      <c r="AR151" s="64"/>
+      <c r="AS151" s="64"/>
+      <c r="AT151" s="64"/>
       <c r="AU151" s="9"/>
       <c r="AV151" s="10"/>
       <c r="AW151" s="10"/>
@@ -9726,8 +9722,8 @@
     <row r="152" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P152" s="12"/>
       <c r="Q152" s="14"/>
-      <c r="R152" s="75"/>
-      <c r="S152" s="76"/>
+      <c r="R152" s="90"/>
+      <c r="S152" s="91"/>
       <c r="T152" s="12"/>
       <c r="U152" s="14"/>
       <c r="V152" s="12"/>
@@ -9749,12 +9745,12 @@
       <c r="AL152" s="14"/>
       <c r="AM152" s="12"/>
       <c r="AN152" s="14"/>
-      <c r="AO152" s="56"/>
-      <c r="AP152" s="56"/>
-      <c r="AQ152" s="56"/>
-      <c r="AR152" s="56"/>
-      <c r="AS152" s="56"/>
-      <c r="AT152" s="56"/>
+      <c r="AO152" s="64"/>
+      <c r="AP152" s="64"/>
+      <c r="AQ152" s="64"/>
+      <c r="AR152" s="64"/>
+      <c r="AS152" s="64"/>
+      <c r="AT152" s="64"/>
       <c r="AU152" s="12"/>
       <c r="AV152" s="13"/>
       <c r="AW152" s="13"/>
@@ -9768,8 +9764,8 @@
     <row r="153" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P153" s="12"/>
       <c r="Q153" s="14"/>
-      <c r="R153" s="75"/>
-      <c r="S153" s="76"/>
+      <c r="R153" s="90"/>
+      <c r="S153" s="91"/>
       <c r="T153" s="12"/>
       <c r="U153" s="14"/>
       <c r="V153" s="12"/>
@@ -9791,12 +9787,12 @@
       <c r="AL153" s="14"/>
       <c r="AM153" s="12"/>
       <c r="AN153" s="14"/>
-      <c r="AO153" s="56"/>
-      <c r="AP153" s="56"/>
-      <c r="AQ153" s="56"/>
-      <c r="AR153" s="56"/>
-      <c r="AS153" s="56"/>
-      <c r="AT153" s="56"/>
+      <c r="AO153" s="64"/>
+      <c r="AP153" s="64"/>
+      <c r="AQ153" s="64"/>
+      <c r="AR153" s="64"/>
+      <c r="AS153" s="64"/>
+      <c r="AT153" s="64"/>
       <c r="AU153" s="12"/>
       <c r="AV153" s="13"/>
       <c r="AW153" s="13"/>
@@ -9810,8 +9806,8 @@
     <row r="154" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P154" s="12"/>
       <c r="Q154" s="14"/>
-      <c r="R154" s="75"/>
-      <c r="S154" s="76"/>
+      <c r="R154" s="90"/>
+      <c r="S154" s="91"/>
       <c r="T154" s="12"/>
       <c r="U154" s="14"/>
       <c r="V154" s="12"/>
@@ -9833,12 +9829,12 @@
       <c r="AL154" s="14"/>
       <c r="AM154" s="12"/>
       <c r="AN154" s="14"/>
-      <c r="AO154" s="56"/>
-      <c r="AP154" s="56"/>
-      <c r="AQ154" s="56"/>
-      <c r="AR154" s="56"/>
-      <c r="AS154" s="56"/>
-      <c r="AT154" s="56"/>
+      <c r="AO154" s="64"/>
+      <c r="AP154" s="64"/>
+      <c r="AQ154" s="64"/>
+      <c r="AR154" s="64"/>
+      <c r="AS154" s="64"/>
+      <c r="AT154" s="64"/>
       <c r="AU154" s="12"/>
       <c r="AV154" s="13"/>
       <c r="AW154" s="13"/>
@@ -9852,8 +9848,8 @@
     <row r="155" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P155" s="12"/>
       <c r="Q155" s="14"/>
-      <c r="R155" s="75"/>
-      <c r="S155" s="76"/>
+      <c r="R155" s="90"/>
+      <c r="S155" s="91"/>
       <c r="T155" s="12"/>
       <c r="U155" s="14"/>
       <c r="V155" s="12"/>
@@ -9875,12 +9871,12 @@
       <c r="AL155" s="14"/>
       <c r="AM155" s="12"/>
       <c r="AN155" s="14"/>
-      <c r="AO155" s="56"/>
-      <c r="AP155" s="56"/>
-      <c r="AQ155" s="56"/>
-      <c r="AR155" s="56"/>
-      <c r="AS155" s="56"/>
-      <c r="AT155" s="56"/>
+      <c r="AO155" s="64"/>
+      <c r="AP155" s="64"/>
+      <c r="AQ155" s="64"/>
+      <c r="AR155" s="64"/>
+      <c r="AS155" s="64"/>
+      <c r="AT155" s="64"/>
       <c r="AU155" s="12"/>
       <c r="AV155" s="13"/>
       <c r="AW155" s="13"/>
@@ -9894,8 +9890,8 @@
     <row r="156" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P156" s="12"/>
       <c r="Q156" s="14"/>
-      <c r="R156" s="75"/>
-      <c r="S156" s="76"/>
+      <c r="R156" s="90"/>
+      <c r="S156" s="91"/>
       <c r="T156" s="12"/>
       <c r="U156" s="14"/>
       <c r="V156" s="12"/>
@@ -9917,12 +9913,12 @@
       <c r="AL156" s="14"/>
       <c r="AM156" s="12"/>
       <c r="AN156" s="14"/>
-      <c r="AO156" s="56"/>
-      <c r="AP156" s="56"/>
-      <c r="AQ156" s="56"/>
-      <c r="AR156" s="56"/>
-      <c r="AS156" s="56"/>
-      <c r="AT156" s="56"/>
+      <c r="AO156" s="64"/>
+      <c r="AP156" s="64"/>
+      <c r="AQ156" s="64"/>
+      <c r="AR156" s="64"/>
+      <c r="AS156" s="64"/>
+      <c r="AT156" s="64"/>
       <c r="AU156" s="12"/>
       <c r="AV156" s="13"/>
       <c r="AW156" s="13"/>
@@ -9936,8 +9932,8 @@
     <row r="157" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P157" s="12"/>
       <c r="Q157" s="14"/>
-      <c r="R157" s="75"/>
-      <c r="S157" s="76"/>
+      <c r="R157" s="90"/>
+      <c r="S157" s="91"/>
       <c r="T157" s="12"/>
       <c r="U157" s="14"/>
       <c r="V157" s="12"/>
@@ -9959,12 +9955,12 @@
       <c r="AL157" s="14"/>
       <c r="AM157" s="12"/>
       <c r="AN157" s="14"/>
-      <c r="AO157" s="56"/>
-      <c r="AP157" s="56"/>
-      <c r="AQ157" s="56"/>
-      <c r="AR157" s="56"/>
-      <c r="AS157" s="56"/>
-      <c r="AT157" s="56"/>
+      <c r="AO157" s="64"/>
+      <c r="AP157" s="64"/>
+      <c r="AQ157" s="64"/>
+      <c r="AR157" s="64"/>
+      <c r="AS157" s="64"/>
+      <c r="AT157" s="64"/>
       <c r="AU157" s="12"/>
       <c r="AV157" s="13"/>
       <c r="AW157" s="13"/>
@@ -9978,8 +9974,8 @@
     <row r="158" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P158" s="12"/>
       <c r="Q158" s="14"/>
-      <c r="R158" s="75"/>
-      <c r="S158" s="76"/>
+      <c r="R158" s="90"/>
+      <c r="S158" s="91"/>
       <c r="T158" s="12"/>
       <c r="U158" s="14"/>
       <c r="V158" s="12"/>
@@ -10001,12 +9997,12 @@
       <c r="AL158" s="14"/>
       <c r="AM158" s="12"/>
       <c r="AN158" s="14"/>
-      <c r="AO158" s="56"/>
-      <c r="AP158" s="56"/>
-      <c r="AQ158" s="56"/>
-      <c r="AR158" s="56"/>
-      <c r="AS158" s="56"/>
-      <c r="AT158" s="56"/>
+      <c r="AO158" s="64"/>
+      <c r="AP158" s="64"/>
+      <c r="AQ158" s="64"/>
+      <c r="AR158" s="64"/>
+      <c r="AS158" s="64"/>
+      <c r="AT158" s="64"/>
       <c r="AU158" s="12"/>
       <c r="AV158" s="13"/>
       <c r="AW158" s="13"/>
@@ -10020,8 +10016,8 @@
     <row r="159" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P159" s="12"/>
       <c r="Q159" s="14"/>
-      <c r="R159" s="75"/>
-      <c r="S159" s="76"/>
+      <c r="R159" s="90"/>
+      <c r="S159" s="91"/>
       <c r="T159" s="12"/>
       <c r="U159" s="14"/>
       <c r="V159" s="12"/>
@@ -10043,12 +10039,12 @@
       <c r="AL159" s="14"/>
       <c r="AM159" s="12"/>
       <c r="AN159" s="14"/>
-      <c r="AO159" s="56"/>
-      <c r="AP159" s="56"/>
-      <c r="AQ159" s="56"/>
-      <c r="AR159" s="56"/>
-      <c r="AS159" s="56"/>
-      <c r="AT159" s="56"/>
+      <c r="AO159" s="64"/>
+      <c r="AP159" s="64"/>
+      <c r="AQ159" s="64"/>
+      <c r="AR159" s="64"/>
+      <c r="AS159" s="64"/>
+      <c r="AT159" s="64"/>
       <c r="AU159" s="12"/>
       <c r="AV159" s="13"/>
       <c r="AW159" s="13"/>
@@ -10062,8 +10058,8 @@
     <row r="160" spans="6:55" x14ac:dyDescent="0.25">
       <c r="P160" s="12"/>
       <c r="Q160" s="14"/>
-      <c r="R160" s="75"/>
-      <c r="S160" s="76"/>
+      <c r="R160" s="90"/>
+      <c r="S160" s="91"/>
       <c r="T160" s="12"/>
       <c r="U160" s="14"/>
       <c r="V160" s="12"/>
@@ -10085,12 +10081,12 @@
       <c r="AL160" s="14"/>
       <c r="AM160" s="12"/>
       <c r="AN160" s="14"/>
-      <c r="AO160" s="56"/>
-      <c r="AP160" s="56"/>
-      <c r="AQ160" s="56"/>
-      <c r="AR160" s="56"/>
-      <c r="AS160" s="56"/>
-      <c r="AT160" s="56"/>
+      <c r="AO160" s="64"/>
+      <c r="AP160" s="64"/>
+      <c r="AQ160" s="64"/>
+      <c r="AR160" s="64"/>
+      <c r="AS160" s="64"/>
+      <c r="AT160" s="64"/>
       <c r="AU160" s="12"/>
       <c r="AV160" s="13"/>
       <c r="AW160" s="13"/>
@@ -10104,8 +10100,8 @@
     <row r="161" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P161" s="12"/>
       <c r="Q161" s="14"/>
-      <c r="R161" s="75"/>
-      <c r="S161" s="76"/>
+      <c r="R161" s="90"/>
+      <c r="S161" s="91"/>
       <c r="T161" s="12"/>
       <c r="U161" s="14"/>
       <c r="V161" s="12"/>
@@ -10127,12 +10123,12 @@
       <c r="AL161" s="14"/>
       <c r="AM161" s="12"/>
       <c r="AN161" s="14"/>
-      <c r="AO161" s="56"/>
-      <c r="AP161" s="56"/>
-      <c r="AQ161" s="56"/>
-      <c r="AR161" s="56"/>
-      <c r="AS161" s="56"/>
-      <c r="AT161" s="56"/>
+      <c r="AO161" s="64"/>
+      <c r="AP161" s="64"/>
+      <c r="AQ161" s="64"/>
+      <c r="AR161" s="64"/>
+      <c r="AS161" s="64"/>
+      <c r="AT161" s="64"/>
       <c r="AU161" s="12"/>
       <c r="AV161" s="13"/>
       <c r="AW161" s="13"/>
@@ -10146,8 +10142,8 @@
     <row r="162" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P162" s="12"/>
       <c r="Q162" s="14"/>
-      <c r="R162" s="75"/>
-      <c r="S162" s="76"/>
+      <c r="R162" s="90"/>
+      <c r="S162" s="91"/>
       <c r="T162" s="12"/>
       <c r="U162" s="14"/>
       <c r="V162" s="12"/>
@@ -10169,12 +10165,12 @@
       <c r="AL162" s="14"/>
       <c r="AM162" s="12"/>
       <c r="AN162" s="14"/>
-      <c r="AO162" s="56"/>
-      <c r="AP162" s="56"/>
-      <c r="AQ162" s="56"/>
-      <c r="AR162" s="56"/>
-      <c r="AS162" s="56"/>
-      <c r="AT162" s="56"/>
+      <c r="AO162" s="64"/>
+      <c r="AP162" s="64"/>
+      <c r="AQ162" s="64"/>
+      <c r="AR162" s="64"/>
+      <c r="AS162" s="64"/>
+      <c r="AT162" s="64"/>
       <c r="AU162" s="12"/>
       <c r="AV162" s="13"/>
       <c r="AW162" s="13"/>
@@ -10188,8 +10184,8 @@
     <row r="163" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P163" s="12"/>
       <c r="Q163" s="14"/>
-      <c r="R163" s="75"/>
-      <c r="S163" s="76"/>
+      <c r="R163" s="90"/>
+      <c r="S163" s="91"/>
       <c r="T163" s="12"/>
       <c r="U163" s="14"/>
       <c r="V163" s="12"/>
@@ -10211,12 +10207,12 @@
       <c r="AL163" s="14"/>
       <c r="AM163" s="12"/>
       <c r="AN163" s="14"/>
-      <c r="AO163" s="56"/>
-      <c r="AP163" s="56"/>
-      <c r="AQ163" s="56"/>
-      <c r="AR163" s="56"/>
-      <c r="AS163" s="56"/>
-      <c r="AT163" s="56"/>
+      <c r="AO163" s="64"/>
+      <c r="AP163" s="64"/>
+      <c r="AQ163" s="64"/>
+      <c r="AR163" s="64"/>
+      <c r="AS163" s="64"/>
+      <c r="AT163" s="64"/>
       <c r="AU163" s="12"/>
       <c r="AV163" s="13"/>
       <c r="AW163" s="13"/>
@@ -10230,8 +10226,8 @@
     <row r="164" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P164" s="12"/>
       <c r="Q164" s="14"/>
-      <c r="R164" s="75"/>
-      <c r="S164" s="76"/>
+      <c r="R164" s="90"/>
+      <c r="S164" s="91"/>
       <c r="T164" s="12"/>
       <c r="U164" s="14"/>
       <c r="V164" s="12"/>
@@ -10253,12 +10249,12 @@
       <c r="AL164" s="14"/>
       <c r="AM164" s="12"/>
       <c r="AN164" s="14"/>
-      <c r="AO164" s="56"/>
-      <c r="AP164" s="56"/>
-      <c r="AQ164" s="56"/>
-      <c r="AR164" s="56"/>
-      <c r="AS164" s="56"/>
-      <c r="AT164" s="56"/>
+      <c r="AO164" s="64"/>
+      <c r="AP164" s="64"/>
+      <c r="AQ164" s="64"/>
+      <c r="AR164" s="64"/>
+      <c r="AS164" s="64"/>
+      <c r="AT164" s="64"/>
       <c r="AU164" s="12"/>
       <c r="AV164" s="13"/>
       <c r="AW164" s="13"/>
@@ -10272,8 +10268,8 @@
     <row r="165" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P165" s="12"/>
       <c r="Q165" s="14"/>
-      <c r="R165" s="75"/>
-      <c r="S165" s="76"/>
+      <c r="R165" s="90"/>
+      <c r="S165" s="91"/>
       <c r="T165" s="12"/>
       <c r="U165" s="14"/>
       <c r="V165" s="12"/>
@@ -10295,12 +10291,12 @@
       <c r="AL165" s="14"/>
       <c r="AM165" s="12"/>
       <c r="AN165" s="14"/>
-      <c r="AO165" s="56"/>
-      <c r="AP165" s="56"/>
-      <c r="AQ165" s="56"/>
-      <c r="AR165" s="56"/>
-      <c r="AS165" s="56"/>
-      <c r="AT165" s="56"/>
+      <c r="AO165" s="64"/>
+      <c r="AP165" s="64"/>
+      <c r="AQ165" s="64"/>
+      <c r="AR165" s="64"/>
+      <c r="AS165" s="64"/>
+      <c r="AT165" s="64"/>
       <c r="AU165" s="12"/>
       <c r="AV165" s="13"/>
       <c r="AW165" s="13"/>
@@ -10314,8 +10310,8 @@
     <row r="166" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P166" s="12"/>
       <c r="Q166" s="14"/>
-      <c r="R166" s="75"/>
-      <c r="S166" s="76"/>
+      <c r="R166" s="90"/>
+      <c r="S166" s="91"/>
       <c r="T166" s="12"/>
       <c r="U166" s="14"/>
       <c r="V166" s="12"/>
@@ -10337,12 +10333,12 @@
       <c r="AL166" s="14"/>
       <c r="AM166" s="12"/>
       <c r="AN166" s="14"/>
-      <c r="AO166" s="56"/>
-      <c r="AP166" s="56"/>
-      <c r="AQ166" s="56"/>
-      <c r="AR166" s="56"/>
-      <c r="AS166" s="56"/>
-      <c r="AT166" s="56"/>
+      <c r="AO166" s="64"/>
+      <c r="AP166" s="64"/>
+      <c r="AQ166" s="64"/>
+      <c r="AR166" s="64"/>
+      <c r="AS166" s="64"/>
+      <c r="AT166" s="64"/>
       <c r="AU166" s="12"/>
       <c r="AV166" s="13"/>
       <c r="AW166" s="13"/>
@@ -10356,8 +10352,8 @@
     <row r="167" spans="16:55" x14ac:dyDescent="0.25">
       <c r="P167" s="12"/>
       <c r="Q167" s="14"/>
-      <c r="R167" s="75"/>
-      <c r="S167" s="76"/>
+      <c r="R167" s="90"/>
+      <c r="S167" s="91"/>
       <c r="T167" s="15"/>
       <c r="U167" s="17"/>
       <c r="V167" s="15"/>
@@ -10379,12 +10375,12 @@
       <c r="AL167" s="17"/>
       <c r="AM167" s="15"/>
       <c r="AN167" s="17"/>
-      <c r="AO167" s="56"/>
-      <c r="AP167" s="56"/>
-      <c r="AQ167" s="56"/>
-      <c r="AR167" s="56"/>
-      <c r="AS167" s="56"/>
-      <c r="AT167" s="56"/>
+      <c r="AO167" s="64"/>
+      <c r="AP167" s="64"/>
+      <c r="AQ167" s="64"/>
+      <c r="AR167" s="64"/>
+      <c r="AS167" s="64"/>
+      <c r="AT167" s="64"/>
       <c r="AU167" s="15"/>
       <c r="AV167" s="16"/>
       <c r="AW167" s="16"/>
@@ -10481,6 +10477,8 @@
     </row>
   </sheetData>
   <mergeCells count="277">
+    <mergeCell ref="L102:L105"/>
+    <mergeCell ref="M102:N105"/>
     <mergeCell ref="F104:G105"/>
     <mergeCell ref="AG138:AL150"/>
     <mergeCell ref="AM138:AN150"/>
@@ -10501,8 +10499,6 @@
     <mergeCell ref="K138:N141"/>
     <mergeCell ref="K142:N145"/>
     <mergeCell ref="K146:N149"/>
-    <mergeCell ref="J138:J141"/>
-    <mergeCell ref="J142:J145"/>
     <mergeCell ref="F2:F13"/>
     <mergeCell ref="G2:G13"/>
     <mergeCell ref="H2:H13"/>
@@ -10522,11 +10518,6 @@
     <mergeCell ref="M24:N41"/>
     <mergeCell ref="F56:N57"/>
     <mergeCell ref="F20:I21"/>
-    <mergeCell ref="J20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="F16:N17"/>
-    <mergeCell ref="F18:N19"/>
-    <mergeCell ref="M20:N23"/>
     <mergeCell ref="AU151:AZ167"/>
     <mergeCell ref="BA151:BC167"/>
     <mergeCell ref="AO151:AT167"/>
@@ -10600,6 +10591,11 @@
     <mergeCell ref="AU68:AZ77"/>
     <mergeCell ref="AU88:AZ97"/>
     <mergeCell ref="AO100:AT101"/>
+    <mergeCell ref="J20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="F16:N17"/>
+    <mergeCell ref="F18:N19"/>
+    <mergeCell ref="M20:N23"/>
     <mergeCell ref="F24:G32"/>
     <mergeCell ref="F33:G41"/>
     <mergeCell ref="H24:I32"/>
@@ -10610,6 +10606,8 @@
     <mergeCell ref="J33:K41"/>
     <mergeCell ref="L24:L32"/>
     <mergeCell ref="L33:L41"/>
+    <mergeCell ref="J138:J141"/>
+    <mergeCell ref="J142:J145"/>
     <mergeCell ref="J146:J149"/>
     <mergeCell ref="H136:I137"/>
     <mergeCell ref="J136:J137"/>
@@ -10632,8 +10630,6 @@
     <mergeCell ref="R100:S101"/>
     <mergeCell ref="F102:I103"/>
     <mergeCell ref="J102:K105"/>
-    <mergeCell ref="L102:L105"/>
-    <mergeCell ref="M102:N105"/>
     <mergeCell ref="T88:U97"/>
     <mergeCell ref="V88:W97"/>
     <mergeCell ref="X88:AA97"/>

</xml_diff>